<commit_message>
Updated how data frames are produced for each calc
</commit_message>
<xml_diff>
--- a/tests/testmodels/TestJob1/mf_results/tm59mechvent/TM59MechVent__TestJob1.xlsx
+++ b/tests/testmodels/TestJob1/mf_results/tm59mechvent/TM59MechVent__TestJob1.xlsx
@@ -27,12 +27,12 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1002" uniqueCount="121">
   <si>
+    <t>Author</t>
+  </si>
+  <si>
     <t>Date</t>
   </si>
   <si>
-    <t>Author</t>
-  </si>
-  <si>
     <t>sheet_name</t>
   </si>
   <si>
@@ -72,12 +72,12 @@
     <t>10</t>
   </si>
   <si>
+    <t>jovyan</t>
+  </si>
+  <si>
     <t>20220308</t>
   </si>
   <si>
-    <t>jovyan</t>
-  </si>
-  <si>
     <t>Project Information</t>
   </si>
   <si>
@@ -177,7 +177,7 @@
     <t>51.38</t>
   </si>
   <si>
-    <t>2022-03-08 14:52:59.628024</t>
+    <t>2022-03-08 17:54:33.453856</t>
   </si>
   <si>
     <t>2021.4.0.0</t>
@@ -571,8 +571,8 @@
   <autoFilter ref="A1:E12"/>
   <tableColumns count="5">
     <tableColumn id="1" name="index"/>
-    <tableColumn id="2" name="Date"/>
-    <tableColumn id="3" name="Author"/>
+    <tableColumn id="2" name="Author"/>
+    <tableColumn id="3" name="Date"/>
     <tableColumn id="4" name="sheet_name"/>
     <tableColumn id="5" name="JobNo"/>
   </tableColumns>
@@ -586,8 +586,8 @@
   <tableColumns count="4">
     <tableColumn id="1" name="Room ID"/>
     <tableColumn id="2" name="Room Name"/>
-    <tableColumn id="3" name="Fixed Temp Criterion (% Hours Operative Temp &gt; 26 Deg. Celsius)"/>
-    <tableColumn id="4" name="Fixed Temp Criterion (Pass/Fail)"/>
+    <tableColumn id="3" name="Fixed Temp Criterion (Pass/Fail)"/>
+    <tableColumn id="4" name="Fixed Temp Criterion (% Hours Operative Temp &gt; 26 Deg. Celsius)"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -599,8 +599,8 @@
   <tableColumns count="4">
     <tableColumn id="1" name="Room ID"/>
     <tableColumn id="2" name="Room Name"/>
-    <tableColumn id="3" name="Fixed Temp Criterion (% Hours Operative Temp &gt; 26 Deg. Celsius)"/>
-    <tableColumn id="4" name="Fixed Temp Criterion (Pass/Fail)"/>
+    <tableColumn id="3" name="Fixed Temp Criterion (Pass/Fail)"/>
+    <tableColumn id="4" name="Fixed Temp Criterion (% Hours Operative Temp &gt; 26 Deg. Celsius)"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -612,8 +612,8 @@
   <tableColumns count="4">
     <tableColumn id="1" name="Room ID"/>
     <tableColumn id="2" name="Room Name"/>
-    <tableColumn id="3" name="Fixed Temp Criterion (% Hours Operative Temp &gt; 26 Deg. Celsius)"/>
-    <tableColumn id="4" name="Fixed Temp Criterion (Pass/Fail)"/>
+    <tableColumn id="3" name="Fixed Temp Criterion (Pass/Fail)"/>
+    <tableColumn id="4" name="Fixed Temp Criterion (% Hours Operative Temp &gt; 26 Deg. Celsius)"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -647,8 +647,8 @@
   <tableColumns count="4">
     <tableColumn id="1" name="Room ID"/>
     <tableColumn id="2" name="Room Name"/>
-    <tableColumn id="3" name="Fixed Temp Criterion (% Hours Operative Temp &gt; 26 Deg. Celsius)"/>
-    <tableColumn id="4" name="Fixed Temp Criterion (Pass/Fail)"/>
+    <tableColumn id="3" name="Fixed Temp Criterion (Pass/Fail)"/>
+    <tableColumn id="4" name="Fixed Temp Criterion (% Hours Operative Temp &gt; 26 Deg. Celsius)"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -660,8 +660,8 @@
   <tableColumns count="4">
     <tableColumn id="1" name="Room ID"/>
     <tableColumn id="2" name="Room Name"/>
-    <tableColumn id="3" name="Fixed Temp Criterion (% Hours Operative Temp &gt; 26 Deg. Celsius)"/>
-    <tableColumn id="4" name="Fixed Temp Criterion (Pass/Fail)"/>
+    <tableColumn id="3" name="Fixed Temp Criterion (Pass/Fail)"/>
+    <tableColumn id="4" name="Fixed Temp Criterion (% Hours Operative Temp &gt; 26 Deg. Celsius)"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -673,8 +673,8 @@
   <tableColumns count="4">
     <tableColumn id="1" name="Room ID"/>
     <tableColumn id="2" name="Room Name"/>
-    <tableColumn id="3" name="Fixed Temp Criterion (% Hours Operative Temp &gt; 26 Deg. Celsius)"/>
-    <tableColumn id="4" name="Fixed Temp Criterion (Pass/Fail)"/>
+    <tableColumn id="3" name="Fixed Temp Criterion (Pass/Fail)"/>
+    <tableColumn id="4" name="Fixed Temp Criterion (% Hours Operative Temp &gt; 26 Deg. Celsius)"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -686,8 +686,8 @@
   <tableColumns count="4">
     <tableColumn id="1" name="Room ID"/>
     <tableColumn id="2" name="Room Name"/>
-    <tableColumn id="3" name="Fixed Temp Criterion (% Hours Operative Temp &gt; 26 Deg. Celsius)"/>
-    <tableColumn id="4" name="Fixed Temp Criterion (Pass/Fail)"/>
+    <tableColumn id="3" name="Fixed Temp Criterion (Pass/Fail)"/>
+    <tableColumn id="4" name="Fixed Temp Criterion (% Hours Operative Temp &gt; 26 Deg. Celsius)"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -699,8 +699,8 @@
   <tableColumns count="4">
     <tableColumn id="1" name="Room ID"/>
     <tableColumn id="2" name="Room Name"/>
-    <tableColumn id="3" name="Fixed Temp Criterion (% Hours Operative Temp &gt; 26 Deg. Celsius)"/>
-    <tableColumn id="4" name="Fixed Temp Criterion (Pass/Fail)"/>
+    <tableColumn id="3" name="Fixed Temp Criterion (Pass/Fail)"/>
+    <tableColumn id="4" name="Fixed Temp Criterion (% Hours Operative Temp &gt; 26 Deg. Celsius)"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -712,8 +712,8 @@
   <tableColumns count="4">
     <tableColumn id="1" name="Room ID"/>
     <tableColumn id="2" name="Room Name"/>
-    <tableColumn id="3" name="Fixed Temp Criterion (% Hours Operative Temp &gt; 26 Deg. Celsius)"/>
-    <tableColumn id="4" name="Fixed Temp Criterion (Pass/Fail)"/>
+    <tableColumn id="3" name="Fixed Temp Criterion (Pass/Fail)"/>
+    <tableColumn id="4" name="Fixed Temp Criterion (% Hours Operative Temp &gt; 26 Deg. Celsius)"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1253,10 +1253,10 @@
         <v>55</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1266,11 +1266,11 @@
       <c r="B2" t="s">
         <v>89</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D2">
         <v>11.2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1280,11 +1280,11 @@
       <c r="B3" t="s">
         <v>90</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D3">
         <v>16.5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1294,11 +1294,11 @@
       <c r="B4" t="s">
         <v>91</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4">
         <v>16.67</v>
-      </c>
-      <c r="D4" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1308,11 +1308,11 @@
       <c r="B5" t="s">
         <v>92</v>
       </c>
-      <c r="C5">
+      <c r="C5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5">
         <v>5.58</v>
-      </c>
-      <c r="D5" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1322,11 +1322,11 @@
       <c r="B6" t="s">
         <v>93</v>
       </c>
-      <c r="C6">
+      <c r="C6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D6">
         <v>5.74</v>
-      </c>
-      <c r="D6" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1336,11 +1336,11 @@
       <c r="B7" t="s">
         <v>94</v>
       </c>
-      <c r="C7">
+      <c r="C7" t="s">
+        <v>120</v>
+      </c>
+      <c r="D7">
         <v>5.7</v>
-      </c>
-      <c r="D7" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1350,11 +1350,11 @@
       <c r="B8" t="s">
         <v>95</v>
       </c>
-      <c r="C8">
+      <c r="C8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D8">
         <v>5.55</v>
-      </c>
-      <c r="D8" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1364,11 +1364,11 @@
       <c r="B9" t="s">
         <v>96</v>
       </c>
-      <c r="C9">
+      <c r="C9" t="s">
+        <v>120</v>
+      </c>
+      <c r="D9">
         <v>17.87</v>
-      </c>
-      <c r="D9" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1378,11 +1378,11 @@
       <c r="B10" t="s">
         <v>97</v>
       </c>
-      <c r="C10">
+      <c r="C10" t="s">
+        <v>120</v>
+      </c>
+      <c r="D10">
         <v>23.75</v>
-      </c>
-      <c r="D10" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1392,11 +1392,11 @@
       <c r="B11" t="s">
         <v>98</v>
       </c>
-      <c r="C11">
+      <c r="C11" t="s">
+        <v>120</v>
+      </c>
+      <c r="D11">
         <v>18.57</v>
-      </c>
-      <c r="D11" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -1406,11 +1406,11 @@
       <c r="B12" t="s">
         <v>99</v>
       </c>
-      <c r="C12">
+      <c r="C12" t="s">
+        <v>120</v>
+      </c>
+      <c r="D12">
         <v>24.03</v>
-      </c>
-      <c r="D12" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1420,11 +1420,11 @@
       <c r="B13" t="s">
         <v>100</v>
       </c>
-      <c r="C13">
+      <c r="C13" t="s">
+        <v>120</v>
+      </c>
+      <c r="D13">
         <v>10.9</v>
-      </c>
-      <c r="D13" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1434,11 +1434,11 @@
       <c r="B14" t="s">
         <v>101</v>
       </c>
-      <c r="C14">
+      <c r="C14" t="s">
+        <v>120</v>
+      </c>
+      <c r="D14">
         <v>11.37</v>
-      </c>
-      <c r="D14" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -1448,11 +1448,11 @@
       <c r="B15" t="s">
         <v>102</v>
       </c>
-      <c r="C15">
+      <c r="C15" t="s">
+        <v>120</v>
+      </c>
+      <c r="D15">
         <v>11.4</v>
-      </c>
-      <c r="D15" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1462,11 +1462,11 @@
       <c r="B16" t="s">
         <v>103</v>
       </c>
-      <c r="C16">
+      <c r="C16" t="s">
+        <v>120</v>
+      </c>
+      <c r="D16">
         <v>10.94</v>
-      </c>
-      <c r="D16" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1476,11 +1476,11 @@
       <c r="B17" t="s">
         <v>104</v>
       </c>
-      <c r="C17">
+      <c r="C17" t="s">
+        <v>120</v>
+      </c>
+      <c r="D17">
         <v>18.81</v>
-      </c>
-      <c r="D17" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1490,11 +1490,11 @@
       <c r="B18" t="s">
         <v>105</v>
       </c>
-      <c r="C18">
+      <c r="C18" t="s">
+        <v>120</v>
+      </c>
+      <c r="D18">
         <v>25.52</v>
-      </c>
-      <c r="D18" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1504,11 +1504,11 @@
       <c r="B19" t="s">
         <v>106</v>
       </c>
-      <c r="C19">
+      <c r="C19" t="s">
+        <v>120</v>
+      </c>
+      <c r="D19">
         <v>19.47</v>
-      </c>
-      <c r="D19" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1518,11 +1518,11 @@
       <c r="B20" t="s">
         <v>107</v>
       </c>
-      <c r="C20">
+      <c r="C20" t="s">
+        <v>120</v>
+      </c>
+      <c r="D20">
         <v>25.73</v>
-      </c>
-      <c r="D20" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -1532,11 +1532,11 @@
       <c r="B21" t="s">
         <v>108</v>
       </c>
-      <c r="C21">
+      <c r="C21" t="s">
+        <v>120</v>
+      </c>
+      <c r="D21">
         <v>11.88</v>
-      </c>
-      <c r="D21" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -1546,11 +1546,11 @@
       <c r="B22" t="s">
         <v>109</v>
       </c>
-      <c r="C22">
+      <c r="C22" t="s">
+        <v>120</v>
+      </c>
+      <c r="D22">
         <v>12.45</v>
-      </c>
-      <c r="D22" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1560,11 +1560,11 @@
       <c r="B23" t="s">
         <v>110</v>
       </c>
-      <c r="C23">
+      <c r="C23" t="s">
+        <v>120</v>
+      </c>
+      <c r="D23">
         <v>12.67</v>
-      </c>
-      <c r="D23" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1574,11 +1574,11 @@
       <c r="B24" t="s">
         <v>111</v>
       </c>
-      <c r="C24">
+      <c r="C24" t="s">
+        <v>120</v>
+      </c>
+      <c r="D24">
         <v>11.91</v>
-      </c>
-      <c r="D24" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1588,11 +1588,11 @@
       <c r="B25" t="s">
         <v>112</v>
       </c>
-      <c r="C25">
+      <c r="C25" t="s">
+        <v>120</v>
+      </c>
+      <c r="D25">
         <v>14.46</v>
-      </c>
-      <c r="D25" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1602,11 +1602,11 @@
       <c r="B26" t="s">
         <v>113</v>
       </c>
-      <c r="C26">
+      <c r="C26" t="s">
+        <v>120</v>
+      </c>
+      <c r="D26">
         <v>20.44</v>
-      </c>
-      <c r="D26" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1616,11 +1616,11 @@
       <c r="B27" t="s">
         <v>114</v>
       </c>
-      <c r="C27">
+      <c r="C27" t="s">
+        <v>120</v>
+      </c>
+      <c r="D27">
         <v>14.7</v>
-      </c>
-      <c r="D27" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1630,11 +1630,11 @@
       <c r="B28" t="s">
         <v>115</v>
       </c>
-      <c r="C28">
+      <c r="C28" t="s">
+        <v>120</v>
+      </c>
+      <c r="D28">
         <v>20.65</v>
-      </c>
-      <c r="D28" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1644,11 +1644,11 @@
       <c r="B29" t="s">
         <v>116</v>
       </c>
-      <c r="C29">
+      <c r="C29" t="s">
+        <v>120</v>
+      </c>
+      <c r="D29">
         <v>9.470000000000001</v>
-      </c>
-      <c r="D29" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1658,11 +1658,11 @@
       <c r="B30" t="s">
         <v>117</v>
       </c>
-      <c r="C30">
+      <c r="C30" t="s">
+        <v>120</v>
+      </c>
+      <c r="D30">
         <v>9.32</v>
-      </c>
-      <c r="D30" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1672,11 +1672,11 @@
       <c r="B31" t="s">
         <v>118</v>
       </c>
-      <c r="C31">
+      <c r="C31" t="s">
+        <v>120</v>
+      </c>
+      <c r="D31">
         <v>9.44</v>
-      </c>
-      <c r="D31" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1686,11 +1686,11 @@
       <c r="B32" t="s">
         <v>119</v>
       </c>
-      <c r="C32">
+      <c r="C32" t="s">
+        <v>120</v>
+      </c>
+      <c r="D32">
         <v>9.59</v>
-      </c>
-      <c r="D32" t="s">
-        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -1722,10 +1722,10 @@
         <v>55</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1735,11 +1735,11 @@
       <c r="B2" t="s">
         <v>89</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D2">
         <v>11.2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1749,11 +1749,11 @@
       <c r="B3" t="s">
         <v>90</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D3">
         <v>16.52</v>
-      </c>
-      <c r="D3" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1763,11 +1763,11 @@
       <c r="B4" t="s">
         <v>91</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4">
         <v>16.67</v>
-      </c>
-      <c r="D4" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1777,11 +1777,11 @@
       <c r="B5" t="s">
         <v>92</v>
       </c>
-      <c r="C5">
+      <c r="C5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5">
         <v>5.58</v>
-      </c>
-      <c r="D5" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1791,11 +1791,11 @@
       <c r="B6" t="s">
         <v>93</v>
       </c>
-      <c r="C6">
+      <c r="C6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D6">
         <v>5.73</v>
-      </c>
-      <c r="D6" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1805,11 +1805,11 @@
       <c r="B7" t="s">
         <v>94</v>
       </c>
-      <c r="C7">
+      <c r="C7" t="s">
+        <v>120</v>
+      </c>
+      <c r="D7">
         <v>5.7</v>
-      </c>
-      <c r="D7" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1819,11 +1819,11 @@
       <c r="B8" t="s">
         <v>95</v>
       </c>
-      <c r="C8">
+      <c r="C8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D8">
         <v>5.55</v>
-      </c>
-      <c r="D8" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1833,11 +1833,11 @@
       <c r="B9" t="s">
         <v>96</v>
       </c>
-      <c r="C9">
+      <c r="C9" t="s">
+        <v>120</v>
+      </c>
+      <c r="D9">
         <v>17.87</v>
-      </c>
-      <c r="D9" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1847,11 +1847,11 @@
       <c r="B10" t="s">
         <v>97</v>
       </c>
-      <c r="C10">
+      <c r="C10" t="s">
+        <v>120</v>
+      </c>
+      <c r="D10">
         <v>23.75</v>
-      </c>
-      <c r="D10" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1861,11 +1861,11 @@
       <c r="B11" t="s">
         <v>98</v>
       </c>
-      <c r="C11">
+      <c r="C11" t="s">
+        <v>120</v>
+      </c>
+      <c r="D11">
         <v>18.57</v>
-      </c>
-      <c r="D11" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -1875,11 +1875,11 @@
       <c r="B12" t="s">
         <v>99</v>
       </c>
-      <c r="C12">
+      <c r="C12" t="s">
+        <v>120</v>
+      </c>
+      <c r="D12">
         <v>24.03</v>
-      </c>
-      <c r="D12" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1889,11 +1889,11 @@
       <c r="B13" t="s">
         <v>100</v>
       </c>
-      <c r="C13">
+      <c r="C13" t="s">
+        <v>120</v>
+      </c>
+      <c r="D13">
         <v>10.9</v>
-      </c>
-      <c r="D13" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1903,11 +1903,11 @@
       <c r="B14" t="s">
         <v>101</v>
       </c>
-      <c r="C14">
+      <c r="C14" t="s">
+        <v>120</v>
+      </c>
+      <c r="D14">
         <v>11.37</v>
-      </c>
-      <c r="D14" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -1917,11 +1917,11 @@
       <c r="B15" t="s">
         <v>102</v>
       </c>
-      <c r="C15">
+      <c r="C15" t="s">
+        <v>120</v>
+      </c>
+      <c r="D15">
         <v>11.4</v>
-      </c>
-      <c r="D15" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1931,11 +1931,11 @@
       <c r="B16" t="s">
         <v>103</v>
       </c>
-      <c r="C16">
+      <c r="C16" t="s">
+        <v>120</v>
+      </c>
+      <c r="D16">
         <v>10.92</v>
-      </c>
-      <c r="D16" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1945,11 +1945,11 @@
       <c r="B17" t="s">
         <v>104</v>
       </c>
-      <c r="C17">
+      <c r="C17" t="s">
+        <v>120</v>
+      </c>
+      <c r="D17">
         <v>18.81</v>
-      </c>
-      <c r="D17" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1959,11 +1959,11 @@
       <c r="B18" t="s">
         <v>105</v>
       </c>
-      <c r="C18">
+      <c r="C18" t="s">
+        <v>120</v>
+      </c>
+      <c r="D18">
         <v>25.54</v>
-      </c>
-      <c r="D18" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1973,11 +1973,11 @@
       <c r="B19" t="s">
         <v>106</v>
       </c>
-      <c r="C19">
+      <c r="C19" t="s">
+        <v>120</v>
+      </c>
+      <c r="D19">
         <v>19.47</v>
-      </c>
-      <c r="D19" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1987,11 +1987,11 @@
       <c r="B20" t="s">
         <v>107</v>
       </c>
-      <c r="C20">
+      <c r="C20" t="s">
+        <v>120</v>
+      </c>
+      <c r="D20">
         <v>25.75</v>
-      </c>
-      <c r="D20" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -2001,11 +2001,11 @@
       <c r="B21" t="s">
         <v>108</v>
       </c>
-      <c r="C21">
+      <c r="C21" t="s">
+        <v>120</v>
+      </c>
+      <c r="D21">
         <v>11.87</v>
-      </c>
-      <c r="D21" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -2015,11 +2015,11 @@
       <c r="B22" t="s">
         <v>109</v>
       </c>
-      <c r="C22">
+      <c r="C22" t="s">
+        <v>120</v>
+      </c>
+      <c r="D22">
         <v>12.45</v>
-      </c>
-      <c r="D22" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -2029,11 +2029,11 @@
       <c r="B23" t="s">
         <v>110</v>
       </c>
-      <c r="C23">
+      <c r="C23" t="s">
+        <v>120</v>
+      </c>
+      <c r="D23">
         <v>12.67</v>
-      </c>
-      <c r="D23" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -2043,11 +2043,11 @@
       <c r="B24" t="s">
         <v>111</v>
       </c>
-      <c r="C24">
+      <c r="C24" t="s">
+        <v>120</v>
+      </c>
+      <c r="D24">
         <v>11.91</v>
-      </c>
-      <c r="D24" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -2057,11 +2057,11 @@
       <c r="B25" t="s">
         <v>112</v>
       </c>
-      <c r="C25">
+      <c r="C25" t="s">
+        <v>120</v>
+      </c>
+      <c r="D25">
         <v>14.45</v>
-      </c>
-      <c r="D25" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -2071,11 +2071,11 @@
       <c r="B26" t="s">
         <v>113</v>
       </c>
-      <c r="C26">
+      <c r="C26" t="s">
+        <v>120</v>
+      </c>
+      <c r="D26">
         <v>20.48</v>
-      </c>
-      <c r="D26" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -2085,11 +2085,11 @@
       <c r="B27" t="s">
         <v>114</v>
       </c>
-      <c r="C27">
+      <c r="C27" t="s">
+        <v>120</v>
+      </c>
+      <c r="D27">
         <v>14.7</v>
-      </c>
-      <c r="D27" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -2099,11 +2099,11 @@
       <c r="B28" t="s">
         <v>115</v>
       </c>
-      <c r="C28">
+      <c r="C28" t="s">
+        <v>120</v>
+      </c>
+      <c r="D28">
         <v>20.67</v>
-      </c>
-      <c r="D28" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -2113,11 +2113,11 @@
       <c r="B29" t="s">
         <v>116</v>
       </c>
-      <c r="C29">
+      <c r="C29" t="s">
+        <v>120</v>
+      </c>
+      <c r="D29">
         <v>9.470000000000001</v>
-      </c>
-      <c r="D29" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -2127,11 +2127,11 @@
       <c r="B30" t="s">
         <v>117</v>
       </c>
-      <c r="C30">
+      <c r="C30" t="s">
+        <v>120</v>
+      </c>
+      <c r="D30">
         <v>9.32</v>
-      </c>
-      <c r="D30" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -2141,11 +2141,11 @@
       <c r="B31" t="s">
         <v>118</v>
       </c>
-      <c r="C31">
+      <c r="C31" t="s">
+        <v>120</v>
+      </c>
+      <c r="D31">
         <v>9.44</v>
-      </c>
-      <c r="D31" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -2155,11 +2155,11 @@
       <c r="B32" t="s">
         <v>119</v>
       </c>
-      <c r="C32">
+      <c r="C32" t="s">
+        <v>120</v>
+      </c>
+      <c r="D32">
         <v>9.59</v>
-      </c>
-      <c r="D32" t="s">
-        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -2191,10 +2191,10 @@
         <v>55</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -2204,11 +2204,11 @@
       <c r="B2" t="s">
         <v>89</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D2">
         <v>11.2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -2218,11 +2218,11 @@
       <c r="B3" t="s">
         <v>90</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D3">
         <v>16.52</v>
-      </c>
-      <c r="D3" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -2232,11 +2232,11 @@
       <c r="B4" t="s">
         <v>91</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4">
         <v>16.67</v>
-      </c>
-      <c r="D4" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -2246,11 +2246,11 @@
       <c r="B5" t="s">
         <v>92</v>
       </c>
-      <c r="C5">
+      <c r="C5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5">
         <v>5.58</v>
-      </c>
-      <c r="D5" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -2260,11 +2260,11 @@
       <c r="B6" t="s">
         <v>93</v>
       </c>
-      <c r="C6">
+      <c r="C6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D6">
         <v>5.73</v>
-      </c>
-      <c r="D6" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -2274,11 +2274,11 @@
       <c r="B7" t="s">
         <v>94</v>
       </c>
-      <c r="C7">
+      <c r="C7" t="s">
+        <v>120</v>
+      </c>
+      <c r="D7">
         <v>5.7</v>
-      </c>
-      <c r="D7" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -2288,11 +2288,11 @@
       <c r="B8" t="s">
         <v>95</v>
       </c>
-      <c r="C8">
+      <c r="C8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D8">
         <v>5.54</v>
-      </c>
-      <c r="D8" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -2302,11 +2302,11 @@
       <c r="B9" t="s">
         <v>96</v>
       </c>
-      <c r="C9">
+      <c r="C9" t="s">
+        <v>120</v>
+      </c>
+      <c r="D9">
         <v>17.87</v>
-      </c>
-      <c r="D9" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -2316,11 +2316,11 @@
       <c r="B10" t="s">
         <v>97</v>
       </c>
-      <c r="C10">
+      <c r="C10" t="s">
+        <v>120</v>
+      </c>
+      <c r="D10">
         <v>23.77</v>
-      </c>
-      <c r="D10" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -2330,11 +2330,11 @@
       <c r="B11" t="s">
         <v>98</v>
       </c>
-      <c r="C11">
+      <c r="C11" t="s">
+        <v>120</v>
+      </c>
+      <c r="D11">
         <v>18.57</v>
-      </c>
-      <c r="D11" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -2344,11 +2344,11 @@
       <c r="B12" t="s">
         <v>99</v>
       </c>
-      <c r="C12">
+      <c r="C12" t="s">
+        <v>120</v>
+      </c>
+      <c r="D12">
         <v>24.03</v>
-      </c>
-      <c r="D12" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -2358,11 +2358,11 @@
       <c r="B13" t="s">
         <v>100</v>
       </c>
-      <c r="C13">
+      <c r="C13" t="s">
+        <v>120</v>
+      </c>
+      <c r="D13">
         <v>10.89</v>
-      </c>
-      <c r="D13" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -2372,11 +2372,11 @@
       <c r="B14" t="s">
         <v>101</v>
       </c>
-      <c r="C14">
+      <c r="C14" t="s">
+        <v>120</v>
+      </c>
+      <c r="D14">
         <v>11.37</v>
-      </c>
-      <c r="D14" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -2386,11 +2386,11 @@
       <c r="B15" t="s">
         <v>102</v>
       </c>
-      <c r="C15">
+      <c r="C15" t="s">
+        <v>120</v>
+      </c>
+      <c r="D15">
         <v>11.4</v>
-      </c>
-      <c r="D15" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -2400,11 +2400,11 @@
       <c r="B16" t="s">
         <v>103</v>
       </c>
-      <c r="C16">
+      <c r="C16" t="s">
+        <v>120</v>
+      </c>
+      <c r="D16">
         <v>10.92</v>
-      </c>
-      <c r="D16" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -2414,11 +2414,11 @@
       <c r="B17" t="s">
         <v>104</v>
       </c>
-      <c r="C17">
+      <c r="C17" t="s">
+        <v>120</v>
+      </c>
+      <c r="D17">
         <v>18.81</v>
-      </c>
-      <c r="D17" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -2428,11 +2428,11 @@
       <c r="B18" t="s">
         <v>105</v>
       </c>
-      <c r="C18">
+      <c r="C18" t="s">
+        <v>120</v>
+      </c>
+      <c r="D18">
         <v>25.54</v>
-      </c>
-      <c r="D18" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -2442,11 +2442,11 @@
       <c r="B19" t="s">
         <v>106</v>
       </c>
-      <c r="C19">
+      <c r="C19" t="s">
+        <v>120</v>
+      </c>
+      <c r="D19">
         <v>19.47</v>
-      </c>
-      <c r="D19" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -2456,11 +2456,11 @@
       <c r="B20" t="s">
         <v>107</v>
       </c>
-      <c r="C20">
+      <c r="C20" t="s">
+        <v>120</v>
+      </c>
+      <c r="D20">
         <v>25.75</v>
-      </c>
-      <c r="D20" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -2470,11 +2470,11 @@
       <c r="B21" t="s">
         <v>108</v>
       </c>
-      <c r="C21">
+      <c r="C21" t="s">
+        <v>120</v>
+      </c>
+      <c r="D21">
         <v>11.87</v>
-      </c>
-      <c r="D21" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -2484,11 +2484,11 @@
       <c r="B22" t="s">
         <v>109</v>
       </c>
-      <c r="C22">
+      <c r="C22" t="s">
+        <v>120</v>
+      </c>
+      <c r="D22">
         <v>12.47</v>
-      </c>
-      <c r="D22" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -2498,11 +2498,11 @@
       <c r="B23" t="s">
         <v>110</v>
       </c>
-      <c r="C23">
+      <c r="C23" t="s">
+        <v>120</v>
+      </c>
+      <c r="D23">
         <v>12.67</v>
-      </c>
-      <c r="D23" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -2512,11 +2512,11 @@
       <c r="B24" t="s">
         <v>111</v>
       </c>
-      <c r="C24">
+      <c r="C24" t="s">
+        <v>120</v>
+      </c>
+      <c r="D24">
         <v>11.91</v>
-      </c>
-      <c r="D24" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -2526,11 +2526,11 @@
       <c r="B25" t="s">
         <v>112</v>
       </c>
-      <c r="C25">
+      <c r="C25" t="s">
+        <v>120</v>
+      </c>
+      <c r="D25">
         <v>14.45</v>
-      </c>
-      <c r="D25" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -2540,11 +2540,11 @@
       <c r="B26" t="s">
         <v>113</v>
       </c>
-      <c r="C26">
+      <c r="C26" t="s">
+        <v>120</v>
+      </c>
+      <c r="D26">
         <v>20.48</v>
-      </c>
-      <c r="D26" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -2554,11 +2554,11 @@
       <c r="B27" t="s">
         <v>114</v>
       </c>
-      <c r="C27">
+      <c r="C27" t="s">
+        <v>120</v>
+      </c>
+      <c r="D27">
         <v>14.7</v>
-      </c>
-      <c r="D27" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -2568,11 +2568,11 @@
       <c r="B28" t="s">
         <v>115</v>
       </c>
-      <c r="C28">
+      <c r="C28" t="s">
+        <v>120</v>
+      </c>
+      <c r="D28">
         <v>20.67</v>
-      </c>
-      <c r="D28" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -2582,11 +2582,11 @@
       <c r="B29" t="s">
         <v>116</v>
       </c>
-      <c r="C29">
+      <c r="C29" t="s">
+        <v>120</v>
+      </c>
+      <c r="D29">
         <v>9.470000000000001</v>
-      </c>
-      <c r="D29" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -2596,11 +2596,11 @@
       <c r="B30" t="s">
         <v>117</v>
       </c>
-      <c r="C30">
+      <c r="C30" t="s">
+        <v>120</v>
+      </c>
+      <c r="D30">
         <v>9.32</v>
-      </c>
-      <c r="D30" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -2610,11 +2610,11 @@
       <c r="B31" t="s">
         <v>118</v>
       </c>
-      <c r="C31">
+      <c r="C31" t="s">
+        <v>120</v>
+      </c>
+      <c r="D31">
         <v>9.44</v>
-      </c>
-      <c r="D31" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -2624,11 +2624,11 @@
       <c r="B32" t="s">
         <v>119</v>
       </c>
-      <c r="C32">
+      <c r="C32" t="s">
+        <v>120</v>
+      </c>
+      <c r="D32">
         <v>9.59</v>
-      </c>
-      <c r="D32" t="s">
-        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -2811,10 +2811,10 @@
         <v>55</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -2824,11 +2824,11 @@
       <c r="B2" t="s">
         <v>89</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D2">
         <v>11.21</v>
-      </c>
-      <c r="D2" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -2838,11 +2838,11 @@
       <c r="B3" t="s">
         <v>90</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D3">
         <v>16.33</v>
-      </c>
-      <c r="D3" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -2852,11 +2852,11 @@
       <c r="B4" t="s">
         <v>91</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4">
         <v>16.52</v>
-      </c>
-      <c r="D4" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -2866,11 +2866,11 @@
       <c r="B5" t="s">
         <v>92</v>
       </c>
-      <c r="C5">
+      <c r="C5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5">
         <v>5.57</v>
-      </c>
-      <c r="D5" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -2880,11 +2880,11 @@
       <c r="B6" t="s">
         <v>93</v>
       </c>
-      <c r="C6">
+      <c r="C6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D6">
         <v>5.76</v>
-      </c>
-      <c r="D6" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -2894,11 +2894,11 @@
       <c r="B7" t="s">
         <v>94</v>
       </c>
-      <c r="C7">
+      <c r="C7" t="s">
+        <v>120</v>
+      </c>
+      <c r="D7">
         <v>5.65</v>
-      </c>
-      <c r="D7" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -2908,11 +2908,11 @@
       <c r="B8" t="s">
         <v>95</v>
       </c>
-      <c r="C8">
+      <c r="C8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D8">
         <v>5.56</v>
-      </c>
-      <c r="D8" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -2922,11 +2922,11 @@
       <c r="B9" t="s">
         <v>96</v>
       </c>
-      <c r="C9">
+      <c r="C9" t="s">
+        <v>120</v>
+      </c>
+      <c r="D9">
         <v>17.87</v>
-      </c>
-      <c r="D9" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -2936,11 +2936,11 @@
       <c r="B10" t="s">
         <v>97</v>
       </c>
-      <c r="C10">
+      <c r="C10" t="s">
+        <v>120</v>
+      </c>
+      <c r="D10">
         <v>23.69</v>
-      </c>
-      <c r="D10" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -2950,11 +2950,11 @@
       <c r="B11" t="s">
         <v>98</v>
       </c>
-      <c r="C11">
+      <c r="C11" t="s">
+        <v>120</v>
+      </c>
+      <c r="D11">
         <v>18.61</v>
-      </c>
-      <c r="D11" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -2964,11 +2964,11 @@
       <c r="B12" t="s">
         <v>99</v>
       </c>
-      <c r="C12">
+      <c r="C12" t="s">
+        <v>120</v>
+      </c>
+      <c r="D12">
         <v>23.88</v>
-      </c>
-      <c r="D12" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -2978,11 +2978,11 @@
       <c r="B13" t="s">
         <v>100</v>
       </c>
-      <c r="C13">
+      <c r="C13" t="s">
+        <v>120</v>
+      </c>
+      <c r="D13">
         <v>10.95</v>
-      </c>
-      <c r="D13" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -2992,11 +2992,11 @@
       <c r="B14" t="s">
         <v>101</v>
       </c>
-      <c r="C14">
+      <c r="C14" t="s">
+        <v>120</v>
+      </c>
+      <c r="D14">
         <v>11.38</v>
-      </c>
-      <c r="D14" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -3006,11 +3006,11 @@
       <c r="B15" t="s">
         <v>102</v>
       </c>
-      <c r="C15">
+      <c r="C15" t="s">
+        <v>120</v>
+      </c>
+      <c r="D15">
         <v>11.39</v>
-      </c>
-      <c r="D15" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -3020,11 +3020,11 @@
       <c r="B16" t="s">
         <v>103</v>
       </c>
-      <c r="C16">
+      <c r="C16" t="s">
+        <v>120</v>
+      </c>
+      <c r="D16">
         <v>10.94</v>
-      </c>
-      <c r="D16" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -3034,11 +3034,11 @@
       <c r="B17" t="s">
         <v>104</v>
       </c>
-      <c r="C17">
+      <c r="C17" t="s">
+        <v>120</v>
+      </c>
+      <c r="D17">
         <v>18.82</v>
-      </c>
-      <c r="D17" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -3048,11 +3048,11 @@
       <c r="B18" t="s">
         <v>105</v>
       </c>
-      <c r="C18">
+      <c r="C18" t="s">
+        <v>120</v>
+      </c>
+      <c r="D18">
         <v>25.37</v>
-      </c>
-      <c r="D18" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -3062,11 +3062,11 @@
       <c r="B19" t="s">
         <v>106</v>
       </c>
-      <c r="C19">
+      <c r="C19" t="s">
+        <v>120</v>
+      </c>
+      <c r="D19">
         <v>19.5</v>
-      </c>
-      <c r="D19" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -3076,11 +3076,11 @@
       <c r="B20" t="s">
         <v>107</v>
       </c>
-      <c r="C20">
+      <c r="C20" t="s">
+        <v>120</v>
+      </c>
+      <c r="D20">
         <v>25.58</v>
-      </c>
-      <c r="D20" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -3090,11 +3090,11 @@
       <c r="B21" t="s">
         <v>108</v>
       </c>
-      <c r="C21">
+      <c r="C21" t="s">
+        <v>120</v>
+      </c>
+      <c r="D21">
         <v>11.91</v>
-      </c>
-      <c r="D21" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -3104,11 +3104,11 @@
       <c r="B22" t="s">
         <v>109</v>
       </c>
-      <c r="C22">
+      <c r="C22" t="s">
+        <v>120</v>
+      </c>
+      <c r="D22">
         <v>12.49</v>
-      </c>
-      <c r="D22" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -3118,11 +3118,11 @@
       <c r="B23" t="s">
         <v>110</v>
       </c>
-      <c r="C23">
+      <c r="C23" t="s">
+        <v>120</v>
+      </c>
+      <c r="D23">
         <v>12.67</v>
-      </c>
-      <c r="D23" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -3132,11 +3132,11 @@
       <c r="B24" t="s">
         <v>111</v>
       </c>
-      <c r="C24">
+      <c r="C24" t="s">
+        <v>120</v>
+      </c>
+      <c r="D24">
         <v>11.93</v>
-      </c>
-      <c r="D24" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -3146,11 +3146,11 @@
       <c r="B25" t="s">
         <v>112</v>
       </c>
-      <c r="C25">
+      <c r="C25" t="s">
+        <v>120</v>
+      </c>
+      <c r="D25">
         <v>14.45</v>
-      </c>
-      <c r="D25" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -3160,11 +3160,11 @@
       <c r="B26" t="s">
         <v>113</v>
       </c>
-      <c r="C26">
+      <c r="C26" t="s">
+        <v>120</v>
+      </c>
+      <c r="D26">
         <v>20.3</v>
-      </c>
-      <c r="D26" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -3174,11 +3174,11 @@
       <c r="B27" t="s">
         <v>114</v>
       </c>
-      <c r="C27">
+      <c r="C27" t="s">
+        <v>120</v>
+      </c>
+      <c r="D27">
         <v>14.67</v>
-      </c>
-      <c r="D27" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -3188,11 +3188,11 @@
       <c r="B28" t="s">
         <v>115</v>
       </c>
-      <c r="C28">
+      <c r="C28" t="s">
+        <v>120</v>
+      </c>
+      <c r="D28">
         <v>20.42</v>
-      </c>
-      <c r="D28" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -3202,11 +3202,11 @@
       <c r="B29" t="s">
         <v>116</v>
       </c>
-      <c r="C29">
+      <c r="C29" t="s">
+        <v>120</v>
+      </c>
+      <c r="D29">
         <v>9.470000000000001</v>
-      </c>
-      <c r="D29" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -3216,11 +3216,11 @@
       <c r="B30" t="s">
         <v>117</v>
       </c>
-      <c r="C30">
+      <c r="C30" t="s">
+        <v>120</v>
+      </c>
+      <c r="D30">
         <v>9.33</v>
-      </c>
-      <c r="D30" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -3230,11 +3230,11 @@
       <c r="B31" t="s">
         <v>118</v>
       </c>
-      <c r="C31">
+      <c r="C31" t="s">
+        <v>120</v>
+      </c>
+      <c r="D31">
         <v>9.460000000000001</v>
-      </c>
-      <c r="D31" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -3244,11 +3244,11 @@
       <c r="B32" t="s">
         <v>119</v>
       </c>
-      <c r="C32">
+      <c r="C32" t="s">
+        <v>120</v>
+      </c>
+      <c r="D32">
         <v>9.58</v>
-      </c>
-      <c r="D32" t="s">
-        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -3280,10 +3280,10 @@
         <v>55</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -3293,11 +3293,11 @@
       <c r="B2" t="s">
         <v>89</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D2">
         <v>11.21</v>
-      </c>
-      <c r="D2" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -3307,11 +3307,11 @@
       <c r="B3" t="s">
         <v>90</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D3">
         <v>16.33</v>
-      </c>
-      <c r="D3" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -3321,11 +3321,11 @@
       <c r="B4" t="s">
         <v>91</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4">
         <v>16.56</v>
-      </c>
-      <c r="D4" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -3335,11 +3335,11 @@
       <c r="B5" t="s">
         <v>92</v>
       </c>
-      <c r="C5">
+      <c r="C5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5">
         <v>5.57</v>
-      </c>
-      <c r="D5" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -3349,11 +3349,11 @@
       <c r="B6" t="s">
         <v>93</v>
       </c>
-      <c r="C6">
+      <c r="C6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D6">
         <v>5.76</v>
-      </c>
-      <c r="D6" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -3363,11 +3363,11 @@
       <c r="B7" t="s">
         <v>94</v>
       </c>
-      <c r="C7">
+      <c r="C7" t="s">
+        <v>120</v>
+      </c>
+      <c r="D7">
         <v>5.66</v>
-      </c>
-      <c r="D7" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -3377,11 +3377,11 @@
       <c r="B8" t="s">
         <v>95</v>
       </c>
-      <c r="C8">
+      <c r="C8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D8">
         <v>5.57</v>
-      </c>
-      <c r="D8" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -3391,11 +3391,11 @@
       <c r="B9" t="s">
         <v>96</v>
       </c>
-      <c r="C9">
+      <c r="C9" t="s">
+        <v>120</v>
+      </c>
+      <c r="D9">
         <v>17.87</v>
-      </c>
-      <c r="D9" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -3405,11 +3405,11 @@
       <c r="B10" t="s">
         <v>97</v>
       </c>
-      <c r="C10">
+      <c r="C10" t="s">
+        <v>120</v>
+      </c>
+      <c r="D10">
         <v>23.73</v>
-      </c>
-      <c r="D10" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -3419,11 +3419,11 @@
       <c r="B11" t="s">
         <v>98</v>
       </c>
-      <c r="C11">
+      <c r="C11" t="s">
+        <v>120</v>
+      </c>
+      <c r="D11">
         <v>18.6</v>
-      </c>
-      <c r="D11" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -3433,11 +3433,11 @@
       <c r="B12" t="s">
         <v>99</v>
       </c>
-      <c r="C12">
+      <c r="C12" t="s">
+        <v>120</v>
+      </c>
+      <c r="D12">
         <v>23.9</v>
-      </c>
-      <c r="D12" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -3447,11 +3447,11 @@
       <c r="B13" t="s">
         <v>100</v>
       </c>
-      <c r="C13">
+      <c r="C13" t="s">
+        <v>120</v>
+      </c>
+      <c r="D13">
         <v>10.95</v>
-      </c>
-      <c r="D13" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -3461,11 +3461,11 @@
       <c r="B14" t="s">
         <v>101</v>
       </c>
-      <c r="C14">
+      <c r="C14" t="s">
+        <v>120</v>
+      </c>
+      <c r="D14">
         <v>11.37</v>
-      </c>
-      <c r="D14" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -3475,11 +3475,11 @@
       <c r="B15" t="s">
         <v>102</v>
       </c>
-      <c r="C15">
+      <c r="C15" t="s">
+        <v>120</v>
+      </c>
+      <c r="D15">
         <v>11.4</v>
-      </c>
-      <c r="D15" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -3489,11 +3489,11 @@
       <c r="B16" t="s">
         <v>103</v>
       </c>
-      <c r="C16">
+      <c r="C16" t="s">
+        <v>120</v>
+      </c>
+      <c r="D16">
         <v>10.95</v>
-      </c>
-      <c r="D16" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -3503,11 +3503,11 @@
       <c r="B17" t="s">
         <v>104</v>
       </c>
-      <c r="C17">
+      <c r="C17" t="s">
+        <v>120</v>
+      </c>
+      <c r="D17">
         <v>18.8</v>
-      </c>
-      <c r="D17" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -3517,11 +3517,11 @@
       <c r="B18" t="s">
         <v>105</v>
       </c>
-      <c r="C18">
+      <c r="C18" t="s">
+        <v>120</v>
+      </c>
+      <c r="D18">
         <v>25.37</v>
-      </c>
-      <c r="D18" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -3531,11 +3531,11 @@
       <c r="B19" t="s">
         <v>106</v>
       </c>
-      <c r="C19">
+      <c r="C19" t="s">
+        <v>120</v>
+      </c>
+      <c r="D19">
         <v>19.5</v>
-      </c>
-      <c r="D19" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -3545,11 +3545,11 @@
       <c r="B20" t="s">
         <v>107</v>
       </c>
-      <c r="C20">
+      <c r="C20" t="s">
+        <v>120</v>
+      </c>
+      <c r="D20">
         <v>25.61</v>
-      </c>
-      <c r="D20" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -3559,11 +3559,11 @@
       <c r="B21" t="s">
         <v>108</v>
       </c>
-      <c r="C21">
+      <c r="C21" t="s">
+        <v>120</v>
+      </c>
+      <c r="D21">
         <v>11.89</v>
-      </c>
-      <c r="D21" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -3573,11 +3573,11 @@
       <c r="B22" t="s">
         <v>109</v>
       </c>
-      <c r="C22">
+      <c r="C22" t="s">
+        <v>120</v>
+      </c>
+      <c r="D22">
         <v>12.47</v>
-      </c>
-      <c r="D22" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -3587,11 +3587,11 @@
       <c r="B23" t="s">
         <v>110</v>
       </c>
-      <c r="C23">
+      <c r="C23" t="s">
+        <v>120</v>
+      </c>
+      <c r="D23">
         <v>12.67</v>
-      </c>
-      <c r="D23" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -3601,11 +3601,11 @@
       <c r="B24" t="s">
         <v>111</v>
       </c>
-      <c r="C24">
+      <c r="C24" t="s">
+        <v>120</v>
+      </c>
+      <c r="D24">
         <v>11.93</v>
-      </c>
-      <c r="D24" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -3615,11 +3615,11 @@
       <c r="B25" t="s">
         <v>112</v>
       </c>
-      <c r="C25">
+      <c r="C25" t="s">
+        <v>120</v>
+      </c>
+      <c r="D25">
         <v>14.45</v>
-      </c>
-      <c r="D25" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -3629,11 +3629,11 @@
       <c r="B26" t="s">
         <v>113</v>
       </c>
-      <c r="C26">
+      <c r="C26" t="s">
+        <v>120</v>
+      </c>
+      <c r="D26">
         <v>20.32</v>
-      </c>
-      <c r="D26" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -3643,11 +3643,11 @@
       <c r="B27" t="s">
         <v>114</v>
       </c>
-      <c r="C27">
+      <c r="C27" t="s">
+        <v>120</v>
+      </c>
+      <c r="D27">
         <v>14.67</v>
-      </c>
-      <c r="D27" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -3657,11 +3657,11 @@
       <c r="B28" t="s">
         <v>115</v>
       </c>
-      <c r="C28">
+      <c r="C28" t="s">
+        <v>120</v>
+      </c>
+      <c r="D28">
         <v>20.48</v>
-      </c>
-      <c r="D28" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -3671,11 +3671,11 @@
       <c r="B29" t="s">
         <v>116</v>
       </c>
-      <c r="C29">
+      <c r="C29" t="s">
+        <v>120</v>
+      </c>
+      <c r="D29">
         <v>9.460000000000001</v>
-      </c>
-      <c r="D29" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -3685,11 +3685,11 @@
       <c r="B30" t="s">
         <v>117</v>
       </c>
-      <c r="C30">
+      <c r="C30" t="s">
+        <v>120</v>
+      </c>
+      <c r="D30">
         <v>9.33</v>
-      </c>
-      <c r="D30" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -3699,11 +3699,11 @@
       <c r="B31" t="s">
         <v>118</v>
       </c>
-      <c r="C31">
+      <c r="C31" t="s">
+        <v>120</v>
+      </c>
+      <c r="D31">
         <v>9.449999999999999</v>
-      </c>
-      <c r="D31" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -3713,11 +3713,11 @@
       <c r="B32" t="s">
         <v>119</v>
       </c>
-      <c r="C32">
+      <c r="C32" t="s">
+        <v>120</v>
+      </c>
+      <c r="D32">
         <v>9.59</v>
-      </c>
-      <c r="D32" t="s">
-        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -3749,10 +3749,10 @@
         <v>55</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -3762,11 +3762,11 @@
       <c r="B2" t="s">
         <v>89</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D2">
         <v>11.2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -3776,11 +3776,11 @@
       <c r="B3" t="s">
         <v>90</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D3">
         <v>16.42</v>
-      </c>
-      <c r="D3" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -3790,11 +3790,11 @@
       <c r="B4" t="s">
         <v>91</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4">
         <v>16.59</v>
-      </c>
-      <c r="D4" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -3804,11 +3804,11 @@
       <c r="B5" t="s">
         <v>92</v>
       </c>
-      <c r="C5">
+      <c r="C5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5">
         <v>5.57</v>
-      </c>
-      <c r="D5" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -3818,11 +3818,11 @@
       <c r="B6" t="s">
         <v>93</v>
       </c>
-      <c r="C6">
+      <c r="C6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D6">
         <v>5.76</v>
-      </c>
-      <c r="D6" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -3832,11 +3832,11 @@
       <c r="B7" t="s">
         <v>94</v>
       </c>
-      <c r="C7">
+      <c r="C7" t="s">
+        <v>120</v>
+      </c>
+      <c r="D7">
         <v>5.67</v>
-      </c>
-      <c r="D7" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -3846,11 +3846,11 @@
       <c r="B8" t="s">
         <v>95</v>
       </c>
-      <c r="C8">
+      <c r="C8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D8">
         <v>5.58</v>
-      </c>
-      <c r="D8" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -3860,11 +3860,11 @@
       <c r="B9" t="s">
         <v>96</v>
       </c>
-      <c r="C9">
+      <c r="C9" t="s">
+        <v>120</v>
+      </c>
+      <c r="D9">
         <v>17.87</v>
-      </c>
-      <c r="D9" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -3874,11 +3874,11 @@
       <c r="B10" t="s">
         <v>97</v>
       </c>
-      <c r="C10">
+      <c r="C10" t="s">
+        <v>120</v>
+      </c>
+      <c r="D10">
         <v>23.73</v>
-      </c>
-      <c r="D10" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -3888,11 +3888,11 @@
       <c r="B11" t="s">
         <v>98</v>
       </c>
-      <c r="C11">
+      <c r="C11" t="s">
+        <v>120</v>
+      </c>
+      <c r="D11">
         <v>18.58</v>
-      </c>
-      <c r="D11" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -3902,11 +3902,11 @@
       <c r="B12" t="s">
         <v>99</v>
       </c>
-      <c r="C12">
+      <c r="C12" t="s">
+        <v>120</v>
+      </c>
+      <c r="D12">
         <v>23.9</v>
-      </c>
-      <c r="D12" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -3916,11 +3916,11 @@
       <c r="B13" t="s">
         <v>100</v>
       </c>
-      <c r="C13">
+      <c r="C13" t="s">
+        <v>120</v>
+      </c>
+      <c r="D13">
         <v>10.94</v>
-      </c>
-      <c r="D13" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -3930,11 +3930,11 @@
       <c r="B14" t="s">
         <v>101</v>
       </c>
-      <c r="C14">
+      <c r="C14" t="s">
+        <v>120</v>
+      </c>
+      <c r="D14">
         <v>11.37</v>
-      </c>
-      <c r="D14" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -3944,11 +3944,11 @@
       <c r="B15" t="s">
         <v>102</v>
       </c>
-      <c r="C15">
+      <c r="C15" t="s">
+        <v>120</v>
+      </c>
+      <c r="D15">
         <v>11.39</v>
-      </c>
-      <c r="D15" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -3958,11 +3958,11 @@
       <c r="B16" t="s">
         <v>103</v>
       </c>
-      <c r="C16">
+      <c r="C16" t="s">
+        <v>120</v>
+      </c>
+      <c r="D16">
         <v>10.95</v>
-      </c>
-      <c r="D16" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -3972,11 +3972,11 @@
       <c r="B17" t="s">
         <v>104</v>
       </c>
-      <c r="C17">
+      <c r="C17" t="s">
+        <v>120</v>
+      </c>
+      <c r="D17">
         <v>18.8</v>
-      </c>
-      <c r="D17" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -3986,11 +3986,11 @@
       <c r="B18" t="s">
         <v>105</v>
       </c>
-      <c r="C18">
+      <c r="C18" t="s">
+        <v>120</v>
+      </c>
+      <c r="D18">
         <v>25.48</v>
-      </c>
-      <c r="D18" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -4000,11 +4000,11 @@
       <c r="B19" t="s">
         <v>106</v>
       </c>
-      <c r="C19">
+      <c r="C19" t="s">
+        <v>120</v>
+      </c>
+      <c r="D19">
         <v>19.5</v>
-      </c>
-      <c r="D19" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -4014,11 +4014,11 @@
       <c r="B20" t="s">
         <v>107</v>
       </c>
-      <c r="C20">
+      <c r="C20" t="s">
+        <v>120</v>
+      </c>
+      <c r="D20">
         <v>25.63</v>
-      </c>
-      <c r="D20" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -4028,11 +4028,11 @@
       <c r="B21" t="s">
         <v>108</v>
       </c>
-      <c r="C21">
+      <c r="C21" t="s">
+        <v>120</v>
+      </c>
+      <c r="D21">
         <v>11.89</v>
-      </c>
-      <c r="D21" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -4042,11 +4042,11 @@
       <c r="B22" t="s">
         <v>109</v>
       </c>
-      <c r="C22">
+      <c r="C22" t="s">
+        <v>120</v>
+      </c>
+      <c r="D22">
         <v>12.45</v>
-      </c>
-      <c r="D22" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -4056,11 +4056,11 @@
       <c r="B23" t="s">
         <v>110</v>
       </c>
-      <c r="C23">
+      <c r="C23" t="s">
+        <v>120</v>
+      </c>
+      <c r="D23">
         <v>12.68</v>
-      </c>
-      <c r="D23" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -4070,11 +4070,11 @@
       <c r="B24" t="s">
         <v>111</v>
       </c>
-      <c r="C24">
+      <c r="C24" t="s">
+        <v>120</v>
+      </c>
+      <c r="D24">
         <v>11.94</v>
-      </c>
-      <c r="D24" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -4084,11 +4084,11 @@
       <c r="B25" t="s">
         <v>112</v>
       </c>
-      <c r="C25">
+      <c r="C25" t="s">
+        <v>120</v>
+      </c>
+      <c r="D25">
         <v>14.47</v>
-      </c>
-      <c r="D25" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -4098,11 +4098,11 @@
       <c r="B26" t="s">
         <v>113</v>
       </c>
-      <c r="C26">
+      <c r="C26" t="s">
+        <v>120</v>
+      </c>
+      <c r="D26">
         <v>20.36</v>
-      </c>
-      <c r="D26" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -4112,11 +4112,11 @@
       <c r="B27" t="s">
         <v>114</v>
       </c>
-      <c r="C27">
+      <c r="C27" t="s">
+        <v>120</v>
+      </c>
+      <c r="D27">
         <v>14.69</v>
-      </c>
-      <c r="D27" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -4126,11 +4126,11 @@
       <c r="B28" t="s">
         <v>115</v>
       </c>
-      <c r="C28">
+      <c r="C28" t="s">
+        <v>120</v>
+      </c>
+      <c r="D28">
         <v>20.53</v>
-      </c>
-      <c r="D28" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -4140,11 +4140,11 @@
       <c r="B29" t="s">
         <v>116</v>
       </c>
-      <c r="C29">
+      <c r="C29" t="s">
+        <v>120</v>
+      </c>
+      <c r="D29">
         <v>9.460000000000001</v>
-      </c>
-      <c r="D29" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -4154,11 +4154,11 @@
       <c r="B30" t="s">
         <v>117</v>
       </c>
-      <c r="C30">
+      <c r="C30" t="s">
+        <v>120</v>
+      </c>
+      <c r="D30">
         <v>9.32</v>
-      </c>
-      <c r="D30" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -4168,11 +4168,11 @@
       <c r="B31" t="s">
         <v>118</v>
       </c>
-      <c r="C31">
+      <c r="C31" t="s">
+        <v>120</v>
+      </c>
+      <c r="D31">
         <v>9.449999999999999</v>
-      </c>
-      <c r="D31" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -4182,11 +4182,11 @@
       <c r="B32" t="s">
         <v>119</v>
       </c>
-      <c r="C32">
+      <c r="C32" t="s">
+        <v>120</v>
+      </c>
+      <c r="D32">
         <v>9.59</v>
-      </c>
-      <c r="D32" t="s">
-        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -4218,10 +4218,10 @@
         <v>55</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -4231,11 +4231,11 @@
       <c r="B2" t="s">
         <v>89</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D2">
         <v>11.2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -4245,11 +4245,11 @@
       <c r="B3" t="s">
         <v>90</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D3">
         <v>16.44</v>
-      </c>
-      <c r="D3" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -4259,11 +4259,11 @@
       <c r="B4" t="s">
         <v>91</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4">
         <v>16.63</v>
-      </c>
-      <c r="D4" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -4273,11 +4273,11 @@
       <c r="B5" t="s">
         <v>92</v>
       </c>
-      <c r="C5">
+      <c r="C5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5">
         <v>5.57</v>
-      </c>
-      <c r="D5" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -4287,11 +4287,11 @@
       <c r="B6" t="s">
         <v>93</v>
       </c>
-      <c r="C6">
+      <c r="C6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D6">
         <v>5.75</v>
-      </c>
-      <c r="D6" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -4301,11 +4301,11 @@
       <c r="B7" t="s">
         <v>94</v>
       </c>
-      <c r="C7">
+      <c r="C7" t="s">
+        <v>120</v>
+      </c>
+      <c r="D7">
         <v>5.7</v>
-      </c>
-      <c r="D7" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -4315,11 +4315,11 @@
       <c r="B8" t="s">
         <v>95</v>
       </c>
-      <c r="C8">
+      <c r="C8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D8">
         <v>5.56</v>
-      </c>
-      <c r="D8" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -4329,11 +4329,11 @@
       <c r="B9" t="s">
         <v>96</v>
       </c>
-      <c r="C9">
+      <c r="C9" t="s">
+        <v>120</v>
+      </c>
+      <c r="D9">
         <v>17.87</v>
-      </c>
-      <c r="D9" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -4343,11 +4343,11 @@
       <c r="B10" t="s">
         <v>97</v>
       </c>
-      <c r="C10">
+      <c r="C10" t="s">
+        <v>120</v>
+      </c>
+      <c r="D10">
         <v>23.73</v>
-      </c>
-      <c r="D10" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -4357,11 +4357,11 @@
       <c r="B11" t="s">
         <v>98</v>
       </c>
-      <c r="C11">
+      <c r="C11" t="s">
+        <v>120</v>
+      </c>
+      <c r="D11">
         <v>18.57</v>
-      </c>
-      <c r="D11" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -4371,11 +4371,11 @@
       <c r="B12" t="s">
         <v>99</v>
       </c>
-      <c r="C12">
+      <c r="C12" t="s">
+        <v>120</v>
+      </c>
+      <c r="D12">
         <v>23.96</v>
-      </c>
-      <c r="D12" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -4385,11 +4385,11 @@
       <c r="B13" t="s">
         <v>100</v>
       </c>
-      <c r="C13">
+      <c r="C13" t="s">
+        <v>120</v>
+      </c>
+      <c r="D13">
         <v>10.94</v>
-      </c>
-      <c r="D13" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -4399,11 +4399,11 @@
       <c r="B14" t="s">
         <v>101</v>
       </c>
-      <c r="C14">
+      <c r="C14" t="s">
+        <v>120</v>
+      </c>
+      <c r="D14">
         <v>11.37</v>
-      </c>
-      <c r="D14" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -4413,11 +4413,11 @@
       <c r="B15" t="s">
         <v>102</v>
       </c>
-      <c r="C15">
+      <c r="C15" t="s">
+        <v>120</v>
+      </c>
+      <c r="D15">
         <v>11.42</v>
-      </c>
-      <c r="D15" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -4427,11 +4427,11 @@
       <c r="B16" t="s">
         <v>103</v>
       </c>
-      <c r="C16">
+      <c r="C16" t="s">
+        <v>120</v>
+      </c>
+      <c r="D16">
         <v>10.95</v>
-      </c>
-      <c r="D16" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -4441,11 +4441,11 @@
       <c r="B17" t="s">
         <v>104</v>
       </c>
-      <c r="C17">
+      <c r="C17" t="s">
+        <v>120</v>
+      </c>
+      <c r="D17">
         <v>18.8</v>
-      </c>
-      <c r="D17" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -4455,11 +4455,11 @@
       <c r="B18" t="s">
         <v>105</v>
       </c>
-      <c r="C18">
+      <c r="C18" t="s">
+        <v>120</v>
+      </c>
+      <c r="D18">
         <v>25.48</v>
-      </c>
-      <c r="D18" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -4469,11 +4469,11 @@
       <c r="B19" t="s">
         <v>106</v>
       </c>
-      <c r="C19">
+      <c r="C19" t="s">
+        <v>120</v>
+      </c>
+      <c r="D19">
         <v>19.5</v>
-      </c>
-      <c r="D19" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -4483,11 +4483,11 @@
       <c r="B20" t="s">
         <v>107</v>
       </c>
-      <c r="C20">
+      <c r="C20" t="s">
+        <v>120</v>
+      </c>
+      <c r="D20">
         <v>25.71</v>
-      </c>
-      <c r="D20" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -4497,11 +4497,11 @@
       <c r="B21" t="s">
         <v>108</v>
       </c>
-      <c r="C21">
+      <c r="C21" t="s">
+        <v>120</v>
+      </c>
+      <c r="D21">
         <v>11.89</v>
-      </c>
-      <c r="D21" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -4511,11 +4511,11 @@
       <c r="B22" t="s">
         <v>109</v>
       </c>
-      <c r="C22">
+      <c r="C22" t="s">
+        <v>120</v>
+      </c>
+      <c r="D22">
         <v>12.48</v>
-      </c>
-      <c r="D22" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -4525,11 +4525,11 @@
       <c r="B23" t="s">
         <v>110</v>
       </c>
-      <c r="C23">
+      <c r="C23" t="s">
+        <v>120</v>
+      </c>
+      <c r="D23">
         <v>12.65</v>
-      </c>
-      <c r="D23" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -4539,11 +4539,11 @@
       <c r="B24" t="s">
         <v>111</v>
       </c>
-      <c r="C24">
+      <c r="C24" t="s">
+        <v>120</v>
+      </c>
+      <c r="D24">
         <v>11.93</v>
-      </c>
-      <c r="D24" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -4553,11 +4553,11 @@
       <c r="B25" t="s">
         <v>112</v>
       </c>
-      <c r="C25">
+      <c r="C25" t="s">
+        <v>120</v>
+      </c>
+      <c r="D25">
         <v>14.47</v>
-      </c>
-      <c r="D25" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -4567,11 +4567,11 @@
       <c r="B26" t="s">
         <v>113</v>
       </c>
-      <c r="C26">
+      <c r="C26" t="s">
+        <v>120</v>
+      </c>
+      <c r="D26">
         <v>20.36</v>
-      </c>
-      <c r="D26" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -4581,11 +4581,11 @@
       <c r="B27" t="s">
         <v>114</v>
       </c>
-      <c r="C27">
+      <c r="C27" t="s">
+        <v>120</v>
+      </c>
+      <c r="D27">
         <v>14.69</v>
-      </c>
-      <c r="D27" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -4595,11 +4595,11 @@
       <c r="B28" t="s">
         <v>115</v>
       </c>
-      <c r="C28">
+      <c r="C28" t="s">
+        <v>120</v>
+      </c>
+      <c r="D28">
         <v>20.57</v>
-      </c>
-      <c r="D28" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -4609,11 +4609,11 @@
       <c r="B29" t="s">
         <v>116</v>
       </c>
-      <c r="C29">
+      <c r="C29" t="s">
+        <v>120</v>
+      </c>
+      <c r="D29">
         <v>9.460000000000001</v>
-      </c>
-      <c r="D29" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -4623,11 +4623,11 @@
       <c r="B30" t="s">
         <v>117</v>
       </c>
-      <c r="C30">
+      <c r="C30" t="s">
+        <v>120</v>
+      </c>
+      <c r="D30">
         <v>9.32</v>
-      </c>
-      <c r="D30" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -4637,11 +4637,11 @@
       <c r="B31" t="s">
         <v>118</v>
       </c>
-      <c r="C31">
+      <c r="C31" t="s">
+        <v>120</v>
+      </c>
+      <c r="D31">
         <v>9.449999999999999</v>
-      </c>
-      <c r="D31" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -4651,11 +4651,11 @@
       <c r="B32" t="s">
         <v>119</v>
       </c>
-      <c r="C32">
+      <c r="C32" t="s">
+        <v>120</v>
+      </c>
+      <c r="D32">
         <v>9.59</v>
-      </c>
-      <c r="D32" t="s">
-        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -4687,10 +4687,10 @@
         <v>55</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -4700,11 +4700,11 @@
       <c r="B2" t="s">
         <v>89</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D2">
         <v>11.21</v>
-      </c>
-      <c r="D2" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -4714,11 +4714,11 @@
       <c r="B3" t="s">
         <v>90</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D3">
         <v>16.46</v>
-      </c>
-      <c r="D3" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -4728,11 +4728,11 @@
       <c r="B4" t="s">
         <v>91</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4">
         <v>16.65</v>
-      </c>
-      <c r="D4" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -4742,11 +4742,11 @@
       <c r="B5" t="s">
         <v>92</v>
       </c>
-      <c r="C5">
+      <c r="C5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5">
         <v>5.57</v>
-      </c>
-      <c r="D5" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -4756,11 +4756,11 @@
       <c r="B6" t="s">
         <v>93</v>
       </c>
-      <c r="C6">
+      <c r="C6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D6">
         <v>5.74</v>
-      </c>
-      <c r="D6" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -4770,11 +4770,11 @@
       <c r="B7" t="s">
         <v>94</v>
       </c>
-      <c r="C7">
+      <c r="C7" t="s">
+        <v>120</v>
+      </c>
+      <c r="D7">
         <v>5.7</v>
-      </c>
-      <c r="D7" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -4784,11 +4784,11 @@
       <c r="B8" t="s">
         <v>95</v>
       </c>
-      <c r="C8">
+      <c r="C8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D8">
         <v>5.56</v>
-      </c>
-      <c r="D8" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -4798,11 +4798,11 @@
       <c r="B9" t="s">
         <v>96</v>
       </c>
-      <c r="C9">
+      <c r="C9" t="s">
+        <v>120</v>
+      </c>
+      <c r="D9">
         <v>17.85</v>
-      </c>
-      <c r="D9" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -4812,11 +4812,11 @@
       <c r="B10" t="s">
         <v>97</v>
       </c>
-      <c r="C10">
+      <c r="C10" t="s">
+        <v>120</v>
+      </c>
+      <c r="D10">
         <v>23.73</v>
-      </c>
-      <c r="D10" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -4826,11 +4826,11 @@
       <c r="B11" t="s">
         <v>98</v>
       </c>
-      <c r="C11">
+      <c r="C11" t="s">
+        <v>120</v>
+      </c>
+      <c r="D11">
         <v>18.56</v>
-      </c>
-      <c r="D11" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -4840,11 +4840,11 @@
       <c r="B12" t="s">
         <v>99</v>
       </c>
-      <c r="C12">
+      <c r="C12" t="s">
+        <v>120</v>
+      </c>
+      <c r="D12">
         <v>23.96</v>
-      </c>
-      <c r="D12" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -4854,11 +4854,11 @@
       <c r="B13" t="s">
         <v>100</v>
       </c>
-      <c r="C13">
+      <c r="C13" t="s">
+        <v>120</v>
+      </c>
+      <c r="D13">
         <v>10.91</v>
-      </c>
-      <c r="D13" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -4868,11 +4868,11 @@
       <c r="B14" t="s">
         <v>101</v>
       </c>
-      <c r="C14">
+      <c r="C14" t="s">
+        <v>120</v>
+      </c>
+      <c r="D14">
         <v>11.37</v>
-      </c>
-      <c r="D14" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -4882,11 +4882,11 @@
       <c r="B15" t="s">
         <v>102</v>
       </c>
-      <c r="C15">
+      <c r="C15" t="s">
+        <v>120</v>
+      </c>
+      <c r="D15">
         <v>11.4</v>
-      </c>
-      <c r="D15" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -4896,11 +4896,11 @@
       <c r="B16" t="s">
         <v>103</v>
       </c>
-      <c r="C16">
+      <c r="C16" t="s">
+        <v>120</v>
+      </c>
+      <c r="D16">
         <v>10.95</v>
-      </c>
-      <c r="D16" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -4910,11 +4910,11 @@
       <c r="B17" t="s">
         <v>104</v>
       </c>
-      <c r="C17">
+      <c r="C17" t="s">
+        <v>120</v>
+      </c>
+      <c r="D17">
         <v>18.8</v>
-      </c>
-      <c r="D17" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -4924,11 +4924,11 @@
       <c r="B18" t="s">
         <v>105</v>
       </c>
-      <c r="C18">
+      <c r="C18" t="s">
+        <v>120</v>
+      </c>
+      <c r="D18">
         <v>25.5</v>
-      </c>
-      <c r="D18" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -4938,11 +4938,11 @@
       <c r="B19" t="s">
         <v>106</v>
       </c>
-      <c r="C19">
+      <c r="C19" t="s">
+        <v>120</v>
+      </c>
+      <c r="D19">
         <v>19.46</v>
-      </c>
-      <c r="D19" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -4952,11 +4952,11 @@
       <c r="B20" t="s">
         <v>107</v>
       </c>
-      <c r="C20">
+      <c r="C20" t="s">
+        <v>120</v>
+      </c>
+      <c r="D20">
         <v>25.73</v>
-      </c>
-      <c r="D20" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -4966,11 +4966,11 @@
       <c r="B21" t="s">
         <v>108</v>
       </c>
-      <c r="C21">
+      <c r="C21" t="s">
+        <v>120</v>
+      </c>
+      <c r="D21">
         <v>11.89</v>
-      </c>
-      <c r="D21" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -4980,11 +4980,11 @@
       <c r="B22" t="s">
         <v>109</v>
       </c>
-      <c r="C22">
+      <c r="C22" t="s">
+        <v>120</v>
+      </c>
+      <c r="D22">
         <v>12.45</v>
-      </c>
-      <c r="D22" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -4994,11 +4994,11 @@
       <c r="B23" t="s">
         <v>110</v>
       </c>
-      <c r="C23">
+      <c r="C23" t="s">
+        <v>120</v>
+      </c>
+      <c r="D23">
         <v>12.66</v>
-      </c>
-      <c r="D23" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -5008,11 +5008,11 @@
       <c r="B24" t="s">
         <v>111</v>
       </c>
-      <c r="C24">
+      <c r="C24" t="s">
+        <v>120</v>
+      </c>
+      <c r="D24">
         <v>11.92</v>
-      </c>
-      <c r="D24" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -5022,11 +5022,11 @@
       <c r="B25" t="s">
         <v>112</v>
       </c>
-      <c r="C25">
+      <c r="C25" t="s">
+        <v>120</v>
+      </c>
+      <c r="D25">
         <v>14.46</v>
-      </c>
-      <c r="D25" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -5036,11 +5036,11 @@
       <c r="B26" t="s">
         <v>113</v>
       </c>
-      <c r="C26">
+      <c r="C26" t="s">
+        <v>120</v>
+      </c>
+      <c r="D26">
         <v>20.4</v>
-      </c>
-      <c r="D26" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -5050,11 +5050,11 @@
       <c r="B27" t="s">
         <v>114</v>
       </c>
-      <c r="C27">
+      <c r="C27" t="s">
+        <v>120</v>
+      </c>
+      <c r="D27">
         <v>14.71</v>
-      </c>
-      <c r="D27" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -5064,11 +5064,11 @@
       <c r="B28" t="s">
         <v>115</v>
       </c>
-      <c r="C28">
+      <c r="C28" t="s">
+        <v>120</v>
+      </c>
+      <c r="D28">
         <v>20.59</v>
-      </c>
-      <c r="D28" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -5078,11 +5078,11 @@
       <c r="B29" t="s">
         <v>116</v>
       </c>
-      <c r="C29">
+      <c r="C29" t="s">
+        <v>120</v>
+      </c>
+      <c r="D29">
         <v>9.460000000000001</v>
-      </c>
-      <c r="D29" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -5092,11 +5092,11 @@
       <c r="B30" t="s">
         <v>117</v>
       </c>
-      <c r="C30">
+      <c r="C30" t="s">
+        <v>120</v>
+      </c>
+      <c r="D30">
         <v>9.32</v>
-      </c>
-      <c r="D30" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -5106,11 +5106,11 @@
       <c r="B31" t="s">
         <v>118</v>
       </c>
-      <c r="C31">
+      <c r="C31" t="s">
+        <v>120</v>
+      </c>
+      <c r="D31">
         <v>9.44</v>
-      </c>
-      <c r="D31" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -5120,11 +5120,11 @@
       <c r="B32" t="s">
         <v>119</v>
       </c>
-      <c r="C32">
+      <c r="C32" t="s">
+        <v>120</v>
+      </c>
+      <c r="D32">
         <v>9.59</v>
-      </c>
-      <c r="D32" t="s">
-        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -5156,10 +5156,10 @@
         <v>55</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -5169,11 +5169,11 @@
       <c r="B2" t="s">
         <v>89</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D2">
         <v>11.2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -5183,11 +5183,11 @@
       <c r="B3" t="s">
         <v>90</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D3">
         <v>16.5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -5197,11 +5197,11 @@
       <c r="B4" t="s">
         <v>91</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4">
         <v>16.67</v>
-      </c>
-      <c r="D4" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -5211,11 +5211,11 @@
       <c r="B5" t="s">
         <v>92</v>
       </c>
-      <c r="C5">
+      <c r="C5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5">
         <v>5.57</v>
-      </c>
-      <c r="D5" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -5225,11 +5225,11 @@
       <c r="B6" t="s">
         <v>93</v>
       </c>
-      <c r="C6">
+      <c r="C6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D6">
         <v>5.74</v>
-      </c>
-      <c r="D6" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -5239,11 +5239,11 @@
       <c r="B7" t="s">
         <v>94</v>
       </c>
-      <c r="C7">
+      <c r="C7" t="s">
+        <v>120</v>
+      </c>
+      <c r="D7">
         <v>5.7</v>
-      </c>
-      <c r="D7" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -5253,11 +5253,11 @@
       <c r="B8" t="s">
         <v>95</v>
       </c>
-      <c r="C8">
+      <c r="C8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D8">
         <v>5.55</v>
-      </c>
-      <c r="D8" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -5267,11 +5267,11 @@
       <c r="B9" t="s">
         <v>96</v>
       </c>
-      <c r="C9">
+      <c r="C9" t="s">
+        <v>120</v>
+      </c>
+      <c r="D9">
         <v>17.85</v>
-      </c>
-      <c r="D9" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -5281,11 +5281,11 @@
       <c r="B10" t="s">
         <v>97</v>
       </c>
-      <c r="C10">
+      <c r="C10" t="s">
+        <v>120</v>
+      </c>
+      <c r="D10">
         <v>23.75</v>
-      </c>
-      <c r="D10" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -5295,11 +5295,11 @@
       <c r="B11" t="s">
         <v>98</v>
       </c>
-      <c r="C11">
+      <c r="C11" t="s">
+        <v>120</v>
+      </c>
+      <c r="D11">
         <v>18.57</v>
-      </c>
-      <c r="D11" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -5309,11 +5309,11 @@
       <c r="B12" t="s">
         <v>99</v>
       </c>
-      <c r="C12">
+      <c r="C12" t="s">
+        <v>120</v>
+      </c>
+      <c r="D12">
         <v>24</v>
-      </c>
-      <c r="D12" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -5323,11 +5323,11 @@
       <c r="B13" t="s">
         <v>100</v>
       </c>
-      <c r="C13">
+      <c r="C13" t="s">
+        <v>120</v>
+      </c>
+      <c r="D13">
         <v>10.9</v>
-      </c>
-      <c r="D13" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -5337,11 +5337,11 @@
       <c r="B14" t="s">
         <v>101</v>
       </c>
-      <c r="C14">
+      <c r="C14" t="s">
+        <v>120</v>
+      </c>
+      <c r="D14">
         <v>11.37</v>
-      </c>
-      <c r="D14" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -5351,11 +5351,11 @@
       <c r="B15" t="s">
         <v>102</v>
       </c>
-      <c r="C15">
+      <c r="C15" t="s">
+        <v>120</v>
+      </c>
+      <c r="D15">
         <v>11.4</v>
-      </c>
-      <c r="D15" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -5365,11 +5365,11 @@
       <c r="B16" t="s">
         <v>103</v>
       </c>
-      <c r="C16">
+      <c r="C16" t="s">
+        <v>120</v>
+      </c>
+      <c r="D16">
         <v>10.94</v>
-      </c>
-      <c r="D16" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -5379,11 +5379,11 @@
       <c r="B17" t="s">
         <v>104</v>
       </c>
-      <c r="C17">
+      <c r="C17" t="s">
+        <v>120</v>
+      </c>
+      <c r="D17">
         <v>18.81</v>
-      </c>
-      <c r="D17" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -5393,11 +5393,11 @@
       <c r="B18" t="s">
         <v>105</v>
       </c>
-      <c r="C18">
+      <c r="C18" t="s">
+        <v>120</v>
+      </c>
+      <c r="D18">
         <v>25.5</v>
-      </c>
-      <c r="D18" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -5407,11 +5407,11 @@
       <c r="B19" t="s">
         <v>106</v>
       </c>
-      <c r="C19">
+      <c r="C19" t="s">
+        <v>120</v>
+      </c>
+      <c r="D19">
         <v>19.49</v>
-      </c>
-      <c r="D19" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -5421,11 +5421,11 @@
       <c r="B20" t="s">
         <v>107</v>
       </c>
-      <c r="C20">
+      <c r="C20" t="s">
+        <v>120</v>
+      </c>
+      <c r="D20">
         <v>25.73</v>
-      </c>
-      <c r="D20" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -5435,11 +5435,11 @@
       <c r="B21" t="s">
         <v>108</v>
       </c>
-      <c r="C21">
+      <c r="C21" t="s">
+        <v>120</v>
+      </c>
+      <c r="D21">
         <v>11.89</v>
-      </c>
-      <c r="D21" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -5449,11 +5449,11 @@
       <c r="B22" t="s">
         <v>109</v>
       </c>
-      <c r="C22">
+      <c r="C22" t="s">
+        <v>120</v>
+      </c>
+      <c r="D22">
         <v>12.45</v>
-      </c>
-      <c r="D22" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -5463,11 +5463,11 @@
       <c r="B23" t="s">
         <v>110</v>
       </c>
-      <c r="C23">
+      <c r="C23" t="s">
+        <v>120</v>
+      </c>
+      <c r="D23">
         <v>12.68</v>
-      </c>
-      <c r="D23" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -5477,11 +5477,11 @@
       <c r="B24" t="s">
         <v>111</v>
       </c>
-      <c r="C24">
+      <c r="C24" t="s">
+        <v>120</v>
+      </c>
+      <c r="D24">
         <v>11.92</v>
-      </c>
-      <c r="D24" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -5491,11 +5491,11 @@
       <c r="B25" t="s">
         <v>112</v>
       </c>
-      <c r="C25">
+      <c r="C25" t="s">
+        <v>120</v>
+      </c>
+      <c r="D25">
         <v>14.47</v>
-      </c>
-      <c r="D25" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -5505,11 +5505,11 @@
       <c r="B26" t="s">
         <v>113</v>
       </c>
-      <c r="C26">
+      <c r="C26" t="s">
+        <v>120</v>
+      </c>
+      <c r="D26">
         <v>20.42</v>
-      </c>
-      <c r="D26" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -5519,11 +5519,11 @@
       <c r="B27" t="s">
         <v>114</v>
       </c>
-      <c r="C27">
+      <c r="C27" t="s">
+        <v>120</v>
+      </c>
+      <c r="D27">
         <v>14.7</v>
-      </c>
-      <c r="D27" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -5533,11 +5533,11 @@
       <c r="B28" t="s">
         <v>115</v>
       </c>
-      <c r="C28">
+      <c r="C28" t="s">
+        <v>120</v>
+      </c>
+      <c r="D28">
         <v>20.63</v>
-      </c>
-      <c r="D28" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -5547,11 +5547,11 @@
       <c r="B29" t="s">
         <v>116</v>
       </c>
-      <c r="C29">
+      <c r="C29" t="s">
+        <v>120</v>
+      </c>
+      <c r="D29">
         <v>9.460000000000001</v>
-      </c>
-      <c r="D29" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -5561,11 +5561,11 @@
       <c r="B30" t="s">
         <v>117</v>
       </c>
-      <c r="C30">
+      <c r="C30" t="s">
+        <v>120</v>
+      </c>
+      <c r="D30">
         <v>9.33</v>
-      </c>
-      <c r="D30" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -5575,11 +5575,11 @@
       <c r="B31" t="s">
         <v>118</v>
       </c>
-      <c r="C31">
+      <c r="C31" t="s">
+        <v>120</v>
+      </c>
+      <c r="D31">
         <v>9.44</v>
-      </c>
-      <c r="D31" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -5589,11 +5589,11 @@
       <c r="B32" t="s">
         <v>119</v>
       </c>
-      <c r="C32">
+      <c r="C32" t="s">
+        <v>120</v>
+      </c>
+      <c r="D32">
         <v>9.59</v>
-      </c>
-      <c r="D32" t="s">
-        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ran tests with updated IES scripts
</commit_message>
<xml_diff>
--- a/tests/testmodels/TestJob1/mf_results/tm59mechvent/TM59MechVent__TestJob1.xlsx
+++ b/tests/testmodels/TestJob1/mf_results/tm59mechvent/TM59MechVent__TestJob1.xlsx
@@ -27,18 +27,18 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1002" uniqueCount="121">
   <si>
+    <t>JobNo</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
     <t>sheet_name</t>
   </si>
   <si>
-    <t>JobNo</t>
-  </si>
-  <si>
     <t>Author</t>
   </si>
   <si>
-    <t>Date</t>
-  </si>
-  <si>
     <t>0</t>
   </si>
   <si>
@@ -72,6 +72,12 @@
     <t>10</t>
   </si>
   <si>
+    <t>/c/e</t>
+  </si>
+  <si>
+    <t>20220316</t>
+  </si>
+  <si>
     <t>Project Information</t>
   </si>
   <si>
@@ -105,15 +111,9 @@
     <t>Results, Air Speed 0.8</t>
   </si>
   <si>
-    <t>/c/e</t>
-  </si>
-  <si>
     <t>jovyan</t>
   </si>
   <si>
-    <t>20220309</t>
-  </si>
-  <si>
     <t>index</t>
   </si>
   <si>
@@ -177,7 +177,7 @@
     <t>51.38</t>
   </si>
   <si>
-    <t>2022-03-09 10:59:06.519565</t>
+    <t>2022-03-16 17:29:22.271374</t>
   </si>
   <si>
     <t>2021.4.0.0</t>
@@ -571,10 +571,10 @@
   <autoFilter ref="A1:E12"/>
   <tableColumns count="5">
     <tableColumn id="1" name="index"/>
-    <tableColumn id="2" name="sheet_name"/>
-    <tableColumn id="3" name="JobNo"/>
-    <tableColumn id="4" name="Author"/>
-    <tableColumn id="5" name="Date"/>
+    <tableColumn id="2" name="JobNo"/>
+    <tableColumn id="3" name="Date"/>
+    <tableColumn id="4" name="sheet_name"/>
+    <tableColumn id="5" name="Author"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -586,8 +586,8 @@
   <tableColumns count="4">
     <tableColumn id="1" name="Room ID"/>
     <tableColumn id="2" name="Room Name"/>
-    <tableColumn id="3" name="Fixed Temp Criterion (% Hours Operative Temp &gt; 26 Deg. Celsius)"/>
-    <tableColumn id="4" name="Fixed Temp Criterion (Pass/Fail)"/>
+    <tableColumn id="3" name="Fixed Temp Criterion (Pass/Fail)"/>
+    <tableColumn id="4" name="Fixed Temp Criterion (% Hours Operative Temp &gt; 26 Deg. Celsius)"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -599,8 +599,8 @@
   <tableColumns count="4">
     <tableColumn id="1" name="Room ID"/>
     <tableColumn id="2" name="Room Name"/>
-    <tableColumn id="3" name="Fixed Temp Criterion (% Hours Operative Temp &gt; 26 Deg. Celsius)"/>
-    <tableColumn id="4" name="Fixed Temp Criterion (Pass/Fail)"/>
+    <tableColumn id="3" name="Fixed Temp Criterion (Pass/Fail)"/>
+    <tableColumn id="4" name="Fixed Temp Criterion (% Hours Operative Temp &gt; 26 Deg. Celsius)"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -612,8 +612,8 @@
   <tableColumns count="4">
     <tableColumn id="1" name="Room ID"/>
     <tableColumn id="2" name="Room Name"/>
-    <tableColumn id="3" name="Fixed Temp Criterion (% Hours Operative Temp &gt; 26 Deg. Celsius)"/>
-    <tableColumn id="4" name="Fixed Temp Criterion (Pass/Fail)"/>
+    <tableColumn id="3" name="Fixed Temp Criterion (Pass/Fail)"/>
+    <tableColumn id="4" name="Fixed Temp Criterion (% Hours Operative Temp &gt; 26 Deg. Celsius)"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -647,8 +647,8 @@
   <tableColumns count="4">
     <tableColumn id="1" name="Room ID"/>
     <tableColumn id="2" name="Room Name"/>
-    <tableColumn id="3" name="Fixed Temp Criterion (% Hours Operative Temp &gt; 26 Deg. Celsius)"/>
-    <tableColumn id="4" name="Fixed Temp Criterion (Pass/Fail)"/>
+    <tableColumn id="3" name="Fixed Temp Criterion (Pass/Fail)"/>
+    <tableColumn id="4" name="Fixed Temp Criterion (% Hours Operative Temp &gt; 26 Deg. Celsius)"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -660,8 +660,8 @@
   <tableColumns count="4">
     <tableColumn id="1" name="Room ID"/>
     <tableColumn id="2" name="Room Name"/>
-    <tableColumn id="3" name="Fixed Temp Criterion (% Hours Operative Temp &gt; 26 Deg. Celsius)"/>
-    <tableColumn id="4" name="Fixed Temp Criterion (Pass/Fail)"/>
+    <tableColumn id="3" name="Fixed Temp Criterion (Pass/Fail)"/>
+    <tableColumn id="4" name="Fixed Temp Criterion (% Hours Operative Temp &gt; 26 Deg. Celsius)"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -673,8 +673,8 @@
   <tableColumns count="4">
     <tableColumn id="1" name="Room ID"/>
     <tableColumn id="2" name="Room Name"/>
-    <tableColumn id="3" name="Fixed Temp Criterion (% Hours Operative Temp &gt; 26 Deg. Celsius)"/>
-    <tableColumn id="4" name="Fixed Temp Criterion (Pass/Fail)"/>
+    <tableColumn id="3" name="Fixed Temp Criterion (Pass/Fail)"/>
+    <tableColumn id="4" name="Fixed Temp Criterion (% Hours Operative Temp &gt; 26 Deg. Celsius)"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -686,8 +686,8 @@
   <tableColumns count="4">
     <tableColumn id="1" name="Room ID"/>
     <tableColumn id="2" name="Room Name"/>
-    <tableColumn id="3" name="Fixed Temp Criterion (% Hours Operative Temp &gt; 26 Deg. Celsius)"/>
-    <tableColumn id="4" name="Fixed Temp Criterion (Pass/Fail)"/>
+    <tableColumn id="3" name="Fixed Temp Criterion (Pass/Fail)"/>
+    <tableColumn id="4" name="Fixed Temp Criterion (% Hours Operative Temp &gt; 26 Deg. Celsius)"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -699,8 +699,8 @@
   <tableColumns count="4">
     <tableColumn id="1" name="Room ID"/>
     <tableColumn id="2" name="Room Name"/>
-    <tableColumn id="3" name="Fixed Temp Criterion (% Hours Operative Temp &gt; 26 Deg. Celsius)"/>
-    <tableColumn id="4" name="Fixed Temp Criterion (Pass/Fail)"/>
+    <tableColumn id="3" name="Fixed Temp Criterion (Pass/Fail)"/>
+    <tableColumn id="4" name="Fixed Temp Criterion (% Hours Operative Temp &gt; 26 Deg. Celsius)"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -712,8 +712,8 @@
   <tableColumns count="4">
     <tableColumn id="1" name="Room ID"/>
     <tableColumn id="2" name="Room Name"/>
-    <tableColumn id="3" name="Fixed Temp Criterion (% Hours Operative Temp &gt; 26 Deg. Celsius)"/>
-    <tableColumn id="4" name="Fixed Temp Criterion (Pass/Fail)"/>
+    <tableColumn id="3" name="Fixed Temp Criterion (Pass/Fail)"/>
+    <tableColumn id="4" name="Fixed Temp Criterion (% Hours Operative Temp &gt; 26 Deg. Celsius)"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1044,10 +1044,10 @@
         <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>28</v>
@@ -1058,13 +1058,13 @@
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="D3" s="1" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>28</v>
@@ -1075,13 +1075,13 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>28</v>
@@ -1092,13 +1092,13 @@
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>28</v>
@@ -1109,13 +1109,13 @@
         <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>28</v>
@@ -1126,13 +1126,13 @@
         <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>28</v>
@@ -1143,13 +1143,13 @@
         <v>10</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>28</v>
@@ -1160,13 +1160,13 @@
         <v>11</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>28</v>
@@ -1177,13 +1177,13 @@
         <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>28</v>
@@ -1194,13 +1194,13 @@
         <v>13</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>28</v>
@@ -1211,10 +1211,10 @@
         <v>14</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>27</v>
@@ -1253,10 +1253,10 @@
         <v>55</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1266,11 +1266,11 @@
       <c r="B2" t="s">
         <v>89</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D2">
         <v>11.2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1280,11 +1280,11 @@
       <c r="B3" t="s">
         <v>90</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D3">
         <v>16.5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1294,11 +1294,11 @@
       <c r="B4" t="s">
         <v>91</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4">
         <v>16.67</v>
-      </c>
-      <c r="D4" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1308,11 +1308,11 @@
       <c r="B5" t="s">
         <v>92</v>
       </c>
-      <c r="C5">
+      <c r="C5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5">
         <v>5.58</v>
-      </c>
-      <c r="D5" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1322,11 +1322,11 @@
       <c r="B6" t="s">
         <v>93</v>
       </c>
-      <c r="C6">
+      <c r="C6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D6">
         <v>5.74</v>
-      </c>
-      <c r="D6" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1336,11 +1336,11 @@
       <c r="B7" t="s">
         <v>94</v>
       </c>
-      <c r="C7">
+      <c r="C7" t="s">
+        <v>120</v>
+      </c>
+      <c r="D7">
         <v>5.7</v>
-      </c>
-      <c r="D7" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1350,11 +1350,11 @@
       <c r="B8" t="s">
         <v>95</v>
       </c>
-      <c r="C8">
+      <c r="C8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D8">
         <v>5.55</v>
-      </c>
-      <c r="D8" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1364,11 +1364,11 @@
       <c r="B9" t="s">
         <v>96</v>
       </c>
-      <c r="C9">
+      <c r="C9" t="s">
+        <v>120</v>
+      </c>
+      <c r="D9">
         <v>17.87</v>
-      </c>
-      <c r="D9" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1378,11 +1378,11 @@
       <c r="B10" t="s">
         <v>97</v>
       </c>
-      <c r="C10">
+      <c r="C10" t="s">
+        <v>120</v>
+      </c>
+      <c r="D10">
         <v>23.75</v>
-      </c>
-      <c r="D10" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1392,11 +1392,11 @@
       <c r="B11" t="s">
         <v>98</v>
       </c>
-      <c r="C11">
+      <c r="C11" t="s">
+        <v>120</v>
+      </c>
+      <c r="D11">
         <v>18.57</v>
-      </c>
-      <c r="D11" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -1406,11 +1406,11 @@
       <c r="B12" t="s">
         <v>99</v>
       </c>
-      <c r="C12">
+      <c r="C12" t="s">
+        <v>120</v>
+      </c>
+      <c r="D12">
         <v>24.03</v>
-      </c>
-      <c r="D12" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1420,11 +1420,11 @@
       <c r="B13" t="s">
         <v>100</v>
       </c>
-      <c r="C13">
+      <c r="C13" t="s">
+        <v>120</v>
+      </c>
+      <c r="D13">
         <v>10.9</v>
-      </c>
-      <c r="D13" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1434,11 +1434,11 @@
       <c r="B14" t="s">
         <v>101</v>
       </c>
-      <c r="C14">
+      <c r="C14" t="s">
+        <v>120</v>
+      </c>
+      <c r="D14">
         <v>11.37</v>
-      </c>
-      <c r="D14" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -1448,11 +1448,11 @@
       <c r="B15" t="s">
         <v>102</v>
       </c>
-      <c r="C15">
+      <c r="C15" t="s">
+        <v>120</v>
+      </c>
+      <c r="D15">
         <v>11.4</v>
-      </c>
-      <c r="D15" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1462,11 +1462,11 @@
       <c r="B16" t="s">
         <v>103</v>
       </c>
-      <c r="C16">
+      <c r="C16" t="s">
+        <v>120</v>
+      </c>
+      <c r="D16">
         <v>10.94</v>
-      </c>
-      <c r="D16" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1476,11 +1476,11 @@
       <c r="B17" t="s">
         <v>104</v>
       </c>
-      <c r="C17">
+      <c r="C17" t="s">
+        <v>120</v>
+      </c>
+      <c r="D17">
         <v>18.81</v>
-      </c>
-      <c r="D17" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1490,11 +1490,11 @@
       <c r="B18" t="s">
         <v>105</v>
       </c>
-      <c r="C18">
+      <c r="C18" t="s">
+        <v>120</v>
+      </c>
+      <c r="D18">
         <v>25.52</v>
-      </c>
-      <c r="D18" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1504,11 +1504,11 @@
       <c r="B19" t="s">
         <v>106</v>
       </c>
-      <c r="C19">
+      <c r="C19" t="s">
+        <v>120</v>
+      </c>
+      <c r="D19">
         <v>19.47</v>
-      </c>
-      <c r="D19" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1518,11 +1518,11 @@
       <c r="B20" t="s">
         <v>107</v>
       </c>
-      <c r="C20">
+      <c r="C20" t="s">
+        <v>120</v>
+      </c>
+      <c r="D20">
         <v>25.73</v>
-      </c>
-      <c r="D20" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -1532,11 +1532,11 @@
       <c r="B21" t="s">
         <v>108</v>
       </c>
-      <c r="C21">
+      <c r="C21" t="s">
+        <v>120</v>
+      </c>
+      <c r="D21">
         <v>11.88</v>
-      </c>
-      <c r="D21" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -1546,11 +1546,11 @@
       <c r="B22" t="s">
         <v>109</v>
       </c>
-      <c r="C22">
+      <c r="C22" t="s">
+        <v>120</v>
+      </c>
+      <c r="D22">
         <v>12.45</v>
-      </c>
-      <c r="D22" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1560,11 +1560,11 @@
       <c r="B23" t="s">
         <v>110</v>
       </c>
-      <c r="C23">
+      <c r="C23" t="s">
+        <v>120</v>
+      </c>
+      <c r="D23">
         <v>12.67</v>
-      </c>
-      <c r="D23" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1574,11 +1574,11 @@
       <c r="B24" t="s">
         <v>111</v>
       </c>
-      <c r="C24">
+      <c r="C24" t="s">
+        <v>120</v>
+      </c>
+      <c r="D24">
         <v>11.91</v>
-      </c>
-      <c r="D24" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1588,11 +1588,11 @@
       <c r="B25" t="s">
         <v>112</v>
       </c>
-      <c r="C25">
+      <c r="C25" t="s">
+        <v>120</v>
+      </c>
+      <c r="D25">
         <v>14.46</v>
-      </c>
-      <c r="D25" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1602,11 +1602,11 @@
       <c r="B26" t="s">
         <v>113</v>
       </c>
-      <c r="C26">
+      <c r="C26" t="s">
+        <v>120</v>
+      </c>
+      <c r="D26">
         <v>20.44</v>
-      </c>
-      <c r="D26" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1616,11 +1616,11 @@
       <c r="B27" t="s">
         <v>114</v>
       </c>
-      <c r="C27">
+      <c r="C27" t="s">
+        <v>120</v>
+      </c>
+      <c r="D27">
         <v>14.7</v>
-      </c>
-      <c r="D27" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1630,11 +1630,11 @@
       <c r="B28" t="s">
         <v>115</v>
       </c>
-      <c r="C28">
+      <c r="C28" t="s">
+        <v>120</v>
+      </c>
+      <c r="D28">
         <v>20.65</v>
-      </c>
-      <c r="D28" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1644,11 +1644,11 @@
       <c r="B29" t="s">
         <v>116</v>
       </c>
-      <c r="C29">
+      <c r="C29" t="s">
+        <v>120</v>
+      </c>
+      <c r="D29">
         <v>9.470000000000001</v>
-      </c>
-      <c r="D29" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1658,11 +1658,11 @@
       <c r="B30" t="s">
         <v>117</v>
       </c>
-      <c r="C30">
+      <c r="C30" t="s">
+        <v>120</v>
+      </c>
+      <c r="D30">
         <v>9.32</v>
-      </c>
-      <c r="D30" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1672,11 +1672,11 @@
       <c r="B31" t="s">
         <v>118</v>
       </c>
-      <c r="C31">
+      <c r="C31" t="s">
+        <v>120</v>
+      </c>
+      <c r="D31">
         <v>9.44</v>
-      </c>
-      <c r="D31" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1686,11 +1686,11 @@
       <c r="B32" t="s">
         <v>119</v>
       </c>
-      <c r="C32">
+      <c r="C32" t="s">
+        <v>120</v>
+      </c>
+      <c r="D32">
         <v>9.59</v>
-      </c>
-      <c r="D32" t="s">
-        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -1722,10 +1722,10 @@
         <v>55</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1735,11 +1735,11 @@
       <c r="B2" t="s">
         <v>89</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D2">
         <v>11.2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1749,11 +1749,11 @@
       <c r="B3" t="s">
         <v>90</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D3">
         <v>16.52</v>
-      </c>
-      <c r="D3" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1763,11 +1763,11 @@
       <c r="B4" t="s">
         <v>91</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4">
         <v>16.67</v>
-      </c>
-      <c r="D4" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1777,11 +1777,11 @@
       <c r="B5" t="s">
         <v>92</v>
       </c>
-      <c r="C5">
+      <c r="C5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5">
         <v>5.58</v>
-      </c>
-      <c r="D5" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1791,11 +1791,11 @@
       <c r="B6" t="s">
         <v>93</v>
       </c>
-      <c r="C6">
+      <c r="C6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D6">
         <v>5.73</v>
-      </c>
-      <c r="D6" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1805,11 +1805,11 @@
       <c r="B7" t="s">
         <v>94</v>
       </c>
-      <c r="C7">
+      <c r="C7" t="s">
+        <v>120</v>
+      </c>
+      <c r="D7">
         <v>5.7</v>
-      </c>
-      <c r="D7" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1819,11 +1819,11 @@
       <c r="B8" t="s">
         <v>95</v>
       </c>
-      <c r="C8">
+      <c r="C8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D8">
         <v>5.55</v>
-      </c>
-      <c r="D8" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1833,11 +1833,11 @@
       <c r="B9" t="s">
         <v>96</v>
       </c>
-      <c r="C9">
+      <c r="C9" t="s">
+        <v>120</v>
+      </c>
+      <c r="D9">
         <v>17.87</v>
-      </c>
-      <c r="D9" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1847,11 +1847,11 @@
       <c r="B10" t="s">
         <v>97</v>
       </c>
-      <c r="C10">
+      <c r="C10" t="s">
+        <v>120</v>
+      </c>
+      <c r="D10">
         <v>23.75</v>
-      </c>
-      <c r="D10" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1861,11 +1861,11 @@
       <c r="B11" t="s">
         <v>98</v>
       </c>
-      <c r="C11">
+      <c r="C11" t="s">
+        <v>120</v>
+      </c>
+      <c r="D11">
         <v>18.57</v>
-      </c>
-      <c r="D11" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -1875,11 +1875,11 @@
       <c r="B12" t="s">
         <v>99</v>
       </c>
-      <c r="C12">
+      <c r="C12" t="s">
+        <v>120</v>
+      </c>
+      <c r="D12">
         <v>24.03</v>
-      </c>
-      <c r="D12" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1889,11 +1889,11 @@
       <c r="B13" t="s">
         <v>100</v>
       </c>
-      <c r="C13">
+      <c r="C13" t="s">
+        <v>120</v>
+      </c>
+      <c r="D13">
         <v>10.9</v>
-      </c>
-      <c r="D13" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1903,11 +1903,11 @@
       <c r="B14" t="s">
         <v>101</v>
       </c>
-      <c r="C14">
+      <c r="C14" t="s">
+        <v>120</v>
+      </c>
+      <c r="D14">
         <v>11.37</v>
-      </c>
-      <c r="D14" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -1917,11 +1917,11 @@
       <c r="B15" t="s">
         <v>102</v>
       </c>
-      <c r="C15">
+      <c r="C15" t="s">
+        <v>120</v>
+      </c>
+      <c r="D15">
         <v>11.4</v>
-      </c>
-      <c r="D15" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1931,11 +1931,11 @@
       <c r="B16" t="s">
         <v>103</v>
       </c>
-      <c r="C16">
+      <c r="C16" t="s">
+        <v>120</v>
+      </c>
+      <c r="D16">
         <v>10.92</v>
-      </c>
-      <c r="D16" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1945,11 +1945,11 @@
       <c r="B17" t="s">
         <v>104</v>
       </c>
-      <c r="C17">
+      <c r="C17" t="s">
+        <v>120</v>
+      </c>
+      <c r="D17">
         <v>18.81</v>
-      </c>
-      <c r="D17" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1959,11 +1959,11 @@
       <c r="B18" t="s">
         <v>105</v>
       </c>
-      <c r="C18">
+      <c r="C18" t="s">
+        <v>120</v>
+      </c>
+      <c r="D18">
         <v>25.54</v>
-      </c>
-      <c r="D18" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1973,11 +1973,11 @@
       <c r="B19" t="s">
         <v>106</v>
       </c>
-      <c r="C19">
+      <c r="C19" t="s">
+        <v>120</v>
+      </c>
+      <c r="D19">
         <v>19.47</v>
-      </c>
-      <c r="D19" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1987,11 +1987,11 @@
       <c r="B20" t="s">
         <v>107</v>
       </c>
-      <c r="C20">
+      <c r="C20" t="s">
+        <v>120</v>
+      </c>
+      <c r="D20">
         <v>25.75</v>
-      </c>
-      <c r="D20" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -2001,11 +2001,11 @@
       <c r="B21" t="s">
         <v>108</v>
       </c>
-      <c r="C21">
+      <c r="C21" t="s">
+        <v>120</v>
+      </c>
+      <c r="D21">
         <v>11.87</v>
-      </c>
-      <c r="D21" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -2015,11 +2015,11 @@
       <c r="B22" t="s">
         <v>109</v>
       </c>
-      <c r="C22">
+      <c r="C22" t="s">
+        <v>120</v>
+      </c>
+      <c r="D22">
         <v>12.45</v>
-      </c>
-      <c r="D22" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -2029,11 +2029,11 @@
       <c r="B23" t="s">
         <v>110</v>
       </c>
-      <c r="C23">
+      <c r="C23" t="s">
+        <v>120</v>
+      </c>
+      <c r="D23">
         <v>12.67</v>
-      </c>
-      <c r="D23" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -2043,11 +2043,11 @@
       <c r="B24" t="s">
         <v>111</v>
       </c>
-      <c r="C24">
+      <c r="C24" t="s">
+        <v>120</v>
+      </c>
+      <c r="D24">
         <v>11.91</v>
-      </c>
-      <c r="D24" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -2057,11 +2057,11 @@
       <c r="B25" t="s">
         <v>112</v>
       </c>
-      <c r="C25">
+      <c r="C25" t="s">
+        <v>120</v>
+      </c>
+      <c r="D25">
         <v>14.45</v>
-      </c>
-      <c r="D25" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -2071,11 +2071,11 @@
       <c r="B26" t="s">
         <v>113</v>
       </c>
-      <c r="C26">
+      <c r="C26" t="s">
+        <v>120</v>
+      </c>
+      <c r="D26">
         <v>20.48</v>
-      </c>
-      <c r="D26" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -2085,11 +2085,11 @@
       <c r="B27" t="s">
         <v>114</v>
       </c>
-      <c r="C27">
+      <c r="C27" t="s">
+        <v>120</v>
+      </c>
+      <c r="D27">
         <v>14.7</v>
-      </c>
-      <c r="D27" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -2099,11 +2099,11 @@
       <c r="B28" t="s">
         <v>115</v>
       </c>
-      <c r="C28">
+      <c r="C28" t="s">
+        <v>120</v>
+      </c>
+      <c r="D28">
         <v>20.67</v>
-      </c>
-      <c r="D28" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -2113,11 +2113,11 @@
       <c r="B29" t="s">
         <v>116</v>
       </c>
-      <c r="C29">
+      <c r="C29" t="s">
+        <v>120</v>
+      </c>
+      <c r="D29">
         <v>9.470000000000001</v>
-      </c>
-      <c r="D29" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -2127,11 +2127,11 @@
       <c r="B30" t="s">
         <v>117</v>
       </c>
-      <c r="C30">
+      <c r="C30" t="s">
+        <v>120</v>
+      </c>
+      <c r="D30">
         <v>9.32</v>
-      </c>
-      <c r="D30" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -2141,11 +2141,11 @@
       <c r="B31" t="s">
         <v>118</v>
       </c>
-      <c r="C31">
+      <c r="C31" t="s">
+        <v>120</v>
+      </c>
+      <c r="D31">
         <v>9.44</v>
-      </c>
-      <c r="D31" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -2155,11 +2155,11 @@
       <c r="B32" t="s">
         <v>119</v>
       </c>
-      <c r="C32">
+      <c r="C32" t="s">
+        <v>120</v>
+      </c>
+      <c r="D32">
         <v>9.59</v>
-      </c>
-      <c r="D32" t="s">
-        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -2191,10 +2191,10 @@
         <v>55</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -2204,11 +2204,11 @@
       <c r="B2" t="s">
         <v>89</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D2">
         <v>11.2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -2218,11 +2218,11 @@
       <c r="B3" t="s">
         <v>90</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D3">
         <v>16.52</v>
-      </c>
-      <c r="D3" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -2232,11 +2232,11 @@
       <c r="B4" t="s">
         <v>91</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4">
         <v>16.67</v>
-      </c>
-      <c r="D4" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -2246,11 +2246,11 @@
       <c r="B5" t="s">
         <v>92</v>
       </c>
-      <c r="C5">
+      <c r="C5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5">
         <v>5.58</v>
-      </c>
-      <c r="D5" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -2260,11 +2260,11 @@
       <c r="B6" t="s">
         <v>93</v>
       </c>
-      <c r="C6">
+      <c r="C6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D6">
         <v>5.73</v>
-      </c>
-      <c r="D6" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -2274,11 +2274,11 @@
       <c r="B7" t="s">
         <v>94</v>
       </c>
-      <c r="C7">
+      <c r="C7" t="s">
+        <v>120</v>
+      </c>
+      <c r="D7">
         <v>5.7</v>
-      </c>
-      <c r="D7" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -2288,11 +2288,11 @@
       <c r="B8" t="s">
         <v>95</v>
       </c>
-      <c r="C8">
+      <c r="C8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D8">
         <v>5.54</v>
-      </c>
-      <c r="D8" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -2302,11 +2302,11 @@
       <c r="B9" t="s">
         <v>96</v>
       </c>
-      <c r="C9">
+      <c r="C9" t="s">
+        <v>120</v>
+      </c>
+      <c r="D9">
         <v>17.87</v>
-      </c>
-      <c r="D9" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -2316,11 +2316,11 @@
       <c r="B10" t="s">
         <v>97</v>
       </c>
-      <c r="C10">
+      <c r="C10" t="s">
+        <v>120</v>
+      </c>
+      <c r="D10">
         <v>23.77</v>
-      </c>
-      <c r="D10" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -2330,11 +2330,11 @@
       <c r="B11" t="s">
         <v>98</v>
       </c>
-      <c r="C11">
+      <c r="C11" t="s">
+        <v>120</v>
+      </c>
+      <c r="D11">
         <v>18.57</v>
-      </c>
-      <c r="D11" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -2344,11 +2344,11 @@
       <c r="B12" t="s">
         <v>99</v>
       </c>
-      <c r="C12">
+      <c r="C12" t="s">
+        <v>120</v>
+      </c>
+      <c r="D12">
         <v>24.03</v>
-      </c>
-      <c r="D12" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -2358,11 +2358,11 @@
       <c r="B13" t="s">
         <v>100</v>
       </c>
-      <c r="C13">
+      <c r="C13" t="s">
+        <v>120</v>
+      </c>
+      <c r="D13">
         <v>10.89</v>
-      </c>
-      <c r="D13" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -2372,11 +2372,11 @@
       <c r="B14" t="s">
         <v>101</v>
       </c>
-      <c r="C14">
+      <c r="C14" t="s">
+        <v>120</v>
+      </c>
+      <c r="D14">
         <v>11.37</v>
-      </c>
-      <c r="D14" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -2386,11 +2386,11 @@
       <c r="B15" t="s">
         <v>102</v>
       </c>
-      <c r="C15">
+      <c r="C15" t="s">
+        <v>120</v>
+      </c>
+      <c r="D15">
         <v>11.4</v>
-      </c>
-      <c r="D15" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -2400,11 +2400,11 @@
       <c r="B16" t="s">
         <v>103</v>
       </c>
-      <c r="C16">
+      <c r="C16" t="s">
+        <v>120</v>
+      </c>
+      <c r="D16">
         <v>10.92</v>
-      </c>
-      <c r="D16" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -2414,11 +2414,11 @@
       <c r="B17" t="s">
         <v>104</v>
       </c>
-      <c r="C17">
+      <c r="C17" t="s">
+        <v>120</v>
+      </c>
+      <c r="D17">
         <v>18.81</v>
-      </c>
-      <c r="D17" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -2428,11 +2428,11 @@
       <c r="B18" t="s">
         <v>105</v>
       </c>
-      <c r="C18">
+      <c r="C18" t="s">
+        <v>120</v>
+      </c>
+      <c r="D18">
         <v>25.54</v>
-      </c>
-      <c r="D18" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -2442,11 +2442,11 @@
       <c r="B19" t="s">
         <v>106</v>
       </c>
-      <c r="C19">
+      <c r="C19" t="s">
+        <v>120</v>
+      </c>
+      <c r="D19">
         <v>19.47</v>
-      </c>
-      <c r="D19" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -2456,11 +2456,11 @@
       <c r="B20" t="s">
         <v>107</v>
       </c>
-      <c r="C20">
+      <c r="C20" t="s">
+        <v>120</v>
+      </c>
+      <c r="D20">
         <v>25.75</v>
-      </c>
-      <c r="D20" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -2470,11 +2470,11 @@
       <c r="B21" t="s">
         <v>108</v>
       </c>
-      <c r="C21">
+      <c r="C21" t="s">
+        <v>120</v>
+      </c>
+      <c r="D21">
         <v>11.87</v>
-      </c>
-      <c r="D21" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -2484,11 +2484,11 @@
       <c r="B22" t="s">
         <v>109</v>
       </c>
-      <c r="C22">
+      <c r="C22" t="s">
+        <v>120</v>
+      </c>
+      <c r="D22">
         <v>12.47</v>
-      </c>
-      <c r="D22" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -2498,11 +2498,11 @@
       <c r="B23" t="s">
         <v>110</v>
       </c>
-      <c r="C23">
+      <c r="C23" t="s">
+        <v>120</v>
+      </c>
+      <c r="D23">
         <v>12.67</v>
-      </c>
-      <c r="D23" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -2512,11 +2512,11 @@
       <c r="B24" t="s">
         <v>111</v>
       </c>
-      <c r="C24">
+      <c r="C24" t="s">
+        <v>120</v>
+      </c>
+      <c r="D24">
         <v>11.91</v>
-      </c>
-      <c r="D24" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -2526,11 +2526,11 @@
       <c r="B25" t="s">
         <v>112</v>
       </c>
-      <c r="C25">
+      <c r="C25" t="s">
+        <v>120</v>
+      </c>
+      <c r="D25">
         <v>14.45</v>
-      </c>
-      <c r="D25" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -2540,11 +2540,11 @@
       <c r="B26" t="s">
         <v>113</v>
       </c>
-      <c r="C26">
+      <c r="C26" t="s">
+        <v>120</v>
+      </c>
+      <c r="D26">
         <v>20.48</v>
-      </c>
-      <c r="D26" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -2554,11 +2554,11 @@
       <c r="B27" t="s">
         <v>114</v>
       </c>
-      <c r="C27">
+      <c r="C27" t="s">
+        <v>120</v>
+      </c>
+      <c r="D27">
         <v>14.7</v>
-      </c>
-      <c r="D27" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -2568,11 +2568,11 @@
       <c r="B28" t="s">
         <v>115</v>
       </c>
-      <c r="C28">
+      <c r="C28" t="s">
+        <v>120</v>
+      </c>
+      <c r="D28">
         <v>20.67</v>
-      </c>
-      <c r="D28" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -2582,11 +2582,11 @@
       <c r="B29" t="s">
         <v>116</v>
       </c>
-      <c r="C29">
+      <c r="C29" t="s">
+        <v>120</v>
+      </c>
+      <c r="D29">
         <v>9.470000000000001</v>
-      </c>
-      <c r="D29" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -2596,11 +2596,11 @@
       <c r="B30" t="s">
         <v>117</v>
       </c>
-      <c r="C30">
+      <c r="C30" t="s">
+        <v>120</v>
+      </c>
+      <c r="D30">
         <v>9.32</v>
-      </c>
-      <c r="D30" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -2610,11 +2610,11 @@
       <c r="B31" t="s">
         <v>118</v>
       </c>
-      <c r="C31">
+      <c r="C31" t="s">
+        <v>120</v>
+      </c>
+      <c r="D31">
         <v>9.44</v>
-      </c>
-      <c r="D31" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -2624,11 +2624,11 @@
       <c r="B32" t="s">
         <v>119</v>
       </c>
-      <c r="C32">
+      <c r="C32" t="s">
+        <v>120</v>
+      </c>
+      <c r="D32">
         <v>9.59</v>
-      </c>
-      <c r="D32" t="s">
-        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -2811,10 +2811,10 @@
         <v>55</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -2824,11 +2824,11 @@
       <c r="B2" t="s">
         <v>89</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D2">
         <v>11.21</v>
-      </c>
-      <c r="D2" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -2838,11 +2838,11 @@
       <c r="B3" t="s">
         <v>90</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D3">
         <v>16.33</v>
-      </c>
-      <c r="D3" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -2852,11 +2852,11 @@
       <c r="B4" t="s">
         <v>91</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4">
         <v>16.52</v>
-      </c>
-      <c r="D4" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -2866,11 +2866,11 @@
       <c r="B5" t="s">
         <v>92</v>
       </c>
-      <c r="C5">
+      <c r="C5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5">
         <v>5.57</v>
-      </c>
-      <c r="D5" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -2880,11 +2880,11 @@
       <c r="B6" t="s">
         <v>93</v>
       </c>
-      <c r="C6">
+      <c r="C6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D6">
         <v>5.76</v>
-      </c>
-      <c r="D6" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -2894,11 +2894,11 @@
       <c r="B7" t="s">
         <v>94</v>
       </c>
-      <c r="C7">
+      <c r="C7" t="s">
+        <v>120</v>
+      </c>
+      <c r="D7">
         <v>5.65</v>
-      </c>
-      <c r="D7" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -2908,11 +2908,11 @@
       <c r="B8" t="s">
         <v>95</v>
       </c>
-      <c r="C8">
+      <c r="C8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D8">
         <v>5.56</v>
-      </c>
-      <c r="D8" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -2922,11 +2922,11 @@
       <c r="B9" t="s">
         <v>96</v>
       </c>
-      <c r="C9">
+      <c r="C9" t="s">
+        <v>120</v>
+      </c>
+      <c r="D9">
         <v>17.87</v>
-      </c>
-      <c r="D9" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -2936,11 +2936,11 @@
       <c r="B10" t="s">
         <v>97</v>
       </c>
-      <c r="C10">
+      <c r="C10" t="s">
+        <v>120</v>
+      </c>
+      <c r="D10">
         <v>23.69</v>
-      </c>
-      <c r="D10" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -2950,11 +2950,11 @@
       <c r="B11" t="s">
         <v>98</v>
       </c>
-      <c r="C11">
+      <c r="C11" t="s">
+        <v>120</v>
+      </c>
+      <c r="D11">
         <v>18.61</v>
-      </c>
-      <c r="D11" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -2964,11 +2964,11 @@
       <c r="B12" t="s">
         <v>99</v>
       </c>
-      <c r="C12">
+      <c r="C12" t="s">
+        <v>120</v>
+      </c>
+      <c r="D12">
         <v>23.88</v>
-      </c>
-      <c r="D12" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -2978,11 +2978,11 @@
       <c r="B13" t="s">
         <v>100</v>
       </c>
-      <c r="C13">
+      <c r="C13" t="s">
+        <v>120</v>
+      </c>
+      <c r="D13">
         <v>10.95</v>
-      </c>
-      <c r="D13" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -2992,11 +2992,11 @@
       <c r="B14" t="s">
         <v>101</v>
       </c>
-      <c r="C14">
+      <c r="C14" t="s">
+        <v>120</v>
+      </c>
+      <c r="D14">
         <v>11.38</v>
-      </c>
-      <c r="D14" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -3006,11 +3006,11 @@
       <c r="B15" t="s">
         <v>102</v>
       </c>
-      <c r="C15">
+      <c r="C15" t="s">
+        <v>120</v>
+      </c>
+      <c r="D15">
         <v>11.39</v>
-      </c>
-      <c r="D15" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -3020,11 +3020,11 @@
       <c r="B16" t="s">
         <v>103</v>
       </c>
-      <c r="C16">
+      <c r="C16" t="s">
+        <v>120</v>
+      </c>
+      <c r="D16">
         <v>10.94</v>
-      </c>
-      <c r="D16" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -3034,11 +3034,11 @@
       <c r="B17" t="s">
         <v>104</v>
       </c>
-      <c r="C17">
+      <c r="C17" t="s">
+        <v>120</v>
+      </c>
+      <c r="D17">
         <v>18.82</v>
-      </c>
-      <c r="D17" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -3048,11 +3048,11 @@
       <c r="B18" t="s">
         <v>105</v>
       </c>
-      <c r="C18">
+      <c r="C18" t="s">
+        <v>120</v>
+      </c>
+      <c r="D18">
         <v>25.37</v>
-      </c>
-      <c r="D18" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -3062,11 +3062,11 @@
       <c r="B19" t="s">
         <v>106</v>
       </c>
-      <c r="C19">
+      <c r="C19" t="s">
+        <v>120</v>
+      </c>
+      <c r="D19">
         <v>19.5</v>
-      </c>
-      <c r="D19" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -3076,11 +3076,11 @@
       <c r="B20" t="s">
         <v>107</v>
       </c>
-      <c r="C20">
+      <c r="C20" t="s">
+        <v>120</v>
+      </c>
+      <c r="D20">
         <v>25.58</v>
-      </c>
-      <c r="D20" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -3090,11 +3090,11 @@
       <c r="B21" t="s">
         <v>108</v>
       </c>
-      <c r="C21">
+      <c r="C21" t="s">
+        <v>120</v>
+      </c>
+      <c r="D21">
         <v>11.91</v>
-      </c>
-      <c r="D21" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -3104,11 +3104,11 @@
       <c r="B22" t="s">
         <v>109</v>
       </c>
-      <c r="C22">
+      <c r="C22" t="s">
+        <v>120</v>
+      </c>
+      <c r="D22">
         <v>12.49</v>
-      </c>
-      <c r="D22" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -3118,11 +3118,11 @@
       <c r="B23" t="s">
         <v>110</v>
       </c>
-      <c r="C23">
+      <c r="C23" t="s">
+        <v>120</v>
+      </c>
+      <c r="D23">
         <v>12.67</v>
-      </c>
-      <c r="D23" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -3132,11 +3132,11 @@
       <c r="B24" t="s">
         <v>111</v>
       </c>
-      <c r="C24">
+      <c r="C24" t="s">
+        <v>120</v>
+      </c>
+      <c r="D24">
         <v>11.93</v>
-      </c>
-      <c r="D24" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -3146,11 +3146,11 @@
       <c r="B25" t="s">
         <v>112</v>
       </c>
-      <c r="C25">
+      <c r="C25" t="s">
+        <v>120</v>
+      </c>
+      <c r="D25">
         <v>14.45</v>
-      </c>
-      <c r="D25" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -3160,11 +3160,11 @@
       <c r="B26" t="s">
         <v>113</v>
       </c>
-      <c r="C26">
+      <c r="C26" t="s">
+        <v>120</v>
+      </c>
+      <c r="D26">
         <v>20.3</v>
-      </c>
-      <c r="D26" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -3174,11 +3174,11 @@
       <c r="B27" t="s">
         <v>114</v>
       </c>
-      <c r="C27">
+      <c r="C27" t="s">
+        <v>120</v>
+      </c>
+      <c r="D27">
         <v>14.67</v>
-      </c>
-      <c r="D27" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -3188,11 +3188,11 @@
       <c r="B28" t="s">
         <v>115</v>
       </c>
-      <c r="C28">
+      <c r="C28" t="s">
+        <v>120</v>
+      </c>
+      <c r="D28">
         <v>20.42</v>
-      </c>
-      <c r="D28" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -3202,11 +3202,11 @@
       <c r="B29" t="s">
         <v>116</v>
       </c>
-      <c r="C29">
+      <c r="C29" t="s">
+        <v>120</v>
+      </c>
+      <c r="D29">
         <v>9.470000000000001</v>
-      </c>
-      <c r="D29" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -3216,11 +3216,11 @@
       <c r="B30" t="s">
         <v>117</v>
       </c>
-      <c r="C30">
+      <c r="C30" t="s">
+        <v>120</v>
+      </c>
+      <c r="D30">
         <v>9.33</v>
-      </c>
-      <c r="D30" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -3230,11 +3230,11 @@
       <c r="B31" t="s">
         <v>118</v>
       </c>
-      <c r="C31">
+      <c r="C31" t="s">
+        <v>120</v>
+      </c>
+      <c r="D31">
         <v>9.460000000000001</v>
-      </c>
-      <c r="D31" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -3244,11 +3244,11 @@
       <c r="B32" t="s">
         <v>119</v>
       </c>
-      <c r="C32">
+      <c r="C32" t="s">
+        <v>120</v>
+      </c>
+      <c r="D32">
         <v>9.58</v>
-      </c>
-      <c r="D32" t="s">
-        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -3280,10 +3280,10 @@
         <v>55</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -3293,11 +3293,11 @@
       <c r="B2" t="s">
         <v>89</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D2">
         <v>11.21</v>
-      </c>
-      <c r="D2" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -3307,11 +3307,11 @@
       <c r="B3" t="s">
         <v>90</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D3">
         <v>16.33</v>
-      </c>
-      <c r="D3" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -3321,11 +3321,11 @@
       <c r="B4" t="s">
         <v>91</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4">
         <v>16.56</v>
-      </c>
-      <c r="D4" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -3335,11 +3335,11 @@
       <c r="B5" t="s">
         <v>92</v>
       </c>
-      <c r="C5">
+      <c r="C5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5">
         <v>5.57</v>
-      </c>
-      <c r="D5" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -3349,11 +3349,11 @@
       <c r="B6" t="s">
         <v>93</v>
       </c>
-      <c r="C6">
+      <c r="C6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D6">
         <v>5.76</v>
-      </c>
-      <c r="D6" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -3363,11 +3363,11 @@
       <c r="B7" t="s">
         <v>94</v>
       </c>
-      <c r="C7">
+      <c r="C7" t="s">
+        <v>120</v>
+      </c>
+      <c r="D7">
         <v>5.66</v>
-      </c>
-      <c r="D7" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -3377,11 +3377,11 @@
       <c r="B8" t="s">
         <v>95</v>
       </c>
-      <c r="C8">
+      <c r="C8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D8">
         <v>5.57</v>
-      </c>
-      <c r="D8" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -3391,11 +3391,11 @@
       <c r="B9" t="s">
         <v>96</v>
       </c>
-      <c r="C9">
+      <c r="C9" t="s">
+        <v>120</v>
+      </c>
+      <c r="D9">
         <v>17.87</v>
-      </c>
-      <c r="D9" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -3405,11 +3405,11 @@
       <c r="B10" t="s">
         <v>97</v>
       </c>
-      <c r="C10">
+      <c r="C10" t="s">
+        <v>120</v>
+      </c>
+      <c r="D10">
         <v>23.73</v>
-      </c>
-      <c r="D10" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -3419,11 +3419,11 @@
       <c r="B11" t="s">
         <v>98</v>
       </c>
-      <c r="C11">
+      <c r="C11" t="s">
+        <v>120</v>
+      </c>
+      <c r="D11">
         <v>18.6</v>
-      </c>
-      <c r="D11" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -3433,11 +3433,11 @@
       <c r="B12" t="s">
         <v>99</v>
       </c>
-      <c r="C12">
+      <c r="C12" t="s">
+        <v>120</v>
+      </c>
+      <c r="D12">
         <v>23.9</v>
-      </c>
-      <c r="D12" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -3447,11 +3447,11 @@
       <c r="B13" t="s">
         <v>100</v>
       </c>
-      <c r="C13">
+      <c r="C13" t="s">
+        <v>120</v>
+      </c>
+      <c r="D13">
         <v>10.95</v>
-      </c>
-      <c r="D13" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -3461,11 +3461,11 @@
       <c r="B14" t="s">
         <v>101</v>
       </c>
-      <c r="C14">
+      <c r="C14" t="s">
+        <v>120</v>
+      </c>
+      <c r="D14">
         <v>11.37</v>
-      </c>
-      <c r="D14" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -3475,11 +3475,11 @@
       <c r="B15" t="s">
         <v>102</v>
       </c>
-      <c r="C15">
+      <c r="C15" t="s">
+        <v>120</v>
+      </c>
+      <c r="D15">
         <v>11.4</v>
-      </c>
-      <c r="D15" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -3489,11 +3489,11 @@
       <c r="B16" t="s">
         <v>103</v>
       </c>
-      <c r="C16">
+      <c r="C16" t="s">
+        <v>120</v>
+      </c>
+      <c r="D16">
         <v>10.95</v>
-      </c>
-      <c r="D16" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -3503,11 +3503,11 @@
       <c r="B17" t="s">
         <v>104</v>
       </c>
-      <c r="C17">
+      <c r="C17" t="s">
+        <v>120</v>
+      </c>
+      <c r="D17">
         <v>18.8</v>
-      </c>
-      <c r="D17" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -3517,11 +3517,11 @@
       <c r="B18" t="s">
         <v>105</v>
       </c>
-      <c r="C18">
+      <c r="C18" t="s">
+        <v>120</v>
+      </c>
+      <c r="D18">
         <v>25.37</v>
-      </c>
-      <c r="D18" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -3531,11 +3531,11 @@
       <c r="B19" t="s">
         <v>106</v>
       </c>
-      <c r="C19">
+      <c r="C19" t="s">
+        <v>120</v>
+      </c>
+      <c r="D19">
         <v>19.5</v>
-      </c>
-      <c r="D19" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -3545,11 +3545,11 @@
       <c r="B20" t="s">
         <v>107</v>
       </c>
-      <c r="C20">
+      <c r="C20" t="s">
+        <v>120</v>
+      </c>
+      <c r="D20">
         <v>25.61</v>
-      </c>
-      <c r="D20" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -3559,11 +3559,11 @@
       <c r="B21" t="s">
         <v>108</v>
       </c>
-      <c r="C21">
+      <c r="C21" t="s">
+        <v>120</v>
+      </c>
+      <c r="D21">
         <v>11.89</v>
-      </c>
-      <c r="D21" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -3573,11 +3573,11 @@
       <c r="B22" t="s">
         <v>109</v>
       </c>
-      <c r="C22">
+      <c r="C22" t="s">
+        <v>120</v>
+      </c>
+      <c r="D22">
         <v>12.47</v>
-      </c>
-      <c r="D22" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -3587,11 +3587,11 @@
       <c r="B23" t="s">
         <v>110</v>
       </c>
-      <c r="C23">
+      <c r="C23" t="s">
+        <v>120</v>
+      </c>
+      <c r="D23">
         <v>12.67</v>
-      </c>
-      <c r="D23" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -3601,11 +3601,11 @@
       <c r="B24" t="s">
         <v>111</v>
       </c>
-      <c r="C24">
+      <c r="C24" t="s">
+        <v>120</v>
+      </c>
+      <c r="D24">
         <v>11.93</v>
-      </c>
-      <c r="D24" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -3615,11 +3615,11 @@
       <c r="B25" t="s">
         <v>112</v>
       </c>
-      <c r="C25">
+      <c r="C25" t="s">
+        <v>120</v>
+      </c>
+      <c r="D25">
         <v>14.45</v>
-      </c>
-      <c r="D25" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -3629,11 +3629,11 @@
       <c r="B26" t="s">
         <v>113</v>
       </c>
-      <c r="C26">
+      <c r="C26" t="s">
+        <v>120</v>
+      </c>
+      <c r="D26">
         <v>20.32</v>
-      </c>
-      <c r="D26" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -3643,11 +3643,11 @@
       <c r="B27" t="s">
         <v>114</v>
       </c>
-      <c r="C27">
+      <c r="C27" t="s">
+        <v>120</v>
+      </c>
+      <c r="D27">
         <v>14.67</v>
-      </c>
-      <c r="D27" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -3657,11 +3657,11 @@
       <c r="B28" t="s">
         <v>115</v>
       </c>
-      <c r="C28">
+      <c r="C28" t="s">
+        <v>120</v>
+      </c>
+      <c r="D28">
         <v>20.48</v>
-      </c>
-      <c r="D28" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -3671,11 +3671,11 @@
       <c r="B29" t="s">
         <v>116</v>
       </c>
-      <c r="C29">
+      <c r="C29" t="s">
+        <v>120</v>
+      </c>
+      <c r="D29">
         <v>9.460000000000001</v>
-      </c>
-      <c r="D29" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -3685,11 +3685,11 @@
       <c r="B30" t="s">
         <v>117</v>
       </c>
-      <c r="C30">
+      <c r="C30" t="s">
+        <v>120</v>
+      </c>
+      <c r="D30">
         <v>9.33</v>
-      </c>
-      <c r="D30" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -3699,11 +3699,11 @@
       <c r="B31" t="s">
         <v>118</v>
       </c>
-      <c r="C31">
+      <c r="C31" t="s">
+        <v>120</v>
+      </c>
+      <c r="D31">
         <v>9.449999999999999</v>
-      </c>
-      <c r="D31" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -3713,11 +3713,11 @@
       <c r="B32" t="s">
         <v>119</v>
       </c>
-      <c r="C32">
+      <c r="C32" t="s">
+        <v>120</v>
+      </c>
+      <c r="D32">
         <v>9.59</v>
-      </c>
-      <c r="D32" t="s">
-        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -3749,10 +3749,10 @@
         <v>55</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -3762,11 +3762,11 @@
       <c r="B2" t="s">
         <v>89</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D2">
         <v>11.2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -3776,11 +3776,11 @@
       <c r="B3" t="s">
         <v>90</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D3">
         <v>16.42</v>
-      </c>
-      <c r="D3" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -3790,11 +3790,11 @@
       <c r="B4" t="s">
         <v>91</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4">
         <v>16.59</v>
-      </c>
-      <c r="D4" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -3804,11 +3804,11 @@
       <c r="B5" t="s">
         <v>92</v>
       </c>
-      <c r="C5">
+      <c r="C5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5">
         <v>5.57</v>
-      </c>
-      <c r="D5" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -3818,11 +3818,11 @@
       <c r="B6" t="s">
         <v>93</v>
       </c>
-      <c r="C6">
+      <c r="C6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D6">
         <v>5.76</v>
-      </c>
-      <c r="D6" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -3832,11 +3832,11 @@
       <c r="B7" t="s">
         <v>94</v>
       </c>
-      <c r="C7">
+      <c r="C7" t="s">
+        <v>120</v>
+      </c>
+      <c r="D7">
         <v>5.67</v>
-      </c>
-      <c r="D7" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -3846,11 +3846,11 @@
       <c r="B8" t="s">
         <v>95</v>
       </c>
-      <c r="C8">
+      <c r="C8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D8">
         <v>5.58</v>
-      </c>
-      <c r="D8" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -3860,11 +3860,11 @@
       <c r="B9" t="s">
         <v>96</v>
       </c>
-      <c r="C9">
+      <c r="C9" t="s">
+        <v>120</v>
+      </c>
+      <c r="D9">
         <v>17.87</v>
-      </c>
-      <c r="D9" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -3874,11 +3874,11 @@
       <c r="B10" t="s">
         <v>97</v>
       </c>
-      <c r="C10">
+      <c r="C10" t="s">
+        <v>120</v>
+      </c>
+      <c r="D10">
         <v>23.73</v>
-      </c>
-      <c r="D10" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -3888,11 +3888,11 @@
       <c r="B11" t="s">
         <v>98</v>
       </c>
-      <c r="C11">
+      <c r="C11" t="s">
+        <v>120</v>
+      </c>
+      <c r="D11">
         <v>18.58</v>
-      </c>
-      <c r="D11" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -3902,11 +3902,11 @@
       <c r="B12" t="s">
         <v>99</v>
       </c>
-      <c r="C12">
+      <c r="C12" t="s">
+        <v>120</v>
+      </c>
+      <c r="D12">
         <v>23.9</v>
-      </c>
-      <c r="D12" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -3916,11 +3916,11 @@
       <c r="B13" t="s">
         <v>100</v>
       </c>
-      <c r="C13">
+      <c r="C13" t="s">
+        <v>120</v>
+      </c>
+      <c r="D13">
         <v>10.94</v>
-      </c>
-      <c r="D13" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -3930,11 +3930,11 @@
       <c r="B14" t="s">
         <v>101</v>
       </c>
-      <c r="C14">
+      <c r="C14" t="s">
+        <v>120</v>
+      </c>
+      <c r="D14">
         <v>11.37</v>
-      </c>
-      <c r="D14" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -3944,11 +3944,11 @@
       <c r="B15" t="s">
         <v>102</v>
       </c>
-      <c r="C15">
+      <c r="C15" t="s">
+        <v>120</v>
+      </c>
+      <c r="D15">
         <v>11.39</v>
-      </c>
-      <c r="D15" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -3958,11 +3958,11 @@
       <c r="B16" t="s">
         <v>103</v>
       </c>
-      <c r="C16">
+      <c r="C16" t="s">
+        <v>120</v>
+      </c>
+      <c r="D16">
         <v>10.95</v>
-      </c>
-      <c r="D16" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -3972,11 +3972,11 @@
       <c r="B17" t="s">
         <v>104</v>
       </c>
-      <c r="C17">
+      <c r="C17" t="s">
+        <v>120</v>
+      </c>
+      <c r="D17">
         <v>18.8</v>
-      </c>
-      <c r="D17" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -3986,11 +3986,11 @@
       <c r="B18" t="s">
         <v>105</v>
       </c>
-      <c r="C18">
+      <c r="C18" t="s">
+        <v>120</v>
+      </c>
+      <c r="D18">
         <v>25.48</v>
-      </c>
-      <c r="D18" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -4000,11 +4000,11 @@
       <c r="B19" t="s">
         <v>106</v>
       </c>
-      <c r="C19">
+      <c r="C19" t="s">
+        <v>120</v>
+      </c>
+      <c r="D19">
         <v>19.5</v>
-      </c>
-      <c r="D19" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -4014,11 +4014,11 @@
       <c r="B20" t="s">
         <v>107</v>
       </c>
-      <c r="C20">
+      <c r="C20" t="s">
+        <v>120</v>
+      </c>
+      <c r="D20">
         <v>25.63</v>
-      </c>
-      <c r="D20" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -4028,11 +4028,11 @@
       <c r="B21" t="s">
         <v>108</v>
       </c>
-      <c r="C21">
+      <c r="C21" t="s">
+        <v>120</v>
+      </c>
+      <c r="D21">
         <v>11.89</v>
-      </c>
-      <c r="D21" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -4042,11 +4042,11 @@
       <c r="B22" t="s">
         <v>109</v>
       </c>
-      <c r="C22">
+      <c r="C22" t="s">
+        <v>120</v>
+      </c>
+      <c r="D22">
         <v>12.45</v>
-      </c>
-      <c r="D22" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -4056,11 +4056,11 @@
       <c r="B23" t="s">
         <v>110</v>
       </c>
-      <c r="C23">
+      <c r="C23" t="s">
+        <v>120</v>
+      </c>
+      <c r="D23">
         <v>12.68</v>
-      </c>
-      <c r="D23" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -4070,11 +4070,11 @@
       <c r="B24" t="s">
         <v>111</v>
       </c>
-      <c r="C24">
+      <c r="C24" t="s">
+        <v>120</v>
+      </c>
+      <c r="D24">
         <v>11.94</v>
-      </c>
-      <c r="D24" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -4084,11 +4084,11 @@
       <c r="B25" t="s">
         <v>112</v>
       </c>
-      <c r="C25">
+      <c r="C25" t="s">
+        <v>120</v>
+      </c>
+      <c r="D25">
         <v>14.47</v>
-      </c>
-      <c r="D25" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -4098,11 +4098,11 @@
       <c r="B26" t="s">
         <v>113</v>
       </c>
-      <c r="C26">
+      <c r="C26" t="s">
+        <v>120</v>
+      </c>
+      <c r="D26">
         <v>20.36</v>
-      </c>
-      <c r="D26" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -4112,11 +4112,11 @@
       <c r="B27" t="s">
         <v>114</v>
       </c>
-      <c r="C27">
+      <c r="C27" t="s">
+        <v>120</v>
+      </c>
+      <c r="D27">
         <v>14.69</v>
-      </c>
-      <c r="D27" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -4126,11 +4126,11 @@
       <c r="B28" t="s">
         <v>115</v>
       </c>
-      <c r="C28">
+      <c r="C28" t="s">
+        <v>120</v>
+      </c>
+      <c r="D28">
         <v>20.53</v>
-      </c>
-      <c r="D28" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -4140,11 +4140,11 @@
       <c r="B29" t="s">
         <v>116</v>
       </c>
-      <c r="C29">
+      <c r="C29" t="s">
+        <v>120</v>
+      </c>
+      <c r="D29">
         <v>9.460000000000001</v>
-      </c>
-      <c r="D29" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -4154,11 +4154,11 @@
       <c r="B30" t="s">
         <v>117</v>
       </c>
-      <c r="C30">
+      <c r="C30" t="s">
+        <v>120</v>
+      </c>
+      <c r="D30">
         <v>9.32</v>
-      </c>
-      <c r="D30" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -4168,11 +4168,11 @@
       <c r="B31" t="s">
         <v>118</v>
       </c>
-      <c r="C31">
+      <c r="C31" t="s">
+        <v>120</v>
+      </c>
+      <c r="D31">
         <v>9.449999999999999</v>
-      </c>
-      <c r="D31" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -4182,11 +4182,11 @@
       <c r="B32" t="s">
         <v>119</v>
       </c>
-      <c r="C32">
+      <c r="C32" t="s">
+        <v>120</v>
+      </c>
+      <c r="D32">
         <v>9.59</v>
-      </c>
-      <c r="D32" t="s">
-        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -4218,10 +4218,10 @@
         <v>55</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -4231,11 +4231,11 @@
       <c r="B2" t="s">
         <v>89</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D2">
         <v>11.2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -4245,11 +4245,11 @@
       <c r="B3" t="s">
         <v>90</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D3">
         <v>16.44</v>
-      </c>
-      <c r="D3" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -4259,11 +4259,11 @@
       <c r="B4" t="s">
         <v>91</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4">
         <v>16.63</v>
-      </c>
-      <c r="D4" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -4273,11 +4273,11 @@
       <c r="B5" t="s">
         <v>92</v>
       </c>
-      <c r="C5">
+      <c r="C5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5">
         <v>5.57</v>
-      </c>
-      <c r="D5" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -4287,11 +4287,11 @@
       <c r="B6" t="s">
         <v>93</v>
       </c>
-      <c r="C6">
+      <c r="C6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D6">
         <v>5.75</v>
-      </c>
-      <c r="D6" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -4301,11 +4301,11 @@
       <c r="B7" t="s">
         <v>94</v>
       </c>
-      <c r="C7">
+      <c r="C7" t="s">
+        <v>120</v>
+      </c>
+      <c r="D7">
         <v>5.7</v>
-      </c>
-      <c r="D7" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -4315,11 +4315,11 @@
       <c r="B8" t="s">
         <v>95</v>
       </c>
-      <c r="C8">
+      <c r="C8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D8">
         <v>5.56</v>
-      </c>
-      <c r="D8" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -4329,11 +4329,11 @@
       <c r="B9" t="s">
         <v>96</v>
       </c>
-      <c r="C9">
+      <c r="C9" t="s">
+        <v>120</v>
+      </c>
+      <c r="D9">
         <v>17.87</v>
-      </c>
-      <c r="D9" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -4343,11 +4343,11 @@
       <c r="B10" t="s">
         <v>97</v>
       </c>
-      <c r="C10">
+      <c r="C10" t="s">
+        <v>120</v>
+      </c>
+      <c r="D10">
         <v>23.73</v>
-      </c>
-      <c r="D10" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -4357,11 +4357,11 @@
       <c r="B11" t="s">
         <v>98</v>
       </c>
-      <c r="C11">
+      <c r="C11" t="s">
+        <v>120</v>
+      </c>
+      <c r="D11">
         <v>18.57</v>
-      </c>
-      <c r="D11" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -4371,11 +4371,11 @@
       <c r="B12" t="s">
         <v>99</v>
       </c>
-      <c r="C12">
+      <c r="C12" t="s">
+        <v>120</v>
+      </c>
+      <c r="D12">
         <v>23.96</v>
-      </c>
-      <c r="D12" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -4385,11 +4385,11 @@
       <c r="B13" t="s">
         <v>100</v>
       </c>
-      <c r="C13">
+      <c r="C13" t="s">
+        <v>120</v>
+      </c>
+      <c r="D13">
         <v>10.94</v>
-      </c>
-      <c r="D13" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -4399,11 +4399,11 @@
       <c r="B14" t="s">
         <v>101</v>
       </c>
-      <c r="C14">
+      <c r="C14" t="s">
+        <v>120</v>
+      </c>
+      <c r="D14">
         <v>11.37</v>
-      </c>
-      <c r="D14" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -4413,11 +4413,11 @@
       <c r="B15" t="s">
         <v>102</v>
       </c>
-      <c r="C15">
+      <c r="C15" t="s">
+        <v>120</v>
+      </c>
+      <c r="D15">
         <v>11.42</v>
-      </c>
-      <c r="D15" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -4427,11 +4427,11 @@
       <c r="B16" t="s">
         <v>103</v>
       </c>
-      <c r="C16">
+      <c r="C16" t="s">
+        <v>120</v>
+      </c>
+      <c r="D16">
         <v>10.95</v>
-      </c>
-      <c r="D16" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -4441,11 +4441,11 @@
       <c r="B17" t="s">
         <v>104</v>
       </c>
-      <c r="C17">
+      <c r="C17" t="s">
+        <v>120</v>
+      </c>
+      <c r="D17">
         <v>18.8</v>
-      </c>
-      <c r="D17" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -4455,11 +4455,11 @@
       <c r="B18" t="s">
         <v>105</v>
       </c>
-      <c r="C18">
+      <c r="C18" t="s">
+        <v>120</v>
+      </c>
+      <c r="D18">
         <v>25.48</v>
-      </c>
-      <c r="D18" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -4469,11 +4469,11 @@
       <c r="B19" t="s">
         <v>106</v>
       </c>
-      <c r="C19">
+      <c r="C19" t="s">
+        <v>120</v>
+      </c>
+      <c r="D19">
         <v>19.5</v>
-      </c>
-      <c r="D19" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -4483,11 +4483,11 @@
       <c r="B20" t="s">
         <v>107</v>
       </c>
-      <c r="C20">
+      <c r="C20" t="s">
+        <v>120</v>
+      </c>
+      <c r="D20">
         <v>25.71</v>
-      </c>
-      <c r="D20" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -4497,11 +4497,11 @@
       <c r="B21" t="s">
         <v>108</v>
       </c>
-      <c r="C21">
+      <c r="C21" t="s">
+        <v>120</v>
+      </c>
+      <c r="D21">
         <v>11.89</v>
-      </c>
-      <c r="D21" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -4511,11 +4511,11 @@
       <c r="B22" t="s">
         <v>109</v>
       </c>
-      <c r="C22">
+      <c r="C22" t="s">
+        <v>120</v>
+      </c>
+      <c r="D22">
         <v>12.48</v>
-      </c>
-      <c r="D22" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -4525,11 +4525,11 @@
       <c r="B23" t="s">
         <v>110</v>
       </c>
-      <c r="C23">
+      <c r="C23" t="s">
+        <v>120</v>
+      </c>
+      <c r="D23">
         <v>12.65</v>
-      </c>
-      <c r="D23" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -4539,11 +4539,11 @@
       <c r="B24" t="s">
         <v>111</v>
       </c>
-      <c r="C24">
+      <c r="C24" t="s">
+        <v>120</v>
+      </c>
+      <c r="D24">
         <v>11.93</v>
-      </c>
-      <c r="D24" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -4553,11 +4553,11 @@
       <c r="B25" t="s">
         <v>112</v>
       </c>
-      <c r="C25">
+      <c r="C25" t="s">
+        <v>120</v>
+      </c>
+      <c r="D25">
         <v>14.47</v>
-      </c>
-      <c r="D25" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -4567,11 +4567,11 @@
       <c r="B26" t="s">
         <v>113</v>
       </c>
-      <c r="C26">
+      <c r="C26" t="s">
+        <v>120</v>
+      </c>
+      <c r="D26">
         <v>20.36</v>
-      </c>
-      <c r="D26" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -4581,11 +4581,11 @@
       <c r="B27" t="s">
         <v>114</v>
       </c>
-      <c r="C27">
+      <c r="C27" t="s">
+        <v>120</v>
+      </c>
+      <c r="D27">
         <v>14.69</v>
-      </c>
-      <c r="D27" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -4595,11 +4595,11 @@
       <c r="B28" t="s">
         <v>115</v>
       </c>
-      <c r="C28">
+      <c r="C28" t="s">
+        <v>120</v>
+      </c>
+      <c r="D28">
         <v>20.57</v>
-      </c>
-      <c r="D28" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -4609,11 +4609,11 @@
       <c r="B29" t="s">
         <v>116</v>
       </c>
-      <c r="C29">
+      <c r="C29" t="s">
+        <v>120</v>
+      </c>
+      <c r="D29">
         <v>9.460000000000001</v>
-      </c>
-      <c r="D29" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -4623,11 +4623,11 @@
       <c r="B30" t="s">
         <v>117</v>
       </c>
-      <c r="C30">
+      <c r="C30" t="s">
+        <v>120</v>
+      </c>
+      <c r="D30">
         <v>9.32</v>
-      </c>
-      <c r="D30" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -4637,11 +4637,11 @@
       <c r="B31" t="s">
         <v>118</v>
       </c>
-      <c r="C31">
+      <c r="C31" t="s">
+        <v>120</v>
+      </c>
+      <c r="D31">
         <v>9.449999999999999</v>
-      </c>
-      <c r="D31" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -4651,11 +4651,11 @@
       <c r="B32" t="s">
         <v>119</v>
       </c>
-      <c r="C32">
+      <c r="C32" t="s">
+        <v>120</v>
+      </c>
+      <c r="D32">
         <v>9.59</v>
-      </c>
-      <c r="D32" t="s">
-        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -4687,10 +4687,10 @@
         <v>55</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -4700,11 +4700,11 @@
       <c r="B2" t="s">
         <v>89</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D2">
         <v>11.21</v>
-      </c>
-      <c r="D2" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -4714,11 +4714,11 @@
       <c r="B3" t="s">
         <v>90</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D3">
         <v>16.46</v>
-      </c>
-      <c r="D3" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -4728,11 +4728,11 @@
       <c r="B4" t="s">
         <v>91</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4">
         <v>16.65</v>
-      </c>
-      <c r="D4" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -4742,11 +4742,11 @@
       <c r="B5" t="s">
         <v>92</v>
       </c>
-      <c r="C5">
+      <c r="C5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5">
         <v>5.57</v>
-      </c>
-      <c r="D5" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -4756,11 +4756,11 @@
       <c r="B6" t="s">
         <v>93</v>
       </c>
-      <c r="C6">
+      <c r="C6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D6">
         <v>5.74</v>
-      </c>
-      <c r="D6" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -4770,11 +4770,11 @@
       <c r="B7" t="s">
         <v>94</v>
       </c>
-      <c r="C7">
+      <c r="C7" t="s">
+        <v>120</v>
+      </c>
+      <c r="D7">
         <v>5.7</v>
-      </c>
-      <c r="D7" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -4784,11 +4784,11 @@
       <c r="B8" t="s">
         <v>95</v>
       </c>
-      <c r="C8">
+      <c r="C8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D8">
         <v>5.56</v>
-      </c>
-      <c r="D8" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -4798,11 +4798,11 @@
       <c r="B9" t="s">
         <v>96</v>
       </c>
-      <c r="C9">
+      <c r="C9" t="s">
+        <v>120</v>
+      </c>
+      <c r="D9">
         <v>17.85</v>
-      </c>
-      <c r="D9" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -4812,11 +4812,11 @@
       <c r="B10" t="s">
         <v>97</v>
       </c>
-      <c r="C10">
+      <c r="C10" t="s">
+        <v>120</v>
+      </c>
+      <c r="D10">
         <v>23.73</v>
-      </c>
-      <c r="D10" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -4826,11 +4826,11 @@
       <c r="B11" t="s">
         <v>98</v>
       </c>
-      <c r="C11">
+      <c r="C11" t="s">
+        <v>120</v>
+      </c>
+      <c r="D11">
         <v>18.56</v>
-      </c>
-      <c r="D11" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -4840,11 +4840,11 @@
       <c r="B12" t="s">
         <v>99</v>
       </c>
-      <c r="C12">
+      <c r="C12" t="s">
+        <v>120</v>
+      </c>
+      <c r="D12">
         <v>23.96</v>
-      </c>
-      <c r="D12" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -4854,11 +4854,11 @@
       <c r="B13" t="s">
         <v>100</v>
       </c>
-      <c r="C13">
+      <c r="C13" t="s">
+        <v>120</v>
+      </c>
+      <c r="D13">
         <v>10.91</v>
-      </c>
-      <c r="D13" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -4868,11 +4868,11 @@
       <c r="B14" t="s">
         <v>101</v>
       </c>
-      <c r="C14">
+      <c r="C14" t="s">
+        <v>120</v>
+      </c>
+      <c r="D14">
         <v>11.37</v>
-      </c>
-      <c r="D14" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -4882,11 +4882,11 @@
       <c r="B15" t="s">
         <v>102</v>
       </c>
-      <c r="C15">
+      <c r="C15" t="s">
+        <v>120</v>
+      </c>
+      <c r="D15">
         <v>11.4</v>
-      </c>
-      <c r="D15" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -4896,11 +4896,11 @@
       <c r="B16" t="s">
         <v>103</v>
       </c>
-      <c r="C16">
+      <c r="C16" t="s">
+        <v>120</v>
+      </c>
+      <c r="D16">
         <v>10.95</v>
-      </c>
-      <c r="D16" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -4910,11 +4910,11 @@
       <c r="B17" t="s">
         <v>104</v>
       </c>
-      <c r="C17">
+      <c r="C17" t="s">
+        <v>120</v>
+      </c>
+      <c r="D17">
         <v>18.8</v>
-      </c>
-      <c r="D17" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -4924,11 +4924,11 @@
       <c r="B18" t="s">
         <v>105</v>
       </c>
-      <c r="C18">
+      <c r="C18" t="s">
+        <v>120</v>
+      </c>
+      <c r="D18">
         <v>25.5</v>
-      </c>
-      <c r="D18" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -4938,11 +4938,11 @@
       <c r="B19" t="s">
         <v>106</v>
       </c>
-      <c r="C19">
+      <c r="C19" t="s">
+        <v>120</v>
+      </c>
+      <c r="D19">
         <v>19.46</v>
-      </c>
-      <c r="D19" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -4952,11 +4952,11 @@
       <c r="B20" t="s">
         <v>107</v>
       </c>
-      <c r="C20">
+      <c r="C20" t="s">
+        <v>120</v>
+      </c>
+      <c r="D20">
         <v>25.73</v>
-      </c>
-      <c r="D20" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -4966,11 +4966,11 @@
       <c r="B21" t="s">
         <v>108</v>
       </c>
-      <c r="C21">
+      <c r="C21" t="s">
+        <v>120</v>
+      </c>
+      <c r="D21">
         <v>11.89</v>
-      </c>
-      <c r="D21" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -4980,11 +4980,11 @@
       <c r="B22" t="s">
         <v>109</v>
       </c>
-      <c r="C22">
+      <c r="C22" t="s">
+        <v>120</v>
+      </c>
+      <c r="D22">
         <v>12.45</v>
-      </c>
-      <c r="D22" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -4994,11 +4994,11 @@
       <c r="B23" t="s">
         <v>110</v>
       </c>
-      <c r="C23">
+      <c r="C23" t="s">
+        <v>120</v>
+      </c>
+      <c r="D23">
         <v>12.66</v>
-      </c>
-      <c r="D23" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -5008,11 +5008,11 @@
       <c r="B24" t="s">
         <v>111</v>
       </c>
-      <c r="C24">
+      <c r="C24" t="s">
+        <v>120</v>
+      </c>
+      <c r="D24">
         <v>11.92</v>
-      </c>
-      <c r="D24" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -5022,11 +5022,11 @@
       <c r="B25" t="s">
         <v>112</v>
       </c>
-      <c r="C25">
+      <c r="C25" t="s">
+        <v>120</v>
+      </c>
+      <c r="D25">
         <v>14.46</v>
-      </c>
-      <c r="D25" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -5036,11 +5036,11 @@
       <c r="B26" t="s">
         <v>113</v>
       </c>
-      <c r="C26">
+      <c r="C26" t="s">
+        <v>120</v>
+      </c>
+      <c r="D26">
         <v>20.4</v>
-      </c>
-      <c r="D26" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -5050,11 +5050,11 @@
       <c r="B27" t="s">
         <v>114</v>
       </c>
-      <c r="C27">
+      <c r="C27" t="s">
+        <v>120</v>
+      </c>
+      <c r="D27">
         <v>14.71</v>
-      </c>
-      <c r="D27" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -5064,11 +5064,11 @@
       <c r="B28" t="s">
         <v>115</v>
       </c>
-      <c r="C28">
+      <c r="C28" t="s">
+        <v>120</v>
+      </c>
+      <c r="D28">
         <v>20.59</v>
-      </c>
-      <c r="D28" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -5078,11 +5078,11 @@
       <c r="B29" t="s">
         <v>116</v>
       </c>
-      <c r="C29">
+      <c r="C29" t="s">
+        <v>120</v>
+      </c>
+      <c r="D29">
         <v>9.460000000000001</v>
-      </c>
-      <c r="D29" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -5092,11 +5092,11 @@
       <c r="B30" t="s">
         <v>117</v>
       </c>
-      <c r="C30">
+      <c r="C30" t="s">
+        <v>120</v>
+      </c>
+      <c r="D30">
         <v>9.32</v>
-      </c>
-      <c r="D30" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -5106,11 +5106,11 @@
       <c r="B31" t="s">
         <v>118</v>
       </c>
-      <c r="C31">
+      <c r="C31" t="s">
+        <v>120</v>
+      </c>
+      <c r="D31">
         <v>9.44</v>
-      </c>
-      <c r="D31" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -5120,11 +5120,11 @@
       <c r="B32" t="s">
         <v>119</v>
       </c>
-      <c r="C32">
+      <c r="C32" t="s">
+        <v>120</v>
+      </c>
+      <c r="D32">
         <v>9.59</v>
-      </c>
-      <c r="D32" t="s">
-        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -5156,10 +5156,10 @@
         <v>55</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -5169,11 +5169,11 @@
       <c r="B2" t="s">
         <v>89</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D2">
         <v>11.2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -5183,11 +5183,11 @@
       <c r="B3" t="s">
         <v>90</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D3">
         <v>16.5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -5197,11 +5197,11 @@
       <c r="B4" t="s">
         <v>91</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4">
         <v>16.67</v>
-      </c>
-      <c r="D4" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -5211,11 +5211,11 @@
       <c r="B5" t="s">
         <v>92</v>
       </c>
-      <c r="C5">
+      <c r="C5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5">
         <v>5.57</v>
-      </c>
-      <c r="D5" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -5225,11 +5225,11 @@
       <c r="B6" t="s">
         <v>93</v>
       </c>
-      <c r="C6">
+      <c r="C6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D6">
         <v>5.74</v>
-      </c>
-      <c r="D6" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -5239,11 +5239,11 @@
       <c r="B7" t="s">
         <v>94</v>
       </c>
-      <c r="C7">
+      <c r="C7" t="s">
+        <v>120</v>
+      </c>
+      <c r="D7">
         <v>5.7</v>
-      </c>
-      <c r="D7" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -5253,11 +5253,11 @@
       <c r="B8" t="s">
         <v>95</v>
       </c>
-      <c r="C8">
+      <c r="C8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D8">
         <v>5.55</v>
-      </c>
-      <c r="D8" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -5267,11 +5267,11 @@
       <c r="B9" t="s">
         <v>96</v>
       </c>
-      <c r="C9">
+      <c r="C9" t="s">
+        <v>120</v>
+      </c>
+      <c r="D9">
         <v>17.85</v>
-      </c>
-      <c r="D9" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -5281,11 +5281,11 @@
       <c r="B10" t="s">
         <v>97</v>
       </c>
-      <c r="C10">
+      <c r="C10" t="s">
+        <v>120</v>
+      </c>
+      <c r="D10">
         <v>23.75</v>
-      </c>
-      <c r="D10" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -5295,11 +5295,11 @@
       <c r="B11" t="s">
         <v>98</v>
       </c>
-      <c r="C11">
+      <c r="C11" t="s">
+        <v>120</v>
+      </c>
+      <c r="D11">
         <v>18.57</v>
-      </c>
-      <c r="D11" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -5309,11 +5309,11 @@
       <c r="B12" t="s">
         <v>99</v>
       </c>
-      <c r="C12">
+      <c r="C12" t="s">
+        <v>120</v>
+      </c>
+      <c r="D12">
         <v>24</v>
-      </c>
-      <c r="D12" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -5323,11 +5323,11 @@
       <c r="B13" t="s">
         <v>100</v>
       </c>
-      <c r="C13">
+      <c r="C13" t="s">
+        <v>120</v>
+      </c>
+      <c r="D13">
         <v>10.9</v>
-      </c>
-      <c r="D13" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -5337,11 +5337,11 @@
       <c r="B14" t="s">
         <v>101</v>
       </c>
-      <c r="C14">
+      <c r="C14" t="s">
+        <v>120</v>
+      </c>
+      <c r="D14">
         <v>11.37</v>
-      </c>
-      <c r="D14" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -5351,11 +5351,11 @@
       <c r="B15" t="s">
         <v>102</v>
       </c>
-      <c r="C15">
+      <c r="C15" t="s">
+        <v>120</v>
+      </c>
+      <c r="D15">
         <v>11.4</v>
-      </c>
-      <c r="D15" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -5365,11 +5365,11 @@
       <c r="B16" t="s">
         <v>103</v>
       </c>
-      <c r="C16">
+      <c r="C16" t="s">
+        <v>120</v>
+      </c>
+      <c r="D16">
         <v>10.94</v>
-      </c>
-      <c r="D16" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -5379,11 +5379,11 @@
       <c r="B17" t="s">
         <v>104</v>
       </c>
-      <c r="C17">
+      <c r="C17" t="s">
+        <v>120</v>
+      </c>
+      <c r="D17">
         <v>18.81</v>
-      </c>
-      <c r="D17" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -5393,11 +5393,11 @@
       <c r="B18" t="s">
         <v>105</v>
       </c>
-      <c r="C18">
+      <c r="C18" t="s">
+        <v>120</v>
+      </c>
+      <c r="D18">
         <v>25.5</v>
-      </c>
-      <c r="D18" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -5407,11 +5407,11 @@
       <c r="B19" t="s">
         <v>106</v>
       </c>
-      <c r="C19">
+      <c r="C19" t="s">
+        <v>120</v>
+      </c>
+      <c r="D19">
         <v>19.49</v>
-      </c>
-      <c r="D19" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -5421,11 +5421,11 @@
       <c r="B20" t="s">
         <v>107</v>
       </c>
-      <c r="C20">
+      <c r="C20" t="s">
+        <v>120</v>
+      </c>
+      <c r="D20">
         <v>25.73</v>
-      </c>
-      <c r="D20" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -5435,11 +5435,11 @@
       <c r="B21" t="s">
         <v>108</v>
       </c>
-      <c r="C21">
+      <c r="C21" t="s">
+        <v>120</v>
+      </c>
+      <c r="D21">
         <v>11.89</v>
-      </c>
-      <c r="D21" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -5449,11 +5449,11 @@
       <c r="B22" t="s">
         <v>109</v>
       </c>
-      <c r="C22">
+      <c r="C22" t="s">
+        <v>120</v>
+      </c>
+      <c r="D22">
         <v>12.45</v>
-      </c>
-      <c r="D22" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -5463,11 +5463,11 @@
       <c r="B23" t="s">
         <v>110</v>
       </c>
-      <c r="C23">
+      <c r="C23" t="s">
+        <v>120</v>
+      </c>
+      <c r="D23">
         <v>12.68</v>
-      </c>
-      <c r="D23" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -5477,11 +5477,11 @@
       <c r="B24" t="s">
         <v>111</v>
       </c>
-      <c r="C24">
+      <c r="C24" t="s">
+        <v>120</v>
+      </c>
+      <c r="D24">
         <v>11.92</v>
-      </c>
-      <c r="D24" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -5491,11 +5491,11 @@
       <c r="B25" t="s">
         <v>112</v>
       </c>
-      <c r="C25">
+      <c r="C25" t="s">
+        <v>120</v>
+      </c>
+      <c r="D25">
         <v>14.47</v>
-      </c>
-      <c r="D25" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -5505,11 +5505,11 @@
       <c r="B26" t="s">
         <v>113</v>
       </c>
-      <c r="C26">
+      <c r="C26" t="s">
+        <v>120</v>
+      </c>
+      <c r="D26">
         <v>20.42</v>
-      </c>
-      <c r="D26" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -5519,11 +5519,11 @@
       <c r="B27" t="s">
         <v>114</v>
       </c>
-      <c r="C27">
+      <c r="C27" t="s">
+        <v>120</v>
+      </c>
+      <c r="D27">
         <v>14.7</v>
-      </c>
-      <c r="D27" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -5533,11 +5533,11 @@
       <c r="B28" t="s">
         <v>115</v>
       </c>
-      <c r="C28">
+      <c r="C28" t="s">
+        <v>120</v>
+      </c>
+      <c r="D28">
         <v>20.63</v>
-      </c>
-      <c r="D28" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -5547,11 +5547,11 @@
       <c r="B29" t="s">
         <v>116</v>
       </c>
-      <c r="C29">
+      <c r="C29" t="s">
+        <v>120</v>
+      </c>
+      <c r="D29">
         <v>9.460000000000001</v>
-      </c>
-      <c r="D29" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -5561,11 +5561,11 @@
       <c r="B30" t="s">
         <v>117</v>
       </c>
-      <c r="C30">
+      <c r="C30" t="s">
+        <v>120</v>
+      </c>
+      <c r="D30">
         <v>9.33</v>
-      </c>
-      <c r="D30" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -5575,11 +5575,11 @@
       <c r="B31" t="s">
         <v>118</v>
       </c>
-      <c r="C31">
+      <c r="C31" t="s">
+        <v>120</v>
+      </c>
+      <c r="D31">
         <v>9.44</v>
-      </c>
-      <c r="D31" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -5589,11 +5589,11 @@
       <c r="B32" t="s">
         <v>119</v>
       </c>
-      <c r="C32">
+      <c r="C32" t="s">
+        <v>120</v>
+      </c>
+      <c r="D32">
         <v>9.59</v>
-      </c>
-      <c r="D32" t="s">
-        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Replaced any doc strings where "hour" is used with "time" to show generalisation of functions for any reporting interval
</commit_message>
<xml_diff>
--- a/tests/testmodels/TestJob1/mf_results/tm59mechvent/TM59MechVent__TestJob1.xlsx
+++ b/tests/testmodels/TestJob1/mf_results/tm59mechvent/TM59MechVent__TestJob1.xlsx
@@ -30,15 +30,15 @@
     <t>JobNo</t>
   </si>
   <si>
+    <t>Author</t>
+  </si>
+  <si>
     <t>Date</t>
   </si>
   <si>
     <t>sheet_name</t>
   </si>
   <si>
-    <t>Author</t>
-  </si>
-  <si>
     <t>0</t>
   </si>
   <si>
@@ -75,7 +75,10 @@
     <t>/c/e</t>
   </si>
   <si>
-    <t>20220316</t>
+    <t>jovyan</t>
+  </si>
+  <si>
+    <t>20220324</t>
   </si>
   <si>
     <t>Project Information</t>
@@ -111,9 +114,6 @@
     <t>Results, Air Speed 0.8</t>
   </si>
   <si>
-    <t>jovyan</t>
-  </si>
-  <si>
     <t>index</t>
   </si>
   <si>
@@ -177,7 +177,7 @@
     <t>51.38</t>
   </si>
   <si>
-    <t>2022-03-16 17:29:22.271374</t>
+    <t>2022-03-24 17:14:06.454540</t>
   </si>
   <si>
     <t>2021.4.0.0</t>
@@ -572,9 +572,9 @@
   <tableColumns count="5">
     <tableColumn id="1" name="index"/>
     <tableColumn id="2" name="JobNo"/>
-    <tableColumn id="3" name="Date"/>
-    <tableColumn id="4" name="sheet_name"/>
-    <tableColumn id="5" name="Author"/>
+    <tableColumn id="3" name="Author"/>
+    <tableColumn id="4" name="Date"/>
+    <tableColumn id="5" name="sheet_name"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -586,8 +586,8 @@
   <tableColumns count="4">
     <tableColumn id="1" name="Room ID"/>
     <tableColumn id="2" name="Room Name"/>
-    <tableColumn id="3" name="Fixed Temp Criterion (Pass/Fail)"/>
-    <tableColumn id="4" name="Fixed Temp Criterion (% Hours Operative Temp &gt; 26 Deg. Celsius)"/>
+    <tableColumn id="3" name="Fixed Temp Criterion (% Hours Operative Temp &gt; 26 Deg. Celsius)"/>
+    <tableColumn id="4" name="Fixed Temp Criterion (Pass/Fail)"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -599,8 +599,8 @@
   <tableColumns count="4">
     <tableColumn id="1" name="Room ID"/>
     <tableColumn id="2" name="Room Name"/>
-    <tableColumn id="3" name="Fixed Temp Criterion (Pass/Fail)"/>
-    <tableColumn id="4" name="Fixed Temp Criterion (% Hours Operative Temp &gt; 26 Deg. Celsius)"/>
+    <tableColumn id="3" name="Fixed Temp Criterion (% Hours Operative Temp &gt; 26 Deg. Celsius)"/>
+    <tableColumn id="4" name="Fixed Temp Criterion (Pass/Fail)"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -612,8 +612,8 @@
   <tableColumns count="4">
     <tableColumn id="1" name="Room ID"/>
     <tableColumn id="2" name="Room Name"/>
-    <tableColumn id="3" name="Fixed Temp Criterion (Pass/Fail)"/>
-    <tableColumn id="4" name="Fixed Temp Criterion (% Hours Operative Temp &gt; 26 Deg. Celsius)"/>
+    <tableColumn id="3" name="Fixed Temp Criterion (% Hours Operative Temp &gt; 26 Deg. Celsius)"/>
+    <tableColumn id="4" name="Fixed Temp Criterion (Pass/Fail)"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -647,8 +647,8 @@
   <tableColumns count="4">
     <tableColumn id="1" name="Room ID"/>
     <tableColumn id="2" name="Room Name"/>
-    <tableColumn id="3" name="Fixed Temp Criterion (Pass/Fail)"/>
-    <tableColumn id="4" name="Fixed Temp Criterion (% Hours Operative Temp &gt; 26 Deg. Celsius)"/>
+    <tableColumn id="3" name="Fixed Temp Criterion (% Hours Operative Temp &gt; 26 Deg. Celsius)"/>
+    <tableColumn id="4" name="Fixed Temp Criterion (Pass/Fail)"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -660,8 +660,8 @@
   <tableColumns count="4">
     <tableColumn id="1" name="Room ID"/>
     <tableColumn id="2" name="Room Name"/>
-    <tableColumn id="3" name="Fixed Temp Criterion (Pass/Fail)"/>
-    <tableColumn id="4" name="Fixed Temp Criterion (% Hours Operative Temp &gt; 26 Deg. Celsius)"/>
+    <tableColumn id="3" name="Fixed Temp Criterion (% Hours Operative Temp &gt; 26 Deg. Celsius)"/>
+    <tableColumn id="4" name="Fixed Temp Criterion (Pass/Fail)"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -673,8 +673,8 @@
   <tableColumns count="4">
     <tableColumn id="1" name="Room ID"/>
     <tableColumn id="2" name="Room Name"/>
-    <tableColumn id="3" name="Fixed Temp Criterion (Pass/Fail)"/>
-    <tableColumn id="4" name="Fixed Temp Criterion (% Hours Operative Temp &gt; 26 Deg. Celsius)"/>
+    <tableColumn id="3" name="Fixed Temp Criterion (% Hours Operative Temp &gt; 26 Deg. Celsius)"/>
+    <tableColumn id="4" name="Fixed Temp Criterion (Pass/Fail)"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -686,8 +686,8 @@
   <tableColumns count="4">
     <tableColumn id="1" name="Room ID"/>
     <tableColumn id="2" name="Room Name"/>
-    <tableColumn id="3" name="Fixed Temp Criterion (Pass/Fail)"/>
-    <tableColumn id="4" name="Fixed Temp Criterion (% Hours Operative Temp &gt; 26 Deg. Celsius)"/>
+    <tableColumn id="3" name="Fixed Temp Criterion (% Hours Operative Temp &gt; 26 Deg. Celsius)"/>
+    <tableColumn id="4" name="Fixed Temp Criterion (Pass/Fail)"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -699,8 +699,8 @@
   <tableColumns count="4">
     <tableColumn id="1" name="Room ID"/>
     <tableColumn id="2" name="Room Name"/>
-    <tableColumn id="3" name="Fixed Temp Criterion (Pass/Fail)"/>
-    <tableColumn id="4" name="Fixed Temp Criterion (% Hours Operative Temp &gt; 26 Deg. Celsius)"/>
+    <tableColumn id="3" name="Fixed Temp Criterion (% Hours Operative Temp &gt; 26 Deg. Celsius)"/>
+    <tableColumn id="4" name="Fixed Temp Criterion (Pass/Fail)"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -712,8 +712,8 @@
   <tableColumns count="4">
     <tableColumn id="1" name="Room ID"/>
     <tableColumn id="2" name="Room Name"/>
-    <tableColumn id="3" name="Fixed Temp Criterion (Pass/Fail)"/>
-    <tableColumn id="4" name="Fixed Temp Criterion (% Hours Operative Temp &gt; 26 Deg. Celsius)"/>
+    <tableColumn id="3" name="Fixed Temp Criterion (% Hours Operative Temp &gt; 26 Deg. Celsius)"/>
+    <tableColumn id="4" name="Fixed Temp Criterion (Pass/Fail)"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1050,7 +1050,7 @@
         <v>17</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1064,10 +1064,10 @@
         <v>16</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1081,10 +1081,10 @@
         <v>16</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1098,10 +1098,10 @@
         <v>16</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1115,10 +1115,10 @@
         <v>16</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1132,10 +1132,10 @@
         <v>16</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1149,10 +1149,10 @@
         <v>16</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1166,10 +1166,10 @@
         <v>16</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1183,10 +1183,10 @@
         <v>16</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1200,10 +1200,10 @@
         <v>16</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1217,7 +1217,7 @@
         <v>16</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>28</v>
@@ -1253,10 +1253,10 @@
         <v>55</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1266,11 +1266,11 @@
       <c r="B2" t="s">
         <v>89</v>
       </c>
-      <c r="C2" t="s">
-        <v>120</v>
-      </c>
-      <c r="D2">
+      <c r="C2">
         <v>11.2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1280,11 +1280,11 @@
       <c r="B3" t="s">
         <v>90</v>
       </c>
-      <c r="C3" t="s">
-        <v>120</v>
-      </c>
-      <c r="D3">
+      <c r="C3">
         <v>16.5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1294,11 +1294,11 @@
       <c r="B4" t="s">
         <v>91</v>
       </c>
-      <c r="C4" t="s">
-        <v>120</v>
-      </c>
-      <c r="D4">
+      <c r="C4">
         <v>16.67</v>
+      </c>
+      <c r="D4" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1308,11 +1308,11 @@
       <c r="B5" t="s">
         <v>92</v>
       </c>
-      <c r="C5" t="s">
-        <v>120</v>
-      </c>
-      <c r="D5">
+      <c r="C5">
         <v>5.58</v>
+      </c>
+      <c r="D5" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1322,11 +1322,11 @@
       <c r="B6" t="s">
         <v>93</v>
       </c>
-      <c r="C6" t="s">
-        <v>120</v>
-      </c>
-      <c r="D6">
+      <c r="C6">
         <v>5.74</v>
+      </c>
+      <c r="D6" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1336,11 +1336,11 @@
       <c r="B7" t="s">
         <v>94</v>
       </c>
-      <c r="C7" t="s">
-        <v>120</v>
-      </c>
-      <c r="D7">
+      <c r="C7">
         <v>5.7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1350,11 +1350,11 @@
       <c r="B8" t="s">
         <v>95</v>
       </c>
-      <c r="C8" t="s">
-        <v>120</v>
-      </c>
-      <c r="D8">
+      <c r="C8">
         <v>5.55</v>
+      </c>
+      <c r="D8" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1364,11 +1364,11 @@
       <c r="B9" t="s">
         <v>96</v>
       </c>
-      <c r="C9" t="s">
-        <v>120</v>
-      </c>
-      <c r="D9">
+      <c r="C9">
         <v>17.87</v>
+      </c>
+      <c r="D9" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1378,11 +1378,11 @@
       <c r="B10" t="s">
         <v>97</v>
       </c>
-      <c r="C10" t="s">
-        <v>120</v>
-      </c>
-      <c r="D10">
+      <c r="C10">
         <v>23.75</v>
+      </c>
+      <c r="D10" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1392,11 +1392,11 @@
       <c r="B11" t="s">
         <v>98</v>
       </c>
-      <c r="C11" t="s">
-        <v>120</v>
-      </c>
-      <c r="D11">
+      <c r="C11">
         <v>18.57</v>
+      </c>
+      <c r="D11" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -1406,11 +1406,11 @@
       <c r="B12" t="s">
         <v>99</v>
       </c>
-      <c r="C12" t="s">
-        <v>120</v>
-      </c>
-      <c r="D12">
+      <c r="C12">
         <v>24.03</v>
+      </c>
+      <c r="D12" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1420,11 +1420,11 @@
       <c r="B13" t="s">
         <v>100</v>
       </c>
-      <c r="C13" t="s">
-        <v>120</v>
-      </c>
-      <c r="D13">
+      <c r="C13">
         <v>10.9</v>
+      </c>
+      <c r="D13" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1434,11 +1434,11 @@
       <c r="B14" t="s">
         <v>101</v>
       </c>
-      <c r="C14" t="s">
-        <v>120</v>
-      </c>
-      <c r="D14">
+      <c r="C14">
         <v>11.37</v>
+      </c>
+      <c r="D14" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -1448,11 +1448,11 @@
       <c r="B15" t="s">
         <v>102</v>
       </c>
-      <c r="C15" t="s">
-        <v>120</v>
-      </c>
-      <c r="D15">
+      <c r="C15">
         <v>11.4</v>
+      </c>
+      <c r="D15" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1462,11 +1462,11 @@
       <c r="B16" t="s">
         <v>103</v>
       </c>
-      <c r="C16" t="s">
-        <v>120</v>
-      </c>
-      <c r="D16">
+      <c r="C16">
         <v>10.94</v>
+      </c>
+      <c r="D16" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1476,11 +1476,11 @@
       <c r="B17" t="s">
         <v>104</v>
       </c>
-      <c r="C17" t="s">
-        <v>120</v>
-      </c>
-      <c r="D17">
+      <c r="C17">
         <v>18.81</v>
+      </c>
+      <c r="D17" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1490,11 +1490,11 @@
       <c r="B18" t="s">
         <v>105</v>
       </c>
-      <c r="C18" t="s">
-        <v>120</v>
-      </c>
-      <c r="D18">
+      <c r="C18">
         <v>25.52</v>
+      </c>
+      <c r="D18" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1504,11 +1504,11 @@
       <c r="B19" t="s">
         <v>106</v>
       </c>
-      <c r="C19" t="s">
-        <v>120</v>
-      </c>
-      <c r="D19">
+      <c r="C19">
         <v>19.47</v>
+      </c>
+      <c r="D19" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1518,11 +1518,11 @@
       <c r="B20" t="s">
         <v>107</v>
       </c>
-      <c r="C20" t="s">
-        <v>120</v>
-      </c>
-      <c r="D20">
+      <c r="C20">
         <v>25.73</v>
+      </c>
+      <c r="D20" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -1532,11 +1532,11 @@
       <c r="B21" t="s">
         <v>108</v>
       </c>
-      <c r="C21" t="s">
-        <v>120</v>
-      </c>
-      <c r="D21">
+      <c r="C21">
         <v>11.88</v>
+      </c>
+      <c r="D21" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -1546,11 +1546,11 @@
       <c r="B22" t="s">
         <v>109</v>
       </c>
-      <c r="C22" t="s">
-        <v>120</v>
-      </c>
-      <c r="D22">
+      <c r="C22">
         <v>12.45</v>
+      </c>
+      <c r="D22" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1560,11 +1560,11 @@
       <c r="B23" t="s">
         <v>110</v>
       </c>
-      <c r="C23" t="s">
-        <v>120</v>
-      </c>
-      <c r="D23">
+      <c r="C23">
         <v>12.67</v>
+      </c>
+      <c r="D23" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1574,11 +1574,11 @@
       <c r="B24" t="s">
         <v>111</v>
       </c>
-      <c r="C24" t="s">
-        <v>120</v>
-      </c>
-      <c r="D24">
+      <c r="C24">
         <v>11.91</v>
+      </c>
+      <c r="D24" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1588,11 +1588,11 @@
       <c r="B25" t="s">
         <v>112</v>
       </c>
-      <c r="C25" t="s">
-        <v>120</v>
-      </c>
-      <c r="D25">
+      <c r="C25">
         <v>14.46</v>
+      </c>
+      <c r="D25" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1602,11 +1602,11 @@
       <c r="B26" t="s">
         <v>113</v>
       </c>
-      <c r="C26" t="s">
-        <v>120</v>
-      </c>
-      <c r="D26">
+      <c r="C26">
         <v>20.44</v>
+      </c>
+      <c r="D26" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1616,11 +1616,11 @@
       <c r="B27" t="s">
         <v>114</v>
       </c>
-      <c r="C27" t="s">
-        <v>120</v>
-      </c>
-      <c r="D27">
+      <c r="C27">
         <v>14.7</v>
+      </c>
+      <c r="D27" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1630,11 +1630,11 @@
       <c r="B28" t="s">
         <v>115</v>
       </c>
-      <c r="C28" t="s">
-        <v>120</v>
-      </c>
-      <c r="D28">
+      <c r="C28">
         <v>20.65</v>
+      </c>
+      <c r="D28" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1644,11 +1644,11 @@
       <c r="B29" t="s">
         <v>116</v>
       </c>
-      <c r="C29" t="s">
-        <v>120</v>
-      </c>
-      <c r="D29">
+      <c r="C29">
         <v>9.470000000000001</v>
+      </c>
+      <c r="D29" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1658,11 +1658,11 @@
       <c r="B30" t="s">
         <v>117</v>
       </c>
-      <c r="C30" t="s">
-        <v>120</v>
-      </c>
-      <c r="D30">
+      <c r="C30">
         <v>9.32</v>
+      </c>
+      <c r="D30" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1672,11 +1672,11 @@
       <c r="B31" t="s">
         <v>118</v>
       </c>
-      <c r="C31" t="s">
-        <v>120</v>
-      </c>
-      <c r="D31">
+      <c r="C31">
         <v>9.44</v>
+      </c>
+      <c r="D31" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1686,11 +1686,11 @@
       <c r="B32" t="s">
         <v>119</v>
       </c>
-      <c r="C32" t="s">
-        <v>120</v>
-      </c>
-      <c r="D32">
+      <c r="C32">
         <v>9.59</v>
+      </c>
+      <c r="D32" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -1722,10 +1722,10 @@
         <v>55</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1735,11 +1735,11 @@
       <c r="B2" t="s">
         <v>89</v>
       </c>
-      <c r="C2" t="s">
-        <v>120</v>
-      </c>
-      <c r="D2">
+      <c r="C2">
         <v>11.2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1749,11 +1749,11 @@
       <c r="B3" t="s">
         <v>90</v>
       </c>
-      <c r="C3" t="s">
-        <v>120</v>
-      </c>
-      <c r="D3">
+      <c r="C3">
         <v>16.52</v>
+      </c>
+      <c r="D3" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1763,11 +1763,11 @@
       <c r="B4" t="s">
         <v>91</v>
       </c>
-      <c r="C4" t="s">
-        <v>120</v>
-      </c>
-      <c r="D4">
+      <c r="C4">
         <v>16.67</v>
+      </c>
+      <c r="D4" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1777,11 +1777,11 @@
       <c r="B5" t="s">
         <v>92</v>
       </c>
-      <c r="C5" t="s">
-        <v>120</v>
-      </c>
-      <c r="D5">
+      <c r="C5">
         <v>5.58</v>
+      </c>
+      <c r="D5" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1791,11 +1791,11 @@
       <c r="B6" t="s">
         <v>93</v>
       </c>
-      <c r="C6" t="s">
-        <v>120</v>
-      </c>
-      <c r="D6">
+      <c r="C6">
         <v>5.73</v>
+      </c>
+      <c r="D6" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1805,11 +1805,11 @@
       <c r="B7" t="s">
         <v>94</v>
       </c>
-      <c r="C7" t="s">
-        <v>120</v>
-      </c>
-      <c r="D7">
+      <c r="C7">
         <v>5.7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1819,11 +1819,11 @@
       <c r="B8" t="s">
         <v>95</v>
       </c>
-      <c r="C8" t="s">
-        <v>120</v>
-      </c>
-      <c r="D8">
+      <c r="C8">
         <v>5.55</v>
+      </c>
+      <c r="D8" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1833,11 +1833,11 @@
       <c r="B9" t="s">
         <v>96</v>
       </c>
-      <c r="C9" t="s">
-        <v>120</v>
-      </c>
-      <c r="D9">
+      <c r="C9">
         <v>17.87</v>
+      </c>
+      <c r="D9" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1847,11 +1847,11 @@
       <c r="B10" t="s">
         <v>97</v>
       </c>
-      <c r="C10" t="s">
-        <v>120</v>
-      </c>
-      <c r="D10">
+      <c r="C10">
         <v>23.75</v>
+      </c>
+      <c r="D10" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1861,11 +1861,11 @@
       <c r="B11" t="s">
         <v>98</v>
       </c>
-      <c r="C11" t="s">
-        <v>120</v>
-      </c>
-      <c r="D11">
+      <c r="C11">
         <v>18.57</v>
+      </c>
+      <c r="D11" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -1875,11 +1875,11 @@
       <c r="B12" t="s">
         <v>99</v>
       </c>
-      <c r="C12" t="s">
-        <v>120</v>
-      </c>
-      <c r="D12">
+      <c r="C12">
         <v>24.03</v>
+      </c>
+      <c r="D12" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1889,11 +1889,11 @@
       <c r="B13" t="s">
         <v>100</v>
       </c>
-      <c r="C13" t="s">
-        <v>120</v>
-      </c>
-      <c r="D13">
+      <c r="C13">
         <v>10.9</v>
+      </c>
+      <c r="D13" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1903,11 +1903,11 @@
       <c r="B14" t="s">
         <v>101</v>
       </c>
-      <c r="C14" t="s">
-        <v>120</v>
-      </c>
-      <c r="D14">
+      <c r="C14">
         <v>11.37</v>
+      </c>
+      <c r="D14" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -1917,11 +1917,11 @@
       <c r="B15" t="s">
         <v>102</v>
       </c>
-      <c r="C15" t="s">
-        <v>120</v>
-      </c>
-      <c r="D15">
+      <c r="C15">
         <v>11.4</v>
+      </c>
+      <c r="D15" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1931,11 +1931,11 @@
       <c r="B16" t="s">
         <v>103</v>
       </c>
-      <c r="C16" t="s">
-        <v>120</v>
-      </c>
-      <c r="D16">
+      <c r="C16">
         <v>10.92</v>
+      </c>
+      <c r="D16" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1945,11 +1945,11 @@
       <c r="B17" t="s">
         <v>104</v>
       </c>
-      <c r="C17" t="s">
-        <v>120</v>
-      </c>
-      <c r="D17">
+      <c r="C17">
         <v>18.81</v>
+      </c>
+      <c r="D17" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1959,11 +1959,11 @@
       <c r="B18" t="s">
         <v>105</v>
       </c>
-      <c r="C18" t="s">
-        <v>120</v>
-      </c>
-      <c r="D18">
+      <c r="C18">
         <v>25.54</v>
+      </c>
+      <c r="D18" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1973,11 +1973,11 @@
       <c r="B19" t="s">
         <v>106</v>
       </c>
-      <c r="C19" t="s">
-        <v>120</v>
-      </c>
-      <c r="D19">
+      <c r="C19">
         <v>19.47</v>
+      </c>
+      <c r="D19" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1987,11 +1987,11 @@
       <c r="B20" t="s">
         <v>107</v>
       </c>
-      <c r="C20" t="s">
-        <v>120</v>
-      </c>
-      <c r="D20">
+      <c r="C20">
         <v>25.75</v>
+      </c>
+      <c r="D20" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -2001,11 +2001,11 @@
       <c r="B21" t="s">
         <v>108</v>
       </c>
-      <c r="C21" t="s">
-        <v>120</v>
-      </c>
-      <c r="D21">
+      <c r="C21">
         <v>11.87</v>
+      </c>
+      <c r="D21" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -2015,11 +2015,11 @@
       <c r="B22" t="s">
         <v>109</v>
       </c>
-      <c r="C22" t="s">
-        <v>120</v>
-      </c>
-      <c r="D22">
+      <c r="C22">
         <v>12.45</v>
+      </c>
+      <c r="D22" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -2029,11 +2029,11 @@
       <c r="B23" t="s">
         <v>110</v>
       </c>
-      <c r="C23" t="s">
-        <v>120</v>
-      </c>
-      <c r="D23">
+      <c r="C23">
         <v>12.67</v>
+      </c>
+      <c r="D23" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -2043,11 +2043,11 @@
       <c r="B24" t="s">
         <v>111</v>
       </c>
-      <c r="C24" t="s">
-        <v>120</v>
-      </c>
-      <c r="D24">
+      <c r="C24">
         <v>11.91</v>
+      </c>
+      <c r="D24" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -2057,11 +2057,11 @@
       <c r="B25" t="s">
         <v>112</v>
       </c>
-      <c r="C25" t="s">
-        <v>120</v>
-      </c>
-      <c r="D25">
+      <c r="C25">
         <v>14.45</v>
+      </c>
+      <c r="D25" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -2071,11 +2071,11 @@
       <c r="B26" t="s">
         <v>113</v>
       </c>
-      <c r="C26" t="s">
-        <v>120</v>
-      </c>
-      <c r="D26">
+      <c r="C26">
         <v>20.48</v>
+      </c>
+      <c r="D26" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -2085,11 +2085,11 @@
       <c r="B27" t="s">
         <v>114</v>
       </c>
-      <c r="C27" t="s">
-        <v>120</v>
-      </c>
-      <c r="D27">
+      <c r="C27">
         <v>14.7</v>
+      </c>
+      <c r="D27" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -2099,11 +2099,11 @@
       <c r="B28" t="s">
         <v>115</v>
       </c>
-      <c r="C28" t="s">
-        <v>120</v>
-      </c>
-      <c r="D28">
+      <c r="C28">
         <v>20.67</v>
+      </c>
+      <c r="D28" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -2113,11 +2113,11 @@
       <c r="B29" t="s">
         <v>116</v>
       </c>
-      <c r="C29" t="s">
-        <v>120</v>
-      </c>
-      <c r="D29">
+      <c r="C29">
         <v>9.470000000000001</v>
+      </c>
+      <c r="D29" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -2127,11 +2127,11 @@
       <c r="B30" t="s">
         <v>117</v>
       </c>
-      <c r="C30" t="s">
-        <v>120</v>
-      </c>
-      <c r="D30">
+      <c r="C30">
         <v>9.32</v>
+      </c>
+      <c r="D30" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -2141,11 +2141,11 @@
       <c r="B31" t="s">
         <v>118</v>
       </c>
-      <c r="C31" t="s">
-        <v>120</v>
-      </c>
-      <c r="D31">
+      <c r="C31">
         <v>9.44</v>
+      </c>
+      <c r="D31" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -2155,11 +2155,11 @@
       <c r="B32" t="s">
         <v>119</v>
       </c>
-      <c r="C32" t="s">
-        <v>120</v>
-      </c>
-      <c r="D32">
+      <c r="C32">
         <v>9.59</v>
+      </c>
+      <c r="D32" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -2191,10 +2191,10 @@
         <v>55</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -2204,11 +2204,11 @@
       <c r="B2" t="s">
         <v>89</v>
       </c>
-      <c r="C2" t="s">
-        <v>120</v>
-      </c>
-      <c r="D2">
+      <c r="C2">
         <v>11.2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -2218,11 +2218,11 @@
       <c r="B3" t="s">
         <v>90</v>
       </c>
-      <c r="C3" t="s">
-        <v>120</v>
-      </c>
-      <c r="D3">
+      <c r="C3">
         <v>16.52</v>
+      </c>
+      <c r="D3" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -2232,11 +2232,11 @@
       <c r="B4" t="s">
         <v>91</v>
       </c>
-      <c r="C4" t="s">
-        <v>120</v>
-      </c>
-      <c r="D4">
+      <c r="C4">
         <v>16.67</v>
+      </c>
+      <c r="D4" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -2246,11 +2246,11 @@
       <c r="B5" t="s">
         <v>92</v>
       </c>
-      <c r="C5" t="s">
-        <v>120</v>
-      </c>
-      <c r="D5">
+      <c r="C5">
         <v>5.58</v>
+      </c>
+      <c r="D5" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -2260,11 +2260,11 @@
       <c r="B6" t="s">
         <v>93</v>
       </c>
-      <c r="C6" t="s">
-        <v>120</v>
-      </c>
-      <c r="D6">
+      <c r="C6">
         <v>5.73</v>
+      </c>
+      <c r="D6" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -2274,11 +2274,11 @@
       <c r="B7" t="s">
         <v>94</v>
       </c>
-      <c r="C7" t="s">
-        <v>120</v>
-      </c>
-      <c r="D7">
+      <c r="C7">
         <v>5.7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -2288,11 +2288,11 @@
       <c r="B8" t="s">
         <v>95</v>
       </c>
-      <c r="C8" t="s">
-        <v>120</v>
-      </c>
-      <c r="D8">
+      <c r="C8">
         <v>5.54</v>
+      </c>
+      <c r="D8" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -2302,11 +2302,11 @@
       <c r="B9" t="s">
         <v>96</v>
       </c>
-      <c r="C9" t="s">
-        <v>120</v>
-      </c>
-      <c r="D9">
+      <c r="C9">
         <v>17.87</v>
+      </c>
+      <c r="D9" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -2316,11 +2316,11 @@
       <c r="B10" t="s">
         <v>97</v>
       </c>
-      <c r="C10" t="s">
-        <v>120</v>
-      </c>
-      <c r="D10">
+      <c r="C10">
         <v>23.77</v>
+      </c>
+      <c r="D10" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -2330,11 +2330,11 @@
       <c r="B11" t="s">
         <v>98</v>
       </c>
-      <c r="C11" t="s">
-        <v>120</v>
-      </c>
-      <c r="D11">
+      <c r="C11">
         <v>18.57</v>
+      </c>
+      <c r="D11" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -2344,11 +2344,11 @@
       <c r="B12" t="s">
         <v>99</v>
       </c>
-      <c r="C12" t="s">
-        <v>120</v>
-      </c>
-      <c r="D12">
+      <c r="C12">
         <v>24.03</v>
+      </c>
+      <c r="D12" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -2358,11 +2358,11 @@
       <c r="B13" t="s">
         <v>100</v>
       </c>
-      <c r="C13" t="s">
-        <v>120</v>
-      </c>
-      <c r="D13">
+      <c r="C13">
         <v>10.89</v>
+      </c>
+      <c r="D13" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -2372,11 +2372,11 @@
       <c r="B14" t="s">
         <v>101</v>
       </c>
-      <c r="C14" t="s">
-        <v>120</v>
-      </c>
-      <c r="D14">
+      <c r="C14">
         <v>11.37</v>
+      </c>
+      <c r="D14" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -2386,11 +2386,11 @@
       <c r="B15" t="s">
         <v>102</v>
       </c>
-      <c r="C15" t="s">
-        <v>120</v>
-      </c>
-      <c r="D15">
+      <c r="C15">
         <v>11.4</v>
+      </c>
+      <c r="D15" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -2400,11 +2400,11 @@
       <c r="B16" t="s">
         <v>103</v>
       </c>
-      <c r="C16" t="s">
-        <v>120</v>
-      </c>
-      <c r="D16">
+      <c r="C16">
         <v>10.92</v>
+      </c>
+      <c r="D16" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -2414,11 +2414,11 @@
       <c r="B17" t="s">
         <v>104</v>
       </c>
-      <c r="C17" t="s">
-        <v>120</v>
-      </c>
-      <c r="D17">
+      <c r="C17">
         <v>18.81</v>
+      </c>
+      <c r="D17" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -2428,11 +2428,11 @@
       <c r="B18" t="s">
         <v>105</v>
       </c>
-      <c r="C18" t="s">
-        <v>120</v>
-      </c>
-      <c r="D18">
+      <c r="C18">
         <v>25.54</v>
+      </c>
+      <c r="D18" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -2442,11 +2442,11 @@
       <c r="B19" t="s">
         <v>106</v>
       </c>
-      <c r="C19" t="s">
-        <v>120</v>
-      </c>
-      <c r="D19">
+      <c r="C19">
         <v>19.47</v>
+      </c>
+      <c r="D19" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -2456,11 +2456,11 @@
       <c r="B20" t="s">
         <v>107</v>
       </c>
-      <c r="C20" t="s">
-        <v>120</v>
-      </c>
-      <c r="D20">
+      <c r="C20">
         <v>25.75</v>
+      </c>
+      <c r="D20" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -2470,11 +2470,11 @@
       <c r="B21" t="s">
         <v>108</v>
       </c>
-      <c r="C21" t="s">
-        <v>120</v>
-      </c>
-      <c r="D21">
+      <c r="C21">
         <v>11.87</v>
+      </c>
+      <c r="D21" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -2484,11 +2484,11 @@
       <c r="B22" t="s">
         <v>109</v>
       </c>
-      <c r="C22" t="s">
-        <v>120</v>
-      </c>
-      <c r="D22">
+      <c r="C22">
         <v>12.47</v>
+      </c>
+      <c r="D22" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -2498,11 +2498,11 @@
       <c r="B23" t="s">
         <v>110</v>
       </c>
-      <c r="C23" t="s">
-        <v>120</v>
-      </c>
-      <c r="D23">
+      <c r="C23">
         <v>12.67</v>
+      </c>
+      <c r="D23" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -2512,11 +2512,11 @@
       <c r="B24" t="s">
         <v>111</v>
       </c>
-      <c r="C24" t="s">
-        <v>120</v>
-      </c>
-      <c r="D24">
+      <c r="C24">
         <v>11.91</v>
+      </c>
+      <c r="D24" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -2526,11 +2526,11 @@
       <c r="B25" t="s">
         <v>112</v>
       </c>
-      <c r="C25" t="s">
-        <v>120</v>
-      </c>
-      <c r="D25">
+      <c r="C25">
         <v>14.45</v>
+      </c>
+      <c r="D25" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -2540,11 +2540,11 @@
       <c r="B26" t="s">
         <v>113</v>
       </c>
-      <c r="C26" t="s">
-        <v>120</v>
-      </c>
-      <c r="D26">
+      <c r="C26">
         <v>20.48</v>
+      </c>
+      <c r="D26" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -2554,11 +2554,11 @@
       <c r="B27" t="s">
         <v>114</v>
       </c>
-      <c r="C27" t="s">
-        <v>120</v>
-      </c>
-      <c r="D27">
+      <c r="C27">
         <v>14.7</v>
+      </c>
+      <c r="D27" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -2568,11 +2568,11 @@
       <c r="B28" t="s">
         <v>115</v>
       </c>
-      <c r="C28" t="s">
-        <v>120</v>
-      </c>
-      <c r="D28">
+      <c r="C28">
         <v>20.67</v>
+      </c>
+      <c r="D28" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -2582,11 +2582,11 @@
       <c r="B29" t="s">
         <v>116</v>
       </c>
-      <c r="C29" t="s">
-        <v>120</v>
-      </c>
-      <c r="D29">
+      <c r="C29">
         <v>9.470000000000001</v>
+      </c>
+      <c r="D29" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -2596,11 +2596,11 @@
       <c r="B30" t="s">
         <v>117</v>
       </c>
-      <c r="C30" t="s">
-        <v>120</v>
-      </c>
-      <c r="D30">
+      <c r="C30">
         <v>9.32</v>
+      </c>
+      <c r="D30" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -2610,11 +2610,11 @@
       <c r="B31" t="s">
         <v>118</v>
       </c>
-      <c r="C31" t="s">
-        <v>120</v>
-      </c>
-      <c r="D31">
+      <c r="C31">
         <v>9.44</v>
+      </c>
+      <c r="D31" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -2624,11 +2624,11 @@
       <c r="B32" t="s">
         <v>119</v>
       </c>
-      <c r="C32" t="s">
-        <v>120</v>
-      </c>
-      <c r="D32">
+      <c r="C32">
         <v>9.59</v>
+      </c>
+      <c r="D32" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -2811,10 +2811,10 @@
         <v>55</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -2824,11 +2824,11 @@
       <c r="B2" t="s">
         <v>89</v>
       </c>
-      <c r="C2" t="s">
-        <v>120</v>
-      </c>
-      <c r="D2">
+      <c r="C2">
         <v>11.21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -2838,11 +2838,11 @@
       <c r="B3" t="s">
         <v>90</v>
       </c>
-      <c r="C3" t="s">
-        <v>120</v>
-      </c>
-      <c r="D3">
+      <c r="C3">
         <v>16.33</v>
+      </c>
+      <c r="D3" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -2852,11 +2852,11 @@
       <c r="B4" t="s">
         <v>91</v>
       </c>
-      <c r="C4" t="s">
-        <v>120</v>
-      </c>
-      <c r="D4">
+      <c r="C4">
         <v>16.52</v>
+      </c>
+      <c r="D4" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -2866,11 +2866,11 @@
       <c r="B5" t="s">
         <v>92</v>
       </c>
-      <c r="C5" t="s">
-        <v>120</v>
-      </c>
-      <c r="D5">
+      <c r="C5">
         <v>5.57</v>
+      </c>
+      <c r="D5" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -2880,11 +2880,11 @@
       <c r="B6" t="s">
         <v>93</v>
       </c>
-      <c r="C6" t="s">
-        <v>120</v>
-      </c>
-      <c r="D6">
+      <c r="C6">
         <v>5.76</v>
+      </c>
+      <c r="D6" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -2894,11 +2894,11 @@
       <c r="B7" t="s">
         <v>94</v>
       </c>
-      <c r="C7" t="s">
-        <v>120</v>
-      </c>
-      <c r="D7">
+      <c r="C7">
         <v>5.65</v>
+      </c>
+      <c r="D7" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -2908,11 +2908,11 @@
       <c r="B8" t="s">
         <v>95</v>
       </c>
-      <c r="C8" t="s">
-        <v>120</v>
-      </c>
-      <c r="D8">
+      <c r="C8">
         <v>5.56</v>
+      </c>
+      <c r="D8" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -2922,11 +2922,11 @@
       <c r="B9" t="s">
         <v>96</v>
       </c>
-      <c r="C9" t="s">
-        <v>120</v>
-      </c>
-      <c r="D9">
+      <c r="C9">
         <v>17.87</v>
+      </c>
+      <c r="D9" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -2936,11 +2936,11 @@
       <c r="B10" t="s">
         <v>97</v>
       </c>
-      <c r="C10" t="s">
-        <v>120</v>
-      </c>
-      <c r="D10">
+      <c r="C10">
         <v>23.69</v>
+      </c>
+      <c r="D10" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -2950,11 +2950,11 @@
       <c r="B11" t="s">
         <v>98</v>
       </c>
-      <c r="C11" t="s">
-        <v>120</v>
-      </c>
-      <c r="D11">
+      <c r="C11">
         <v>18.61</v>
+      </c>
+      <c r="D11" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -2964,11 +2964,11 @@
       <c r="B12" t="s">
         <v>99</v>
       </c>
-      <c r="C12" t="s">
-        <v>120</v>
-      </c>
-      <c r="D12">
+      <c r="C12">
         <v>23.88</v>
+      </c>
+      <c r="D12" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -2978,11 +2978,11 @@
       <c r="B13" t="s">
         <v>100</v>
       </c>
-      <c r="C13" t="s">
-        <v>120</v>
-      </c>
-      <c r="D13">
+      <c r="C13">
         <v>10.95</v>
+      </c>
+      <c r="D13" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -2992,11 +2992,11 @@
       <c r="B14" t="s">
         <v>101</v>
       </c>
-      <c r="C14" t="s">
-        <v>120</v>
-      </c>
-      <c r="D14">
+      <c r="C14">
         <v>11.38</v>
+      </c>
+      <c r="D14" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -3006,11 +3006,11 @@
       <c r="B15" t="s">
         <v>102</v>
       </c>
-      <c r="C15" t="s">
-        <v>120</v>
-      </c>
-      <c r="D15">
+      <c r="C15">
         <v>11.39</v>
+      </c>
+      <c r="D15" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -3020,11 +3020,11 @@
       <c r="B16" t="s">
         <v>103</v>
       </c>
-      <c r="C16" t="s">
-        <v>120</v>
-      </c>
-      <c r="D16">
+      <c r="C16">
         <v>10.94</v>
+      </c>
+      <c r="D16" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -3034,11 +3034,11 @@
       <c r="B17" t="s">
         <v>104</v>
       </c>
-      <c r="C17" t="s">
-        <v>120</v>
-      </c>
-      <c r="D17">
+      <c r="C17">
         <v>18.82</v>
+      </c>
+      <c r="D17" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -3048,11 +3048,11 @@
       <c r="B18" t="s">
         <v>105</v>
       </c>
-      <c r="C18" t="s">
-        <v>120</v>
-      </c>
-      <c r="D18">
+      <c r="C18">
         <v>25.37</v>
+      </c>
+      <c r="D18" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -3062,11 +3062,11 @@
       <c r="B19" t="s">
         <v>106</v>
       </c>
-      <c r="C19" t="s">
-        <v>120</v>
-      </c>
-      <c r="D19">
+      <c r="C19">
         <v>19.5</v>
+      </c>
+      <c r="D19" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -3076,11 +3076,11 @@
       <c r="B20" t="s">
         <v>107</v>
       </c>
-      <c r="C20" t="s">
-        <v>120</v>
-      </c>
-      <c r="D20">
+      <c r="C20">
         <v>25.58</v>
+      </c>
+      <c r="D20" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -3090,11 +3090,11 @@
       <c r="B21" t="s">
         <v>108</v>
       </c>
-      <c r="C21" t="s">
-        <v>120</v>
-      </c>
-      <c r="D21">
+      <c r="C21">
         <v>11.91</v>
+      </c>
+      <c r="D21" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -3104,11 +3104,11 @@
       <c r="B22" t="s">
         <v>109</v>
       </c>
-      <c r="C22" t="s">
-        <v>120</v>
-      </c>
-      <c r="D22">
+      <c r="C22">
         <v>12.49</v>
+      </c>
+      <c r="D22" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -3118,11 +3118,11 @@
       <c r="B23" t="s">
         <v>110</v>
       </c>
-      <c r="C23" t="s">
-        <v>120</v>
-      </c>
-      <c r="D23">
+      <c r="C23">
         <v>12.67</v>
+      </c>
+      <c r="D23" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -3132,11 +3132,11 @@
       <c r="B24" t="s">
         <v>111</v>
       </c>
-      <c r="C24" t="s">
-        <v>120</v>
-      </c>
-      <c r="D24">
+      <c r="C24">
         <v>11.93</v>
+      </c>
+      <c r="D24" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -3146,11 +3146,11 @@
       <c r="B25" t="s">
         <v>112</v>
       </c>
-      <c r="C25" t="s">
-        <v>120</v>
-      </c>
-      <c r="D25">
+      <c r="C25">
         <v>14.45</v>
+      </c>
+      <c r="D25" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -3160,11 +3160,11 @@
       <c r="B26" t="s">
         <v>113</v>
       </c>
-      <c r="C26" t="s">
-        <v>120</v>
-      </c>
-      <c r="D26">
+      <c r="C26">
         <v>20.3</v>
+      </c>
+      <c r="D26" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -3174,11 +3174,11 @@
       <c r="B27" t="s">
         <v>114</v>
       </c>
-      <c r="C27" t="s">
-        <v>120</v>
-      </c>
-      <c r="D27">
+      <c r="C27">
         <v>14.67</v>
+      </c>
+      <c r="D27" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -3188,11 +3188,11 @@
       <c r="B28" t="s">
         <v>115</v>
       </c>
-      <c r="C28" t="s">
-        <v>120</v>
-      </c>
-      <c r="D28">
+      <c r="C28">
         <v>20.42</v>
+      </c>
+      <c r="D28" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -3202,11 +3202,11 @@
       <c r="B29" t="s">
         <v>116</v>
       </c>
-      <c r="C29" t="s">
-        <v>120</v>
-      </c>
-      <c r="D29">
+      <c r="C29">
         <v>9.470000000000001</v>
+      </c>
+      <c r="D29" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -3216,11 +3216,11 @@
       <c r="B30" t="s">
         <v>117</v>
       </c>
-      <c r="C30" t="s">
-        <v>120</v>
-      </c>
-      <c r="D30">
+      <c r="C30">
         <v>9.33</v>
+      </c>
+      <c r="D30" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -3230,11 +3230,11 @@
       <c r="B31" t="s">
         <v>118</v>
       </c>
-      <c r="C31" t="s">
-        <v>120</v>
-      </c>
-      <c r="D31">
+      <c r="C31">
         <v>9.460000000000001</v>
+      </c>
+      <c r="D31" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -3244,11 +3244,11 @@
       <c r="B32" t="s">
         <v>119</v>
       </c>
-      <c r="C32" t="s">
-        <v>120</v>
-      </c>
-      <c r="D32">
+      <c r="C32">
         <v>9.58</v>
+      </c>
+      <c r="D32" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -3280,10 +3280,10 @@
         <v>55</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -3293,11 +3293,11 @@
       <c r="B2" t="s">
         <v>89</v>
       </c>
-      <c r="C2" t="s">
-        <v>120</v>
-      </c>
-      <c r="D2">
+      <c r="C2">
         <v>11.21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -3307,11 +3307,11 @@
       <c r="B3" t="s">
         <v>90</v>
       </c>
-      <c r="C3" t="s">
-        <v>120</v>
-      </c>
-      <c r="D3">
+      <c r="C3">
         <v>16.33</v>
+      </c>
+      <c r="D3" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -3321,11 +3321,11 @@
       <c r="B4" t="s">
         <v>91</v>
       </c>
-      <c r="C4" t="s">
-        <v>120</v>
-      </c>
-      <c r="D4">
+      <c r="C4">
         <v>16.56</v>
+      </c>
+      <c r="D4" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -3335,11 +3335,11 @@
       <c r="B5" t="s">
         <v>92</v>
       </c>
-      <c r="C5" t="s">
-        <v>120</v>
-      </c>
-      <c r="D5">
+      <c r="C5">
         <v>5.57</v>
+      </c>
+      <c r="D5" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -3349,11 +3349,11 @@
       <c r="B6" t="s">
         <v>93</v>
       </c>
-      <c r="C6" t="s">
-        <v>120</v>
-      </c>
-      <c r="D6">
+      <c r="C6">
         <v>5.76</v>
+      </c>
+      <c r="D6" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -3363,11 +3363,11 @@
       <c r="B7" t="s">
         <v>94</v>
       </c>
-      <c r="C7" t="s">
-        <v>120</v>
-      </c>
-      <c r="D7">
+      <c r="C7">
         <v>5.66</v>
+      </c>
+      <c r="D7" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -3377,11 +3377,11 @@
       <c r="B8" t="s">
         <v>95</v>
       </c>
-      <c r="C8" t="s">
-        <v>120</v>
-      </c>
-      <c r="D8">
+      <c r="C8">
         <v>5.57</v>
+      </c>
+      <c r="D8" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -3391,11 +3391,11 @@
       <c r="B9" t="s">
         <v>96</v>
       </c>
-      <c r="C9" t="s">
-        <v>120</v>
-      </c>
-      <c r="D9">
+      <c r="C9">
         <v>17.87</v>
+      </c>
+      <c r="D9" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -3405,11 +3405,11 @@
       <c r="B10" t="s">
         <v>97</v>
       </c>
-      <c r="C10" t="s">
-        <v>120</v>
-      </c>
-      <c r="D10">
+      <c r="C10">
         <v>23.73</v>
+      </c>
+      <c r="D10" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -3419,11 +3419,11 @@
       <c r="B11" t="s">
         <v>98</v>
       </c>
-      <c r="C11" t="s">
-        <v>120</v>
-      </c>
-      <c r="D11">
+      <c r="C11">
         <v>18.6</v>
+      </c>
+      <c r="D11" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -3433,11 +3433,11 @@
       <c r="B12" t="s">
         <v>99</v>
       </c>
-      <c r="C12" t="s">
-        <v>120</v>
-      </c>
-      <c r="D12">
+      <c r="C12">
         <v>23.9</v>
+      </c>
+      <c r="D12" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -3447,11 +3447,11 @@
       <c r="B13" t="s">
         <v>100</v>
       </c>
-      <c r="C13" t="s">
-        <v>120</v>
-      </c>
-      <c r="D13">
+      <c r="C13">
         <v>10.95</v>
+      </c>
+      <c r="D13" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -3461,11 +3461,11 @@
       <c r="B14" t="s">
         <v>101</v>
       </c>
-      <c r="C14" t="s">
-        <v>120</v>
-      </c>
-      <c r="D14">
+      <c r="C14">
         <v>11.37</v>
+      </c>
+      <c r="D14" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -3475,11 +3475,11 @@
       <c r="B15" t="s">
         <v>102</v>
       </c>
-      <c r="C15" t="s">
-        <v>120</v>
-      </c>
-      <c r="D15">
+      <c r="C15">
         <v>11.4</v>
+      </c>
+      <c r="D15" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -3489,11 +3489,11 @@
       <c r="B16" t="s">
         <v>103</v>
       </c>
-      <c r="C16" t="s">
-        <v>120</v>
-      </c>
-      <c r="D16">
+      <c r="C16">
         <v>10.95</v>
+      </c>
+      <c r="D16" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -3503,11 +3503,11 @@
       <c r="B17" t="s">
         <v>104</v>
       </c>
-      <c r="C17" t="s">
-        <v>120</v>
-      </c>
-      <c r="D17">
+      <c r="C17">
         <v>18.8</v>
+      </c>
+      <c r="D17" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -3517,11 +3517,11 @@
       <c r="B18" t="s">
         <v>105</v>
       </c>
-      <c r="C18" t="s">
-        <v>120</v>
-      </c>
-      <c r="D18">
+      <c r="C18">
         <v>25.37</v>
+      </c>
+      <c r="D18" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -3531,11 +3531,11 @@
       <c r="B19" t="s">
         <v>106</v>
       </c>
-      <c r="C19" t="s">
-        <v>120</v>
-      </c>
-      <c r="D19">
+      <c r="C19">
         <v>19.5</v>
+      </c>
+      <c r="D19" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -3545,11 +3545,11 @@
       <c r="B20" t="s">
         <v>107</v>
       </c>
-      <c r="C20" t="s">
-        <v>120</v>
-      </c>
-      <c r="D20">
+      <c r="C20">
         <v>25.61</v>
+      </c>
+      <c r="D20" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -3559,11 +3559,11 @@
       <c r="B21" t="s">
         <v>108</v>
       </c>
-      <c r="C21" t="s">
-        <v>120</v>
-      </c>
-      <c r="D21">
+      <c r="C21">
         <v>11.89</v>
+      </c>
+      <c r="D21" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -3573,11 +3573,11 @@
       <c r="B22" t="s">
         <v>109</v>
       </c>
-      <c r="C22" t="s">
-        <v>120</v>
-      </c>
-      <c r="D22">
+      <c r="C22">
         <v>12.47</v>
+      </c>
+      <c r="D22" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -3587,11 +3587,11 @@
       <c r="B23" t="s">
         <v>110</v>
       </c>
-      <c r="C23" t="s">
-        <v>120</v>
-      </c>
-      <c r="D23">
+      <c r="C23">
         <v>12.67</v>
+      </c>
+      <c r="D23" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -3601,11 +3601,11 @@
       <c r="B24" t="s">
         <v>111</v>
       </c>
-      <c r="C24" t="s">
-        <v>120</v>
-      </c>
-      <c r="D24">
+      <c r="C24">
         <v>11.93</v>
+      </c>
+      <c r="D24" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -3615,11 +3615,11 @@
       <c r="B25" t="s">
         <v>112</v>
       </c>
-      <c r="C25" t="s">
-        <v>120</v>
-      </c>
-      <c r="D25">
+      <c r="C25">
         <v>14.45</v>
+      </c>
+      <c r="D25" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -3629,11 +3629,11 @@
       <c r="B26" t="s">
         <v>113</v>
       </c>
-      <c r="C26" t="s">
-        <v>120</v>
-      </c>
-      <c r="D26">
+      <c r="C26">
         <v>20.32</v>
+      </c>
+      <c r="D26" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -3643,11 +3643,11 @@
       <c r="B27" t="s">
         <v>114</v>
       </c>
-      <c r="C27" t="s">
-        <v>120</v>
-      </c>
-      <c r="D27">
+      <c r="C27">
         <v>14.67</v>
+      </c>
+      <c r="D27" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -3657,11 +3657,11 @@
       <c r="B28" t="s">
         <v>115</v>
       </c>
-      <c r="C28" t="s">
-        <v>120</v>
-      </c>
-      <c r="D28">
+      <c r="C28">
         <v>20.48</v>
+      </c>
+      <c r="D28" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -3671,11 +3671,11 @@
       <c r="B29" t="s">
         <v>116</v>
       </c>
-      <c r="C29" t="s">
-        <v>120</v>
-      </c>
-      <c r="D29">
+      <c r="C29">
         <v>9.460000000000001</v>
+      </c>
+      <c r="D29" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -3685,11 +3685,11 @@
       <c r="B30" t="s">
         <v>117</v>
       </c>
-      <c r="C30" t="s">
-        <v>120</v>
-      </c>
-      <c r="D30">
+      <c r="C30">
         <v>9.33</v>
+      </c>
+      <c r="D30" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -3699,11 +3699,11 @@
       <c r="B31" t="s">
         <v>118</v>
       </c>
-      <c r="C31" t="s">
-        <v>120</v>
-      </c>
-      <c r="D31">
+      <c r="C31">
         <v>9.449999999999999</v>
+      </c>
+      <c r="D31" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -3713,11 +3713,11 @@
       <c r="B32" t="s">
         <v>119</v>
       </c>
-      <c r="C32" t="s">
-        <v>120</v>
-      </c>
-      <c r="D32">
+      <c r="C32">
         <v>9.59</v>
+      </c>
+      <c r="D32" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -3749,10 +3749,10 @@
         <v>55</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -3762,11 +3762,11 @@
       <c r="B2" t="s">
         <v>89</v>
       </c>
-      <c r="C2" t="s">
-        <v>120</v>
-      </c>
-      <c r="D2">
+      <c r="C2">
         <v>11.2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -3776,11 +3776,11 @@
       <c r="B3" t="s">
         <v>90</v>
       </c>
-      <c r="C3" t="s">
-        <v>120</v>
-      </c>
-      <c r="D3">
+      <c r="C3">
         <v>16.42</v>
+      </c>
+      <c r="D3" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -3790,11 +3790,11 @@
       <c r="B4" t="s">
         <v>91</v>
       </c>
-      <c r="C4" t="s">
-        <v>120</v>
-      </c>
-      <c r="D4">
+      <c r="C4">
         <v>16.59</v>
+      </c>
+      <c r="D4" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -3804,11 +3804,11 @@
       <c r="B5" t="s">
         <v>92</v>
       </c>
-      <c r="C5" t="s">
-        <v>120</v>
-      </c>
-      <c r="D5">
+      <c r="C5">
         <v>5.57</v>
+      </c>
+      <c r="D5" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -3818,11 +3818,11 @@
       <c r="B6" t="s">
         <v>93</v>
       </c>
-      <c r="C6" t="s">
-        <v>120</v>
-      </c>
-      <c r="D6">
+      <c r="C6">
         <v>5.76</v>
+      </c>
+      <c r="D6" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -3832,11 +3832,11 @@
       <c r="B7" t="s">
         <v>94</v>
       </c>
-      <c r="C7" t="s">
-        <v>120</v>
-      </c>
-      <c r="D7">
+      <c r="C7">
         <v>5.67</v>
+      </c>
+      <c r="D7" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -3846,11 +3846,11 @@
       <c r="B8" t="s">
         <v>95</v>
       </c>
-      <c r="C8" t="s">
-        <v>120</v>
-      </c>
-      <c r="D8">
+      <c r="C8">
         <v>5.58</v>
+      </c>
+      <c r="D8" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -3860,11 +3860,11 @@
       <c r="B9" t="s">
         <v>96</v>
       </c>
-      <c r="C9" t="s">
-        <v>120</v>
-      </c>
-      <c r="D9">
+      <c r="C9">
         <v>17.87</v>
+      </c>
+      <c r="D9" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -3874,11 +3874,11 @@
       <c r="B10" t="s">
         <v>97</v>
       </c>
-      <c r="C10" t="s">
-        <v>120</v>
-      </c>
-      <c r="D10">
+      <c r="C10">
         <v>23.73</v>
+      </c>
+      <c r="D10" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -3888,11 +3888,11 @@
       <c r="B11" t="s">
         <v>98</v>
       </c>
-      <c r="C11" t="s">
-        <v>120</v>
-      </c>
-      <c r="D11">
+      <c r="C11">
         <v>18.58</v>
+      </c>
+      <c r="D11" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -3902,11 +3902,11 @@
       <c r="B12" t="s">
         <v>99</v>
       </c>
-      <c r="C12" t="s">
-        <v>120</v>
-      </c>
-      <c r="D12">
+      <c r="C12">
         <v>23.9</v>
+      </c>
+      <c r="D12" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -3916,11 +3916,11 @@
       <c r="B13" t="s">
         <v>100</v>
       </c>
-      <c r="C13" t="s">
-        <v>120</v>
-      </c>
-      <c r="D13">
+      <c r="C13">
         <v>10.94</v>
+      </c>
+      <c r="D13" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -3930,11 +3930,11 @@
       <c r="B14" t="s">
         <v>101</v>
       </c>
-      <c r="C14" t="s">
-        <v>120</v>
-      </c>
-      <c r="D14">
+      <c r="C14">
         <v>11.37</v>
+      </c>
+      <c r="D14" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -3944,11 +3944,11 @@
       <c r="B15" t="s">
         <v>102</v>
       </c>
-      <c r="C15" t="s">
-        <v>120</v>
-      </c>
-      <c r="D15">
+      <c r="C15">
         <v>11.39</v>
+      </c>
+      <c r="D15" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -3958,11 +3958,11 @@
       <c r="B16" t="s">
         <v>103</v>
       </c>
-      <c r="C16" t="s">
-        <v>120</v>
-      </c>
-      <c r="D16">
+      <c r="C16">
         <v>10.95</v>
+      </c>
+      <c r="D16" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -3972,11 +3972,11 @@
       <c r="B17" t="s">
         <v>104</v>
       </c>
-      <c r="C17" t="s">
-        <v>120</v>
-      </c>
-      <c r="D17">
+      <c r="C17">
         <v>18.8</v>
+      </c>
+      <c r="D17" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -3986,11 +3986,11 @@
       <c r="B18" t="s">
         <v>105</v>
       </c>
-      <c r="C18" t="s">
-        <v>120</v>
-      </c>
-      <c r="D18">
+      <c r="C18">
         <v>25.48</v>
+      </c>
+      <c r="D18" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -4000,11 +4000,11 @@
       <c r="B19" t="s">
         <v>106</v>
       </c>
-      <c r="C19" t="s">
-        <v>120</v>
-      </c>
-      <c r="D19">
+      <c r="C19">
         <v>19.5</v>
+      </c>
+      <c r="D19" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -4014,11 +4014,11 @@
       <c r="B20" t="s">
         <v>107</v>
       </c>
-      <c r="C20" t="s">
-        <v>120</v>
-      </c>
-      <c r="D20">
+      <c r="C20">
         <v>25.63</v>
+      </c>
+      <c r="D20" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -4028,11 +4028,11 @@
       <c r="B21" t="s">
         <v>108</v>
       </c>
-      <c r="C21" t="s">
-        <v>120</v>
-      </c>
-      <c r="D21">
+      <c r="C21">
         <v>11.89</v>
+      </c>
+      <c r="D21" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -4042,11 +4042,11 @@
       <c r="B22" t="s">
         <v>109</v>
       </c>
-      <c r="C22" t="s">
-        <v>120</v>
-      </c>
-      <c r="D22">
+      <c r="C22">
         <v>12.45</v>
+      </c>
+      <c r="D22" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -4056,11 +4056,11 @@
       <c r="B23" t="s">
         <v>110</v>
       </c>
-      <c r="C23" t="s">
-        <v>120</v>
-      </c>
-      <c r="D23">
+      <c r="C23">
         <v>12.68</v>
+      </c>
+      <c r="D23" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -4070,11 +4070,11 @@
       <c r="B24" t="s">
         <v>111</v>
       </c>
-      <c r="C24" t="s">
-        <v>120</v>
-      </c>
-      <c r="D24">
+      <c r="C24">
         <v>11.94</v>
+      </c>
+      <c r="D24" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -4084,11 +4084,11 @@
       <c r="B25" t="s">
         <v>112</v>
       </c>
-      <c r="C25" t="s">
-        <v>120</v>
-      </c>
-      <c r="D25">
+      <c r="C25">
         <v>14.47</v>
+      </c>
+      <c r="D25" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -4098,11 +4098,11 @@
       <c r="B26" t="s">
         <v>113</v>
       </c>
-      <c r="C26" t="s">
-        <v>120</v>
-      </c>
-      <c r="D26">
+      <c r="C26">
         <v>20.36</v>
+      </c>
+      <c r="D26" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -4112,11 +4112,11 @@
       <c r="B27" t="s">
         <v>114</v>
       </c>
-      <c r="C27" t="s">
-        <v>120</v>
-      </c>
-      <c r="D27">
+      <c r="C27">
         <v>14.69</v>
+      </c>
+      <c r="D27" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -4126,11 +4126,11 @@
       <c r="B28" t="s">
         <v>115</v>
       </c>
-      <c r="C28" t="s">
-        <v>120</v>
-      </c>
-      <c r="D28">
+      <c r="C28">
         <v>20.53</v>
+      </c>
+      <c r="D28" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -4140,11 +4140,11 @@
       <c r="B29" t="s">
         <v>116</v>
       </c>
-      <c r="C29" t="s">
-        <v>120</v>
-      </c>
-      <c r="D29">
+      <c r="C29">
         <v>9.460000000000001</v>
+      </c>
+      <c r="D29" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -4154,11 +4154,11 @@
       <c r="B30" t="s">
         <v>117</v>
       </c>
-      <c r="C30" t="s">
-        <v>120</v>
-      </c>
-      <c r="D30">
+      <c r="C30">
         <v>9.32</v>
+      </c>
+      <c r="D30" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -4168,11 +4168,11 @@
       <c r="B31" t="s">
         <v>118</v>
       </c>
-      <c r="C31" t="s">
-        <v>120</v>
-      </c>
-      <c r="D31">
+      <c r="C31">
         <v>9.449999999999999</v>
+      </c>
+      <c r="D31" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -4182,11 +4182,11 @@
       <c r="B32" t="s">
         <v>119</v>
       </c>
-      <c r="C32" t="s">
-        <v>120</v>
-      </c>
-      <c r="D32">
+      <c r="C32">
         <v>9.59</v>
+      </c>
+      <c r="D32" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -4218,10 +4218,10 @@
         <v>55</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -4231,11 +4231,11 @@
       <c r="B2" t="s">
         <v>89</v>
       </c>
-      <c r="C2" t="s">
-        <v>120</v>
-      </c>
-      <c r="D2">
+      <c r="C2">
         <v>11.2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -4245,11 +4245,11 @@
       <c r="B3" t="s">
         <v>90</v>
       </c>
-      <c r="C3" t="s">
-        <v>120</v>
-      </c>
-      <c r="D3">
+      <c r="C3">
         <v>16.44</v>
+      </c>
+      <c r="D3" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -4259,11 +4259,11 @@
       <c r="B4" t="s">
         <v>91</v>
       </c>
-      <c r="C4" t="s">
-        <v>120</v>
-      </c>
-      <c r="D4">
+      <c r="C4">
         <v>16.63</v>
+      </c>
+      <c r="D4" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -4273,11 +4273,11 @@
       <c r="B5" t="s">
         <v>92</v>
       </c>
-      <c r="C5" t="s">
-        <v>120</v>
-      </c>
-      <c r="D5">
+      <c r="C5">
         <v>5.57</v>
+      </c>
+      <c r="D5" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -4287,11 +4287,11 @@
       <c r="B6" t="s">
         <v>93</v>
       </c>
-      <c r="C6" t="s">
-        <v>120</v>
-      </c>
-      <c r="D6">
+      <c r="C6">
         <v>5.75</v>
+      </c>
+      <c r="D6" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -4301,11 +4301,11 @@
       <c r="B7" t="s">
         <v>94</v>
       </c>
-      <c r="C7" t="s">
-        <v>120</v>
-      </c>
-      <c r="D7">
+      <c r="C7">
         <v>5.7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -4315,11 +4315,11 @@
       <c r="B8" t="s">
         <v>95</v>
       </c>
-      <c r="C8" t="s">
-        <v>120</v>
-      </c>
-      <c r="D8">
+      <c r="C8">
         <v>5.56</v>
+      </c>
+      <c r="D8" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -4329,11 +4329,11 @@
       <c r="B9" t="s">
         <v>96</v>
       </c>
-      <c r="C9" t="s">
-        <v>120</v>
-      </c>
-      <c r="D9">
+      <c r="C9">
         <v>17.87</v>
+      </c>
+      <c r="D9" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -4343,11 +4343,11 @@
       <c r="B10" t="s">
         <v>97</v>
       </c>
-      <c r="C10" t="s">
-        <v>120</v>
-      </c>
-      <c r="D10">
+      <c r="C10">
         <v>23.73</v>
+      </c>
+      <c r="D10" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -4357,11 +4357,11 @@
       <c r="B11" t="s">
         <v>98</v>
       </c>
-      <c r="C11" t="s">
-        <v>120</v>
-      </c>
-      <c r="D11">
+      <c r="C11">
         <v>18.57</v>
+      </c>
+      <c r="D11" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -4371,11 +4371,11 @@
       <c r="B12" t="s">
         <v>99</v>
       </c>
-      <c r="C12" t="s">
-        <v>120</v>
-      </c>
-      <c r="D12">
+      <c r="C12">
         <v>23.96</v>
+      </c>
+      <c r="D12" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -4385,11 +4385,11 @@
       <c r="B13" t="s">
         <v>100</v>
       </c>
-      <c r="C13" t="s">
-        <v>120</v>
-      </c>
-      <c r="D13">
+      <c r="C13">
         <v>10.94</v>
+      </c>
+      <c r="D13" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -4399,11 +4399,11 @@
       <c r="B14" t="s">
         <v>101</v>
       </c>
-      <c r="C14" t="s">
-        <v>120</v>
-      </c>
-      <c r="D14">
+      <c r="C14">
         <v>11.37</v>
+      </c>
+      <c r="D14" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -4413,11 +4413,11 @@
       <c r="B15" t="s">
         <v>102</v>
       </c>
-      <c r="C15" t="s">
-        <v>120</v>
-      </c>
-      <c r="D15">
+      <c r="C15">
         <v>11.42</v>
+      </c>
+      <c r="D15" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -4427,11 +4427,11 @@
       <c r="B16" t="s">
         <v>103</v>
       </c>
-      <c r="C16" t="s">
-        <v>120</v>
-      </c>
-      <c r="D16">
+      <c r="C16">
         <v>10.95</v>
+      </c>
+      <c r="D16" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -4441,11 +4441,11 @@
       <c r="B17" t="s">
         <v>104</v>
       </c>
-      <c r="C17" t="s">
-        <v>120</v>
-      </c>
-      <c r="D17">
+      <c r="C17">
         <v>18.8</v>
+      </c>
+      <c r="D17" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -4455,11 +4455,11 @@
       <c r="B18" t="s">
         <v>105</v>
       </c>
-      <c r="C18" t="s">
-        <v>120</v>
-      </c>
-      <c r="D18">
+      <c r="C18">
         <v>25.48</v>
+      </c>
+      <c r="D18" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -4469,11 +4469,11 @@
       <c r="B19" t="s">
         <v>106</v>
       </c>
-      <c r="C19" t="s">
-        <v>120</v>
-      </c>
-      <c r="D19">
+      <c r="C19">
         <v>19.5</v>
+      </c>
+      <c r="D19" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -4483,11 +4483,11 @@
       <c r="B20" t="s">
         <v>107</v>
       </c>
-      <c r="C20" t="s">
-        <v>120</v>
-      </c>
-      <c r="D20">
+      <c r="C20">
         <v>25.71</v>
+      </c>
+      <c r="D20" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -4497,11 +4497,11 @@
       <c r="B21" t="s">
         <v>108</v>
       </c>
-      <c r="C21" t="s">
-        <v>120</v>
-      </c>
-      <c r="D21">
+      <c r="C21">
         <v>11.89</v>
+      </c>
+      <c r="D21" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -4511,11 +4511,11 @@
       <c r="B22" t="s">
         <v>109</v>
       </c>
-      <c r="C22" t="s">
-        <v>120</v>
-      </c>
-      <c r="D22">
+      <c r="C22">
         <v>12.48</v>
+      </c>
+      <c r="D22" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -4525,11 +4525,11 @@
       <c r="B23" t="s">
         <v>110</v>
       </c>
-      <c r="C23" t="s">
-        <v>120</v>
-      </c>
-      <c r="D23">
+      <c r="C23">
         <v>12.65</v>
+      </c>
+      <c r="D23" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -4539,11 +4539,11 @@
       <c r="B24" t="s">
         <v>111</v>
       </c>
-      <c r="C24" t="s">
-        <v>120</v>
-      </c>
-      <c r="D24">
+      <c r="C24">
         <v>11.93</v>
+      </c>
+      <c r="D24" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -4553,11 +4553,11 @@
       <c r="B25" t="s">
         <v>112</v>
       </c>
-      <c r="C25" t="s">
-        <v>120</v>
-      </c>
-      <c r="D25">
+      <c r="C25">
         <v>14.47</v>
+      </c>
+      <c r="D25" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -4567,11 +4567,11 @@
       <c r="B26" t="s">
         <v>113</v>
       </c>
-      <c r="C26" t="s">
-        <v>120</v>
-      </c>
-      <c r="D26">
+      <c r="C26">
         <v>20.36</v>
+      </c>
+      <c r="D26" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -4581,11 +4581,11 @@
       <c r="B27" t="s">
         <v>114</v>
       </c>
-      <c r="C27" t="s">
-        <v>120</v>
-      </c>
-      <c r="D27">
+      <c r="C27">
         <v>14.69</v>
+      </c>
+      <c r="D27" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -4595,11 +4595,11 @@
       <c r="B28" t="s">
         <v>115</v>
       </c>
-      <c r="C28" t="s">
-        <v>120</v>
-      </c>
-      <c r="D28">
+      <c r="C28">
         <v>20.57</v>
+      </c>
+      <c r="D28" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -4609,11 +4609,11 @@
       <c r="B29" t="s">
         <v>116</v>
       </c>
-      <c r="C29" t="s">
-        <v>120</v>
-      </c>
-      <c r="D29">
+      <c r="C29">
         <v>9.460000000000001</v>
+      </c>
+      <c r="D29" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -4623,11 +4623,11 @@
       <c r="B30" t="s">
         <v>117</v>
       </c>
-      <c r="C30" t="s">
-        <v>120</v>
-      </c>
-      <c r="D30">
+      <c r="C30">
         <v>9.32</v>
+      </c>
+      <c r="D30" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -4637,11 +4637,11 @@
       <c r="B31" t="s">
         <v>118</v>
       </c>
-      <c r="C31" t="s">
-        <v>120</v>
-      </c>
-      <c r="D31">
+      <c r="C31">
         <v>9.449999999999999</v>
+      </c>
+      <c r="D31" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -4651,11 +4651,11 @@
       <c r="B32" t="s">
         <v>119</v>
       </c>
-      <c r="C32" t="s">
-        <v>120</v>
-      </c>
-      <c r="D32">
+      <c r="C32">
         <v>9.59</v>
+      </c>
+      <c r="D32" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -4687,10 +4687,10 @@
         <v>55</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -4700,11 +4700,11 @@
       <c r="B2" t="s">
         <v>89</v>
       </c>
-      <c r="C2" t="s">
-        <v>120</v>
-      </c>
-      <c r="D2">
+      <c r="C2">
         <v>11.21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -4714,11 +4714,11 @@
       <c r="B3" t="s">
         <v>90</v>
       </c>
-      <c r="C3" t="s">
-        <v>120</v>
-      </c>
-      <c r="D3">
+      <c r="C3">
         <v>16.46</v>
+      </c>
+      <c r="D3" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -4728,11 +4728,11 @@
       <c r="B4" t="s">
         <v>91</v>
       </c>
-      <c r="C4" t="s">
-        <v>120</v>
-      </c>
-      <c r="D4">
+      <c r="C4">
         <v>16.65</v>
+      </c>
+      <c r="D4" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -4742,11 +4742,11 @@
       <c r="B5" t="s">
         <v>92</v>
       </c>
-      <c r="C5" t="s">
-        <v>120</v>
-      </c>
-      <c r="D5">
+      <c r="C5">
         <v>5.57</v>
+      </c>
+      <c r="D5" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -4756,11 +4756,11 @@
       <c r="B6" t="s">
         <v>93</v>
       </c>
-      <c r="C6" t="s">
-        <v>120</v>
-      </c>
-      <c r="D6">
+      <c r="C6">
         <v>5.74</v>
+      </c>
+      <c r="D6" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -4770,11 +4770,11 @@
       <c r="B7" t="s">
         <v>94</v>
       </c>
-      <c r="C7" t="s">
-        <v>120</v>
-      </c>
-      <c r="D7">
+      <c r="C7">
         <v>5.7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -4784,11 +4784,11 @@
       <c r="B8" t="s">
         <v>95</v>
       </c>
-      <c r="C8" t="s">
-        <v>120</v>
-      </c>
-      <c r="D8">
+      <c r="C8">
         <v>5.56</v>
+      </c>
+      <c r="D8" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -4798,11 +4798,11 @@
       <c r="B9" t="s">
         <v>96</v>
       </c>
-      <c r="C9" t="s">
-        <v>120</v>
-      </c>
-      <c r="D9">
+      <c r="C9">
         <v>17.85</v>
+      </c>
+      <c r="D9" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -4812,11 +4812,11 @@
       <c r="B10" t="s">
         <v>97</v>
       </c>
-      <c r="C10" t="s">
-        <v>120</v>
-      </c>
-      <c r="D10">
+      <c r="C10">
         <v>23.73</v>
+      </c>
+      <c r="D10" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -4826,11 +4826,11 @@
       <c r="B11" t="s">
         <v>98</v>
       </c>
-      <c r="C11" t="s">
-        <v>120</v>
-      </c>
-      <c r="D11">
+      <c r="C11">
         <v>18.56</v>
+      </c>
+      <c r="D11" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -4840,11 +4840,11 @@
       <c r="B12" t="s">
         <v>99</v>
       </c>
-      <c r="C12" t="s">
-        <v>120</v>
-      </c>
-      <c r="D12">
+      <c r="C12">
         <v>23.96</v>
+      </c>
+      <c r="D12" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -4854,11 +4854,11 @@
       <c r="B13" t="s">
         <v>100</v>
       </c>
-      <c r="C13" t="s">
-        <v>120</v>
-      </c>
-      <c r="D13">
+      <c r="C13">
         <v>10.91</v>
+      </c>
+      <c r="D13" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -4868,11 +4868,11 @@
       <c r="B14" t="s">
         <v>101</v>
       </c>
-      <c r="C14" t="s">
-        <v>120</v>
-      </c>
-      <c r="D14">
+      <c r="C14">
         <v>11.37</v>
+      </c>
+      <c r="D14" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -4882,11 +4882,11 @@
       <c r="B15" t="s">
         <v>102</v>
       </c>
-      <c r="C15" t="s">
-        <v>120</v>
-      </c>
-      <c r="D15">
+      <c r="C15">
         <v>11.4</v>
+      </c>
+      <c r="D15" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -4896,11 +4896,11 @@
       <c r="B16" t="s">
         <v>103</v>
       </c>
-      <c r="C16" t="s">
-        <v>120</v>
-      </c>
-      <c r="D16">
+      <c r="C16">
         <v>10.95</v>
+      </c>
+      <c r="D16" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -4910,11 +4910,11 @@
       <c r="B17" t="s">
         <v>104</v>
       </c>
-      <c r="C17" t="s">
-        <v>120</v>
-      </c>
-      <c r="D17">
+      <c r="C17">
         <v>18.8</v>
+      </c>
+      <c r="D17" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -4924,11 +4924,11 @@
       <c r="B18" t="s">
         <v>105</v>
       </c>
-      <c r="C18" t="s">
-        <v>120</v>
-      </c>
-      <c r="D18">
+      <c r="C18">
         <v>25.5</v>
+      </c>
+      <c r="D18" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -4938,11 +4938,11 @@
       <c r="B19" t="s">
         <v>106</v>
       </c>
-      <c r="C19" t="s">
-        <v>120</v>
-      </c>
-      <c r="D19">
+      <c r="C19">
         <v>19.46</v>
+      </c>
+      <c r="D19" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -4952,11 +4952,11 @@
       <c r="B20" t="s">
         <v>107</v>
       </c>
-      <c r="C20" t="s">
-        <v>120</v>
-      </c>
-      <c r="D20">
+      <c r="C20">
         <v>25.73</v>
+      </c>
+      <c r="D20" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -4966,11 +4966,11 @@
       <c r="B21" t="s">
         <v>108</v>
       </c>
-      <c r="C21" t="s">
-        <v>120</v>
-      </c>
-      <c r="D21">
+      <c r="C21">
         <v>11.89</v>
+      </c>
+      <c r="D21" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -4980,11 +4980,11 @@
       <c r="B22" t="s">
         <v>109</v>
       </c>
-      <c r="C22" t="s">
-        <v>120</v>
-      </c>
-      <c r="D22">
+      <c r="C22">
         <v>12.45</v>
+      </c>
+      <c r="D22" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -4994,11 +4994,11 @@
       <c r="B23" t="s">
         <v>110</v>
       </c>
-      <c r="C23" t="s">
-        <v>120</v>
-      </c>
-      <c r="D23">
+      <c r="C23">
         <v>12.66</v>
+      </c>
+      <c r="D23" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -5008,11 +5008,11 @@
       <c r="B24" t="s">
         <v>111</v>
       </c>
-      <c r="C24" t="s">
-        <v>120</v>
-      </c>
-      <c r="D24">
+      <c r="C24">
         <v>11.92</v>
+      </c>
+      <c r="D24" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -5022,11 +5022,11 @@
       <c r="B25" t="s">
         <v>112</v>
       </c>
-      <c r="C25" t="s">
-        <v>120</v>
-      </c>
-      <c r="D25">
+      <c r="C25">
         <v>14.46</v>
+      </c>
+      <c r="D25" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -5036,11 +5036,11 @@
       <c r="B26" t="s">
         <v>113</v>
       </c>
-      <c r="C26" t="s">
-        <v>120</v>
-      </c>
-      <c r="D26">
+      <c r="C26">
         <v>20.4</v>
+      </c>
+      <c r="D26" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -5050,11 +5050,11 @@
       <c r="B27" t="s">
         <v>114</v>
       </c>
-      <c r="C27" t="s">
-        <v>120</v>
-      </c>
-      <c r="D27">
+      <c r="C27">
         <v>14.71</v>
+      </c>
+      <c r="D27" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -5064,11 +5064,11 @@
       <c r="B28" t="s">
         <v>115</v>
       </c>
-      <c r="C28" t="s">
-        <v>120</v>
-      </c>
-      <c r="D28">
+      <c r="C28">
         <v>20.59</v>
+      </c>
+      <c r="D28" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -5078,11 +5078,11 @@
       <c r="B29" t="s">
         <v>116</v>
       </c>
-      <c r="C29" t="s">
-        <v>120</v>
-      </c>
-      <c r="D29">
+      <c r="C29">
         <v>9.460000000000001</v>
+      </c>
+      <c r="D29" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -5092,11 +5092,11 @@
       <c r="B30" t="s">
         <v>117</v>
       </c>
-      <c r="C30" t="s">
-        <v>120</v>
-      </c>
-      <c r="D30">
+      <c r="C30">
         <v>9.32</v>
+      </c>
+      <c r="D30" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -5106,11 +5106,11 @@
       <c r="B31" t="s">
         <v>118</v>
       </c>
-      <c r="C31" t="s">
-        <v>120</v>
-      </c>
-      <c r="D31">
+      <c r="C31">
         <v>9.44</v>
+      </c>
+      <c r="D31" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -5120,11 +5120,11 @@
       <c r="B32" t="s">
         <v>119</v>
       </c>
-      <c r="C32" t="s">
-        <v>120</v>
-      </c>
-      <c r="D32">
+      <c r="C32">
         <v>9.59</v>
+      </c>
+      <c r="D32" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -5156,10 +5156,10 @@
         <v>55</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -5169,11 +5169,11 @@
       <c r="B2" t="s">
         <v>89</v>
       </c>
-      <c r="C2" t="s">
-        <v>120</v>
-      </c>
-      <c r="D2">
+      <c r="C2">
         <v>11.2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -5183,11 +5183,11 @@
       <c r="B3" t="s">
         <v>90</v>
       </c>
-      <c r="C3" t="s">
-        <v>120</v>
-      </c>
-      <c r="D3">
+      <c r="C3">
         <v>16.5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -5197,11 +5197,11 @@
       <c r="B4" t="s">
         <v>91</v>
       </c>
-      <c r="C4" t="s">
-        <v>120</v>
-      </c>
-      <c r="D4">
+      <c r="C4">
         <v>16.67</v>
+      </c>
+      <c r="D4" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -5211,11 +5211,11 @@
       <c r="B5" t="s">
         <v>92</v>
       </c>
-      <c r="C5" t="s">
-        <v>120</v>
-      </c>
-      <c r="D5">
+      <c r="C5">
         <v>5.57</v>
+      </c>
+      <c r="D5" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -5225,11 +5225,11 @@
       <c r="B6" t="s">
         <v>93</v>
       </c>
-      <c r="C6" t="s">
-        <v>120</v>
-      </c>
-      <c r="D6">
+      <c r="C6">
         <v>5.74</v>
+      </c>
+      <c r="D6" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -5239,11 +5239,11 @@
       <c r="B7" t="s">
         <v>94</v>
       </c>
-      <c r="C7" t="s">
-        <v>120</v>
-      </c>
-      <c r="D7">
+      <c r="C7">
         <v>5.7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -5253,11 +5253,11 @@
       <c r="B8" t="s">
         <v>95</v>
       </c>
-      <c r="C8" t="s">
-        <v>120</v>
-      </c>
-      <c r="D8">
+      <c r="C8">
         <v>5.55</v>
+      </c>
+      <c r="D8" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -5267,11 +5267,11 @@
       <c r="B9" t="s">
         <v>96</v>
       </c>
-      <c r="C9" t="s">
-        <v>120</v>
-      </c>
-      <c r="D9">
+      <c r="C9">
         <v>17.85</v>
+      </c>
+      <c r="D9" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -5281,11 +5281,11 @@
       <c r="B10" t="s">
         <v>97</v>
       </c>
-      <c r="C10" t="s">
-        <v>120</v>
-      </c>
-      <c r="D10">
+      <c r="C10">
         <v>23.75</v>
+      </c>
+      <c r="D10" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -5295,11 +5295,11 @@
       <c r="B11" t="s">
         <v>98</v>
       </c>
-      <c r="C11" t="s">
-        <v>120</v>
-      </c>
-      <c r="D11">
+      <c r="C11">
         <v>18.57</v>
+      </c>
+      <c r="D11" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -5309,11 +5309,11 @@
       <c r="B12" t="s">
         <v>99</v>
       </c>
-      <c r="C12" t="s">
-        <v>120</v>
-      </c>
-      <c r="D12">
+      <c r="C12">
         <v>24</v>
+      </c>
+      <c r="D12" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -5323,11 +5323,11 @@
       <c r="B13" t="s">
         <v>100</v>
       </c>
-      <c r="C13" t="s">
-        <v>120</v>
-      </c>
-      <c r="D13">
+      <c r="C13">
         <v>10.9</v>
+      </c>
+      <c r="D13" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -5337,11 +5337,11 @@
       <c r="B14" t="s">
         <v>101</v>
       </c>
-      <c r="C14" t="s">
-        <v>120</v>
-      </c>
-      <c r="D14">
+      <c r="C14">
         <v>11.37</v>
+      </c>
+      <c r="D14" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -5351,11 +5351,11 @@
       <c r="B15" t="s">
         <v>102</v>
       </c>
-      <c r="C15" t="s">
-        <v>120</v>
-      </c>
-      <c r="D15">
+      <c r="C15">
         <v>11.4</v>
+      </c>
+      <c r="D15" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -5365,11 +5365,11 @@
       <c r="B16" t="s">
         <v>103</v>
       </c>
-      <c r="C16" t="s">
-        <v>120</v>
-      </c>
-      <c r="D16">
+      <c r="C16">
         <v>10.94</v>
+      </c>
+      <c r="D16" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -5379,11 +5379,11 @@
       <c r="B17" t="s">
         <v>104</v>
       </c>
-      <c r="C17" t="s">
-        <v>120</v>
-      </c>
-      <c r="D17">
+      <c r="C17">
         <v>18.81</v>
+      </c>
+      <c r="D17" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -5393,11 +5393,11 @@
       <c r="B18" t="s">
         <v>105</v>
       </c>
-      <c r="C18" t="s">
-        <v>120</v>
-      </c>
-      <c r="D18">
+      <c r="C18">
         <v>25.5</v>
+      </c>
+      <c r="D18" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -5407,11 +5407,11 @@
       <c r="B19" t="s">
         <v>106</v>
       </c>
-      <c r="C19" t="s">
-        <v>120</v>
-      </c>
-      <c r="D19">
+      <c r="C19">
         <v>19.49</v>
+      </c>
+      <c r="D19" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -5421,11 +5421,11 @@
       <c r="B20" t="s">
         <v>107</v>
       </c>
-      <c r="C20" t="s">
-        <v>120</v>
-      </c>
-      <c r="D20">
+      <c r="C20">
         <v>25.73</v>
+      </c>
+      <c r="D20" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -5435,11 +5435,11 @@
       <c r="B21" t="s">
         <v>108</v>
       </c>
-      <c r="C21" t="s">
-        <v>120</v>
-      </c>
-      <c r="D21">
+      <c r="C21">
         <v>11.89</v>
+      </c>
+      <c r="D21" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -5449,11 +5449,11 @@
       <c r="B22" t="s">
         <v>109</v>
       </c>
-      <c r="C22" t="s">
-        <v>120</v>
-      </c>
-      <c r="D22">
+      <c r="C22">
         <v>12.45</v>
+      </c>
+      <c r="D22" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -5463,11 +5463,11 @@
       <c r="B23" t="s">
         <v>110</v>
       </c>
-      <c r="C23" t="s">
-        <v>120</v>
-      </c>
-      <c r="D23">
+      <c r="C23">
         <v>12.68</v>
+      </c>
+      <c r="D23" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -5477,11 +5477,11 @@
       <c r="B24" t="s">
         <v>111</v>
       </c>
-      <c r="C24" t="s">
-        <v>120</v>
-      </c>
-      <c r="D24">
+      <c r="C24">
         <v>11.92</v>
+      </c>
+      <c r="D24" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -5491,11 +5491,11 @@
       <c r="B25" t="s">
         <v>112</v>
       </c>
-      <c r="C25" t="s">
-        <v>120</v>
-      </c>
-      <c r="D25">
+      <c r="C25">
         <v>14.47</v>
+      </c>
+      <c r="D25" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -5505,11 +5505,11 @@
       <c r="B26" t="s">
         <v>113</v>
       </c>
-      <c r="C26" t="s">
-        <v>120</v>
-      </c>
-      <c r="D26">
+      <c r="C26">
         <v>20.42</v>
+      </c>
+      <c r="D26" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -5519,11 +5519,11 @@
       <c r="B27" t="s">
         <v>114</v>
       </c>
-      <c r="C27" t="s">
-        <v>120</v>
-      </c>
-      <c r="D27">
+      <c r="C27">
         <v>14.7</v>
+      </c>
+      <c r="D27" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -5533,11 +5533,11 @@
       <c r="B28" t="s">
         <v>115</v>
       </c>
-      <c r="C28" t="s">
-        <v>120</v>
-      </c>
-      <c r="D28">
+      <c r="C28">
         <v>20.63</v>
+      </c>
+      <c r="D28" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -5547,11 +5547,11 @@
       <c r="B29" t="s">
         <v>116</v>
       </c>
-      <c r="C29" t="s">
-        <v>120</v>
-      </c>
-      <c r="D29">
+      <c r="C29">
         <v>9.460000000000001</v>
+      </c>
+      <c r="D29" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -5561,11 +5561,11 @@
       <c r="B30" t="s">
         <v>117</v>
       </c>
-      <c r="C30" t="s">
-        <v>120</v>
-      </c>
-      <c r="D30">
+      <c r="C30">
         <v>9.33</v>
+      </c>
+      <c r="D30" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -5575,11 +5575,11 @@
       <c r="B31" t="s">
         <v>118</v>
       </c>
-      <c r="C31" t="s">
-        <v>120</v>
-      </c>
-      <c r="D31">
+      <c r="C31">
         <v>9.44</v>
+      </c>
+      <c r="D31" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -5589,11 +5589,11 @@
       <c r="B32" t="s">
         <v>119</v>
       </c>
-      <c r="C32" t="s">
-        <v>120</v>
-      </c>
-      <c r="D32">
+      <c r="C32">
         <v>9.59</v>
+      </c>
+      <c r="D32" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed issue where arr_max_adaptive_temp_vulnerable was the incorrect shape. Ran tests to validate
</commit_message>
<xml_diff>
--- a/tests/testmodels/TestJob1/mf_results/tm59mechvent/TM59MechVent__TestJob1.xlsx
+++ b/tests/testmodels/TestJob1/mf_results/tm59mechvent/TM59MechVent__TestJob1.xlsx
@@ -30,15 +30,15 @@
     <t>sheet_name</t>
   </si>
   <si>
+    <t>Date</t>
+  </si>
+  <si>
     <t>JobNo</t>
   </si>
   <si>
     <t>Author</t>
   </si>
   <si>
-    <t>Date</t>
-  </si>
-  <si>
     <t>0</t>
   </si>
   <si>
@@ -105,15 +105,15 @@
     <t>Results, Air Speed 0.8</t>
   </si>
   <si>
+    <t>20220325</t>
+  </si>
+  <si>
     <t>/c/e</t>
   </si>
   <si>
     <t>jovyan</t>
   </si>
   <si>
-    <t>20220325</t>
-  </si>
-  <si>
     <t>index</t>
   </si>
   <si>
@@ -183,7 +183,7 @@
     <t>51.38</t>
   </si>
   <si>
-    <t>2022-03-25 13:28:14.556661</t>
+    <t>2022-03-25 19:32:57.480416</t>
   </si>
   <si>
     <t>2021.4.0.0</t>
@@ -578,9 +578,9 @@
   <tableColumns count="5">
     <tableColumn id="1" name="index"/>
     <tableColumn id="2" name="sheet_name"/>
-    <tableColumn id="3" name="JobNo"/>
-    <tableColumn id="4" name="Author"/>
-    <tableColumn id="5" name="Date"/>
+    <tableColumn id="3" name="Date"/>
+    <tableColumn id="4" name="JobNo"/>
+    <tableColumn id="5" name="Author"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>

</xml_diff>